<commit_message>
Further work on BFG site
</commit_message>
<xml_diff>
--- a/Prototypes/Pinus/Observed.xlsx
+++ b/Prototypes/Pinus/Observed.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\APSIMxSourceTree\Prototypes\Pinus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5CE880C-84D1-4818-83AC-06F4173CAB3D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCD0AC49-4C79-4FE8-A03F-E9F1712571CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" tabRatio="653" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -924,10 +924,10 @@
   <dimension ref="A1:BQ982"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="AH2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D121" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AL1" sqref="AL1"/>
+      <selection pane="bottomRight" activeCell="B151" sqref="B151:C155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="12.75"/>
@@ -5597,7 +5597,12 @@
       <c r="E121" s="20">
         <v>625</v>
       </c>
-      <c r="I121" s="6"/>
+      <c r="I121" s="6">
+        <v>30482.42</v>
+      </c>
+      <c r="J121" s="3">
+        <v>10</v>
+      </c>
       <c r="L121" s="6"/>
       <c r="R121" s="38"/>
       <c r="S121" s="6"/>
@@ -5635,7 +5640,7 @@
         <v>4</v>
       </c>
       <c r="B122" s="5">
-        <v>32600.8236</v>
+        <v>32382.68144</v>
       </c>
       <c r="C122" s="8">
         <v>15.2</v>
@@ -5647,7 +5652,12 @@
       <c r="E122" s="20">
         <v>625</v>
       </c>
-      <c r="I122" s="6"/>
+      <c r="I122" s="6">
+        <v>32382.68144</v>
+      </c>
+      <c r="J122" s="3">
+        <v>15.2</v>
+      </c>
       <c r="L122" s="6"/>
       <c r="R122" s="38"/>
       <c r="S122" s="6"/>
@@ -5685,7 +5695,7 @@
         <v>4</v>
       </c>
       <c r="B123" s="5">
-        <v>37056.775999999998</v>
+        <v>32601.82676</v>
       </c>
       <c r="C123" s="8">
         <v>15.8</v>
@@ -5697,7 +5707,12 @@
       <c r="E123" s="20">
         <v>275</v>
       </c>
-      <c r="I123" s="6"/>
+      <c r="I123" s="6">
+        <v>32601.82676</v>
+      </c>
+      <c r="J123" s="3">
+        <v>15.8</v>
+      </c>
       <c r="L123" s="6"/>
       <c r="R123" s="38"/>
       <c r="S123" s="6"/>
@@ -5735,7 +5750,7 @@
         <v>4</v>
       </c>
       <c r="B124" s="5">
-        <v>32381.678400000001</v>
+        <v>34135.843999999997</v>
       </c>
       <c r="C124" s="8">
         <v>20</v>
@@ -5747,7 +5762,12 @@
       <c r="E124" s="20">
         <v>275</v>
       </c>
-      <c r="I124" s="6"/>
+      <c r="I124" s="6">
+        <v>34135.843999999997</v>
+      </c>
+      <c r="J124" s="3">
+        <v>20</v>
+      </c>
       <c r="L124" s="6"/>
       <c r="R124" s="38"/>
       <c r="S124" s="6"/>
@@ -5785,7 +5805,7 @@
         <v>4</v>
       </c>
       <c r="B125" s="5">
-        <v>34134.839999999997</v>
+        <v>37057.781600000002</v>
       </c>
       <c r="C125" s="8">
         <v>28</v>
@@ -5797,7 +5817,12 @@
       <c r="E125" s="20">
         <v>275</v>
       </c>
-      <c r="I125" s="6"/>
+      <c r="I125" s="6">
+        <v>37057.781600000002</v>
+      </c>
+      <c r="J125" s="3">
+        <v>28</v>
+      </c>
       <c r="L125" s="6"/>
       <c r="R125" s="38"/>
       <c r="S125" s="6"/>
@@ -5835,7 +5860,7 @@
         <v>5</v>
       </c>
       <c r="B126" s="5">
-        <v>32381.678400000001</v>
+        <v>30482.42</v>
       </c>
       <c r="C126" s="8">
         <v>10</v>
@@ -5885,7 +5910,7 @@
         <v>5</v>
       </c>
       <c r="B127" s="5">
-        <v>34134.839999999997</v>
+        <v>32382.68144</v>
       </c>
       <c r="C127" s="8">
         <v>15.2</v>
@@ -5935,7 +5960,7 @@
         <v>5</v>
       </c>
       <c r="B128" s="5">
-        <v>30482.42</v>
+        <v>32601.82676</v>
       </c>
       <c r="C128" s="8">
         <v>15.8</v>
@@ -5985,7 +6010,7 @@
         <v>5</v>
       </c>
       <c r="B129" s="5">
-        <v>32600.8236</v>
+        <v>34135.843999999997</v>
       </c>
       <c r="C129" s="8">
         <v>20</v>
@@ -6035,7 +6060,7 @@
         <v>5</v>
       </c>
       <c r="B130" s="5">
-        <v>37056.775999999998</v>
+        <v>37057.781600000002</v>
       </c>
       <c r="C130" s="8">
         <v>28</v>
@@ -6085,7 +6110,7 @@
         <v>6</v>
       </c>
       <c r="B131" s="5">
-        <v>32600.8236</v>
+        <v>30482.42</v>
       </c>
       <c r="C131" s="8">
         <v>10</v>
@@ -6135,7 +6160,7 @@
         <v>6</v>
       </c>
       <c r="B132" s="5">
-        <v>37056.775999999998</v>
+        <v>32382.68144</v>
       </c>
       <c r="C132" s="8">
         <v>15.2</v>
@@ -6185,7 +6210,7 @@
         <v>6</v>
       </c>
       <c r="B133" s="5">
-        <v>32381.678400000001</v>
+        <v>32601.82676</v>
       </c>
       <c r="C133" s="8">
         <v>15.8</v>
@@ -6235,7 +6260,7 @@
         <v>6</v>
       </c>
       <c r="B134" s="5">
-        <v>34134.839999999997</v>
+        <v>34135.843999999997</v>
       </c>
       <c r="C134" s="8">
         <v>20</v>
@@ -6285,7 +6310,7 @@
         <v>6</v>
       </c>
       <c r="B135" s="5">
-        <v>30482.42</v>
+        <v>37057.781600000002</v>
       </c>
       <c r="C135" s="8">
         <v>28</v>
@@ -6335,7 +6360,7 @@
         <v>9</v>
       </c>
       <c r="B136" s="5">
-        <v>34134.839999999997</v>
+        <v>30482.42</v>
       </c>
       <c r="C136" s="8">
         <v>10</v>
@@ -6385,7 +6410,7 @@
         <v>9</v>
       </c>
       <c r="B137" s="5">
-        <v>30482.42</v>
+        <v>32382.68144</v>
       </c>
       <c r="C137" s="8">
         <v>15.2</v>
@@ -6435,7 +6460,7 @@
         <v>9</v>
       </c>
       <c r="B138" s="5">
-        <v>32600.8236</v>
+        <v>32601.82676</v>
       </c>
       <c r="C138" s="8">
         <v>15.8</v>
@@ -6485,7 +6510,7 @@
         <v>9</v>
       </c>
       <c r="B139" s="5">
-        <v>37056.775999999998</v>
+        <v>34135.843999999997</v>
       </c>
       <c r="C139" s="8">
         <v>20</v>
@@ -6535,7 +6560,7 @@
         <v>9</v>
       </c>
       <c r="B140" s="5">
-        <v>32381.678400000001</v>
+        <v>37057.781600000002</v>
       </c>
       <c r="C140" s="8">
         <v>28</v>
@@ -6585,7 +6610,7 @@
         <v>11</v>
       </c>
       <c r="B141" s="5">
-        <v>37056.775999999998</v>
+        <v>30482.42</v>
       </c>
       <c r="C141" s="24">
         <v>10</v>
@@ -6635,7 +6660,7 @@
         <v>11</v>
       </c>
       <c r="B142" s="5">
-        <v>32381.678400000001</v>
+        <v>32382.68144</v>
       </c>
       <c r="C142" s="24">
         <v>15.2</v>
@@ -6685,7 +6710,7 @@
         <v>11</v>
       </c>
       <c r="B143" s="5">
-        <v>34134.839999999997</v>
+        <v>32601.82676</v>
       </c>
       <c r="C143" s="25">
         <v>15.8</v>
@@ -6736,7 +6761,7 @@
         <v>11</v>
       </c>
       <c r="B144" s="5">
-        <v>30482.42</v>
+        <v>34135.843999999997</v>
       </c>
       <c r="C144" s="25">
         <v>20</v>
@@ -6787,7 +6812,7 @@
         <v>11</v>
       </c>
       <c r="B145" s="5">
-        <v>32600.8236</v>
+        <v>37057.781600000002</v>
       </c>
       <c r="C145" s="25">
         <v>28</v>
@@ -6889,7 +6914,7 @@
         <v>10</v>
       </c>
       <c r="B147" s="5">
-        <v>32600.8236</v>
+        <v>32382.68144</v>
       </c>
       <c r="C147" s="25">
         <v>15.2</v>
@@ -6940,7 +6965,7 @@
         <v>10</v>
       </c>
       <c r="B148" s="5">
-        <v>37056.775999999998</v>
+        <v>32601.82676</v>
       </c>
       <c r="C148" s="25">
         <v>15.8</v>
@@ -6991,7 +7016,7 @@
         <v>10</v>
       </c>
       <c r="B149" s="18">
-        <v>32381.678400000001</v>
+        <v>34135.843999999997</v>
       </c>
       <c r="C149" s="25">
         <v>20</v>
@@ -7042,7 +7067,7 @@
         <v>10</v>
       </c>
       <c r="B150" s="18">
-        <v>34134.839999999997</v>
+        <v>37057.781600000002</v>
       </c>
       <c r="C150" s="25">
         <v>28</v>
@@ -7093,7 +7118,7 @@
         <v>12</v>
       </c>
       <c r="B151" s="18">
-        <v>32381.678400000001</v>
+        <v>30482.42</v>
       </c>
       <c r="C151" s="25">
         <v>10</v>
@@ -7144,7 +7169,7 @@
         <v>12</v>
       </c>
       <c r="B152" s="18">
-        <v>34134.839999999997</v>
+        <v>32382.68144</v>
       </c>
       <c r="C152" s="25">
         <v>15.2</v>
@@ -7195,7 +7220,7 @@
         <v>12</v>
       </c>
       <c r="B153" s="18">
-        <v>30482.42</v>
+        <v>32601.82676</v>
       </c>
       <c r="C153" s="25">
         <v>15.8</v>
@@ -7246,7 +7271,7 @@
         <v>12</v>
       </c>
       <c r="B154" s="18">
-        <v>32600.8236</v>
+        <v>34135.843999999997</v>
       </c>
       <c r="C154" s="25">
         <v>20</v>
@@ -7297,7 +7322,7 @@
         <v>12</v>
       </c>
       <c r="B155" s="18">
-        <v>37056.775999999998</v>
+        <v>37057.781600000002</v>
       </c>
       <c r="C155" s="25">
         <v>28</v>

</xml_diff>

<commit_message>
Worked on BFG site and Pinus model
</commit_message>
<xml_diff>
--- a/Prototypes/Pinus/Observed.xlsx
+++ b/Prototypes/Pinus/Observed.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\APSIMxSourceTree\Prototypes\Pinus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3728368-8A73-4FF6-84CD-44D97AB2CFE4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67908916-C8B9-4A41-B15F-B621AC2B2309}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" tabRatio="653" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -136,9 +136,6 @@
   </si>
   <si>
     <t>Age(y)</t>
-  </si>
-  <si>
-    <t>NContentTotal (kg/ha)</t>
   </si>
   <si>
     <t>LiveFoliarN (kg/ha)</t>
@@ -343,6 +340,9 @@
   </si>
   <si>
     <t>Pinus.AboveGround.Wt</t>
+  </si>
+  <si>
+    <t>Pinus.Aboveground.N</t>
   </si>
 </sst>
 </file>
@@ -921,10 +921,10 @@
   <dimension ref="A1:BP982"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="E120" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D817" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F1" sqref="F1"/>
+      <selection pane="bottomRight" activeCell="U829" sqref="U829:U853"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="12.75"/>
@@ -968,46 +968,46 @@
         <v>25</v>
       </c>
       <c r="E1" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="F1" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="G1" s="30" t="s">
         <v>76</v>
       </c>
-      <c r="F1" s="30" t="s">
-        <v>95</v>
-      </c>
-      <c r="G1" s="30" t="s">
+      <c r="H1" s="30" t="s">
+        <v>93</v>
+      </c>
+      <c r="I1" s="30" t="s">
         <v>77</v>
       </c>
-      <c r="H1" s="30" t="s">
-        <v>94</v>
-      </c>
-      <c r="I1" s="30" t="s">
+      <c r="J1" s="30" t="s">
+        <v>92</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="L1" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="M1" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="N1" s="30" t="s">
+        <v>91</v>
+      </c>
+      <c r="O1" s="30" t="s">
         <v>78</v>
       </c>
-      <c r="J1" s="30" t="s">
-        <v>93</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="L1" s="30" t="s">
-        <v>90</v>
-      </c>
-      <c r="M1" s="30" t="s">
-        <v>91</v>
-      </c>
-      <c r="N1" s="30" t="s">
-        <v>92</v>
-      </c>
-      <c r="O1" s="30" t="s">
+      <c r="P1" s="30" t="s">
         <v>79</v>
       </c>
-      <c r="P1" s="30" t="s">
+      <c r="Q1" s="30" t="s">
         <v>80</v>
       </c>
-      <c r="Q1" s="30" t="s">
+      <c r="R1" s="30" t="s">
         <v>81</v>
-      </c>
-      <c r="R1" s="30" t="s">
-        <v>82</v>
       </c>
       <c r="S1" s="30" t="s">
         <v>3</v>
@@ -1016,16 +1016,16 @@
         <v>7</v>
       </c>
       <c r="U1" s="30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="V1" s="30" t="s">
-        <v>27</v>
+        <v>95</v>
       </c>
       <c r="W1" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="X1" s="30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="Y1" s="30" t="s">
         <v>2</v>
@@ -1034,96 +1034,96 @@
         <v>8</v>
       </c>
       <c r="AA1" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="AB1" s="30" t="s">
         <v>83</v>
       </c>
-      <c r="AB1" s="30" t="s">
+      <c r="AC1" s="30" t="s">
         <v>84</v>
       </c>
-      <c r="AC1" s="30" t="s">
+      <c r="AD1" s="30" t="s">
         <v>85</v>
       </c>
-      <c r="AD1" s="30" t="s">
+      <c r="AE1" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="30" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AI1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="AJ1" s="30" t="s">
         <v>88</v>
       </c>
-      <c r="AG1" s="30" t="s">
-        <v>55</v>
-      </c>
-      <c r="AH1" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="AI1" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AJ1" s="30" t="s">
-        <v>89</v>
-      </c>
       <c r="AK1" s="30" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AL1" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="AM1" s="30" t="s">
         <v>28</v>
-      </c>
-      <c r="AM1" s="30" t="s">
-        <v>29</v>
       </c>
       <c r="AN1" s="30" t="s">
         <v>13</v>
       </c>
       <c r="AO1" s="30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="AP1" s="29"/>
       <c r="AQ1" s="29"/>
       <c r="BB1" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="BC1" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="BC1" s="3" t="s">
+      <c r="BD1" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="BD1" s="3" t="s">
+      <c r="BE1" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="BE1" s="3" t="s">
+      <c r="BF1" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="BF1" s="3" t="s">
+      <c r="BG1" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="BG1" s="3" t="s">
+      <c r="BH1" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="BH1" s="3" t="s">
+      <c r="BI1" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="BI1" s="3" t="s">
+      <c r="BJ1" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="BJ1" s="3" t="s">
+      <c r="BK1" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="BK1" s="3" t="s">
+      <c r="BL1" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="BL1" s="3" t="s">
+      <c r="BM1" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="BM1" s="3" t="s">
+      <c r="BN1" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="BN1" s="3" t="s">
+      <c r="BO1" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="BO1" s="3" t="s">
+      <c r="BP1" s="3" t="s">
         <v>71</v>
-      </c>
-      <c r="BP1" s="3" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:68">
@@ -7302,7 +7302,7 @@
       <c r="AI156" s="1"/>
       <c r="AJ156" s="1"/>
       <c r="AN156" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="157" spans="1:40" ht="15">
@@ -7362,7 +7362,7 @@
       <c r="AI157" s="1"/>
       <c r="AJ157" s="1"/>
       <c r="AN157" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="158" spans="1:40" ht="15">
@@ -7422,7 +7422,7 @@
       <c r="AI158" s="1"/>
       <c r="AJ158" s="1"/>
       <c r="AN158" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="159" spans="1:40" ht="15">
@@ -7482,7 +7482,7 @@
       <c r="AI159" s="1"/>
       <c r="AJ159" s="1"/>
       <c r="AN159" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="160" spans="1:40" ht="15">
@@ -7542,7 +7542,7 @@
       <c r="AI160" s="1"/>
       <c r="AJ160" s="1"/>
       <c r="AN160" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="161" spans="1:40" ht="15">
@@ -7595,7 +7595,7 @@
       <c r="AI161" s="1"/>
       <c r="AJ161" s="1"/>
       <c r="AN161" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="162" spans="1:40" ht="15">
@@ -7650,7 +7650,7 @@
       <c r="AI162" s="1"/>
       <c r="AJ162" s="1"/>
       <c r="AN162" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="163" spans="1:40" ht="15">
@@ -7712,7 +7712,7 @@
       <c r="AI163" s="1"/>
       <c r="AJ163" s="1"/>
       <c r="AN163" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="164" spans="1:40" ht="15">
@@ -7757,7 +7757,7 @@
       <c r="AI164" s="1"/>
       <c r="AJ164" s="1"/>
       <c r="AN164" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="165" spans="1:40" ht="15">
@@ -7802,7 +7802,7 @@
       <c r="AI165" s="1"/>
       <c r="AJ165" s="1"/>
       <c r="AN165" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="166" spans="1:40" ht="15">
@@ -7847,7 +7847,7 @@
       <c r="AI166" s="1"/>
       <c r="AJ166" s="1"/>
       <c r="AN166" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="167" spans="1:40" ht="15">
@@ -7892,7 +7892,7 @@
       <c r="AI167" s="1"/>
       <c r="AJ167" s="1"/>
       <c r="AN167" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="168" spans="1:40" ht="15">
@@ -7937,7 +7937,7 @@
       <c r="AI168" s="1"/>
       <c r="AJ168" s="1"/>
       <c r="AN168" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="169" spans="1:40" ht="15">
@@ -7982,7 +7982,7 @@
       <c r="AI169" s="1"/>
       <c r="AJ169" s="1"/>
       <c r="AN169" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="170" spans="1:40" ht="15">
@@ -8027,7 +8027,7 @@
       <c r="AI170" s="1"/>
       <c r="AJ170" s="1"/>
       <c r="AN170" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="171" spans="1:40" ht="15">
@@ -8087,7 +8087,7 @@
       <c r="AI171" s="1"/>
       <c r="AJ171" s="1"/>
       <c r="AN171" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="172" spans="1:40" ht="15">
@@ -8147,7 +8147,7 @@
       <c r="AI172" s="1"/>
       <c r="AJ172" s="1"/>
       <c r="AN172" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="173" spans="1:40" ht="15">
@@ -8207,7 +8207,7 @@
       <c r="AI173" s="1"/>
       <c r="AJ173" s="1"/>
       <c r="AN173" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="174" spans="1:40" ht="15">
@@ -8267,7 +8267,7 @@
       <c r="AI174" s="1"/>
       <c r="AJ174" s="1"/>
       <c r="AN174" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="175" spans="1:40" ht="15">
@@ -8327,7 +8327,7 @@
       <c r="AI175" s="1"/>
       <c r="AJ175" s="1"/>
       <c r="AN175" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="176" spans="1:40" ht="15">
@@ -8380,7 +8380,7 @@
       <c r="AI176" s="1"/>
       <c r="AJ176" s="1"/>
       <c r="AN176" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="177" spans="1:40" ht="15">
@@ -8433,7 +8433,7 @@
       <c r="AI177" s="1"/>
       <c r="AJ177" s="1"/>
       <c r="AN177" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="178" spans="1:40" ht="15">
@@ -8488,7 +8488,7 @@
       <c r="AI178" s="1"/>
       <c r="AJ178" s="1"/>
       <c r="AN178" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="179" spans="1:40" ht="15">
@@ -8533,7 +8533,7 @@
       <c r="AI179" s="1"/>
       <c r="AJ179" s="1"/>
       <c r="AN179" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="180" spans="1:40" ht="15">
@@ -8578,7 +8578,7 @@
       <c r="AI180" s="1"/>
       <c r="AJ180" s="1"/>
       <c r="AN180" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="181" spans="1:40" ht="15">
@@ -8623,7 +8623,7 @@
       <c r="AI181" s="1"/>
       <c r="AJ181" s="1"/>
       <c r="AN181" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="182" spans="1:40" ht="15">
@@ -8668,7 +8668,7 @@
       <c r="AI182" s="1"/>
       <c r="AJ182" s="1"/>
       <c r="AN182" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="183" spans="1:40" ht="15">
@@ -8713,7 +8713,7 @@
       <c r="AI183" s="1"/>
       <c r="AJ183" s="1"/>
       <c r="AN183" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="184" spans="1:40" ht="15">
@@ -8758,7 +8758,7 @@
       <c r="AI184" s="1"/>
       <c r="AJ184" s="1"/>
       <c r="AN184" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="185" spans="1:40" ht="15">
@@ -8803,7 +8803,7 @@
       <c r="AI185" s="1"/>
       <c r="AJ185" s="1"/>
       <c r="AN185" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="186" spans="1:40" ht="15">
@@ -8863,7 +8863,7 @@
       <c r="AI186" s="1"/>
       <c r="AJ186" s="1"/>
       <c r="AN186" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="187" spans="1:40" ht="15">
@@ -8923,7 +8923,7 @@
       <c r="AI187" s="1"/>
       <c r="AJ187" s="1"/>
       <c r="AN187" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="188" spans="1:40" ht="15">
@@ -8983,7 +8983,7 @@
       <c r="AI188" s="1"/>
       <c r="AJ188" s="1"/>
       <c r="AN188" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="189" spans="1:40" ht="15">
@@ -9043,7 +9043,7 @@
       <c r="AI189" s="1"/>
       <c r="AJ189" s="1"/>
       <c r="AN189" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="190" spans="1:40" ht="15">
@@ -9103,7 +9103,7 @@
       <c r="AI190" s="1"/>
       <c r="AJ190" s="1"/>
       <c r="AN190" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="191" spans="1:40" ht="15">
@@ -9157,7 +9157,7 @@
       <c r="AI191" s="1"/>
       <c r="AJ191" s="1"/>
       <c r="AN191" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="192" spans="1:40" ht="15">
@@ -9213,7 +9213,7 @@
       <c r="AI192" s="1"/>
       <c r="AJ192" s="1"/>
       <c r="AN192" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="193" spans="1:40" ht="15">
@@ -9275,7 +9275,7 @@
       <c r="AI193" s="1"/>
       <c r="AJ193" s="1"/>
       <c r="AN193" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="194" spans="1:40" ht="15">
@@ -9320,7 +9320,7 @@
       <c r="AI194" s="1"/>
       <c r="AJ194" s="1"/>
       <c r="AN194" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="195" spans="1:40" ht="15">
@@ -9365,7 +9365,7 @@
       <c r="AI195" s="1"/>
       <c r="AJ195" s="1"/>
       <c r="AN195" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="196" spans="1:40" ht="15">
@@ -9410,7 +9410,7 @@
       <c r="AI196" s="1"/>
       <c r="AJ196" s="1"/>
       <c r="AN196" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="197" spans="1:40" ht="15">
@@ -9455,7 +9455,7 @@
       <c r="AI197" s="1"/>
       <c r="AJ197" s="1"/>
       <c r="AN197" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="198" spans="1:40" ht="15">
@@ -9500,7 +9500,7 @@
       <c r="AI198" s="1"/>
       <c r="AJ198" s="1"/>
       <c r="AN198" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="199" spans="1:40" ht="15">
@@ -9545,7 +9545,7 @@
       <c r="AI199" s="1"/>
       <c r="AJ199" s="1"/>
       <c r="AN199" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="200" spans="1:40" ht="15">
@@ -9590,7 +9590,7 @@
       <c r="AI200" s="1"/>
       <c r="AJ200" s="1"/>
       <c r="AN200" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="201" spans="1:40" ht="15">
@@ -9648,7 +9648,7 @@
       <c r="AI201" s="1"/>
       <c r="AJ201" s="1"/>
       <c r="AN201" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="202" spans="1:40" ht="15">
@@ -9706,7 +9706,7 @@
       <c r="AI202" s="1"/>
       <c r="AJ202" s="1"/>
       <c r="AN202" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="203" spans="1:40" ht="15">
@@ -9764,7 +9764,7 @@
       <c r="AI203" s="1"/>
       <c r="AJ203" s="1"/>
       <c r="AN203" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="204" spans="1:40" ht="15">
@@ -9822,7 +9822,7 @@
       <c r="AI204" s="1"/>
       <c r="AJ204" s="1"/>
       <c r="AN204" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="205" spans="1:40" ht="15">
@@ -9880,7 +9880,7 @@
       <c r="AI205" s="1"/>
       <c r="AJ205" s="1"/>
       <c r="AN205" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="206" spans="1:40" ht="15">
@@ -9932,7 +9932,7 @@
       <c r="AI206" s="1"/>
       <c r="AJ206" s="1"/>
       <c r="AN206" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="207" spans="1:40" ht="15">
@@ -9983,7 +9983,7 @@
       <c r="AI207" s="1"/>
       <c r="AJ207" s="1"/>
       <c r="AN207" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="208" spans="1:40" ht="15">
@@ -10036,7 +10036,7 @@
       <c r="AI208" s="1"/>
       <c r="AJ208" s="1"/>
       <c r="AN208" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="209" spans="1:40" ht="15">
@@ -10080,7 +10080,7 @@
       <c r="AI209" s="1"/>
       <c r="AJ209" s="1"/>
       <c r="AN209" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="210" spans="1:40" ht="15">
@@ -10123,7 +10123,7 @@
       <c r="AI210" s="1"/>
       <c r="AJ210" s="1"/>
       <c r="AN210" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="211" spans="1:40" ht="15">
@@ -10166,7 +10166,7 @@
       <c r="AI211" s="1"/>
       <c r="AJ211" s="1"/>
       <c r="AN211" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="212" spans="1:40" ht="15">
@@ -10209,7 +10209,7 @@
       <c r="AI212" s="1"/>
       <c r="AJ212" s="1"/>
       <c r="AN212" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="213" spans="1:40" ht="15">
@@ -10252,7 +10252,7 @@
       <c r="AI213" s="1"/>
       <c r="AJ213" s="1"/>
       <c r="AN213" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="214" spans="1:40" ht="15">
@@ -10295,7 +10295,7 @@
       <c r="AI214" s="1"/>
       <c r="AJ214" s="1"/>
       <c r="AN214" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="215" spans="1:40" ht="15">
@@ -10338,7 +10338,7 @@
       <c r="AI215" s="1"/>
       <c r="AJ215" s="1"/>
       <c r="AN215" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="216" spans="1:40" ht="15">
@@ -10396,7 +10396,7 @@
       <c r="AI216" s="1"/>
       <c r="AJ216" s="1"/>
       <c r="AN216" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="217" spans="1:40" ht="15">
@@ -10454,7 +10454,7 @@
       <c r="AI217" s="1"/>
       <c r="AJ217" s="1"/>
       <c r="AN217" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="218" spans="1:40" ht="15">
@@ -10512,7 +10512,7 @@
       <c r="AI218" s="1"/>
       <c r="AJ218" s="1"/>
       <c r="AN218" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="219" spans="1:40" ht="15">
@@ -10570,7 +10570,7 @@
       <c r="AI219" s="1"/>
       <c r="AJ219" s="1"/>
       <c r="AN219" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="220" spans="1:40" ht="15">
@@ -10628,7 +10628,7 @@
       <c r="AI220" s="1"/>
       <c r="AJ220" s="1"/>
       <c r="AN220" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="221" spans="1:40" ht="15">
@@ -10679,7 +10679,7 @@
       <c r="AI221" s="1"/>
       <c r="AJ221" s="1"/>
       <c r="AN221" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="222" spans="1:40" ht="15">
@@ -10730,7 +10730,7 @@
       <c r="AI222" s="1"/>
       <c r="AJ222" s="1"/>
       <c r="AN222" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="223" spans="1:40" ht="15">
@@ -10781,7 +10781,7 @@
       <c r="AI223" s="1"/>
       <c r="AJ223" s="1"/>
       <c r="AN223" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="224" spans="1:40" ht="15">
@@ -10824,7 +10824,7 @@
       <c r="AI224" s="1"/>
       <c r="AJ224" s="1"/>
       <c r="AN224" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="225" spans="1:40" ht="15">
@@ -10867,7 +10867,7 @@
       <c r="AI225" s="1"/>
       <c r="AJ225" s="1"/>
       <c r="AN225" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="226" spans="1:40" ht="15">
@@ -10910,7 +10910,7 @@
       <c r="AI226" s="1"/>
       <c r="AJ226" s="1"/>
       <c r="AN226" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="227" spans="1:40" ht="15">
@@ -10953,7 +10953,7 @@
       <c r="AI227" s="1"/>
       <c r="AJ227" s="1"/>
       <c r="AN227" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="228" spans="1:40" ht="15">
@@ -10996,7 +10996,7 @@
       <c r="AI228" s="1"/>
       <c r="AJ228" s="1"/>
       <c r="AN228" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="229" spans="1:40" ht="15">
@@ -11039,7 +11039,7 @@
       <c r="AI229" s="1"/>
       <c r="AJ229" s="1"/>
       <c r="AN229" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="230" spans="1:40" ht="15">
@@ -11082,7 +11082,7 @@
       <c r="AI230" s="1"/>
       <c r="AJ230" s="1"/>
       <c r="AN230" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="231" spans="1:40" ht="15">
@@ -11142,7 +11142,7 @@
       <c r="AI231" s="1"/>
       <c r="AJ231" s="1"/>
       <c r="AN231" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="232" spans="1:40" ht="15">
@@ -11202,7 +11202,7 @@
       <c r="AI232" s="1"/>
       <c r="AJ232" s="1"/>
       <c r="AN232" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="233" spans="1:40" ht="15">
@@ -11262,7 +11262,7 @@
       <c r="AI233" s="1"/>
       <c r="AJ233" s="1"/>
       <c r="AN233" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="234" spans="1:40" ht="15">
@@ -11322,7 +11322,7 @@
       <c r="AI234" s="1"/>
       <c r="AJ234" s="1"/>
       <c r="AN234" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="235" spans="1:40" ht="15">
@@ -11382,7 +11382,7 @@
       <c r="AI235" s="1"/>
       <c r="AJ235" s="1"/>
       <c r="AN235" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="236" spans="1:40" ht="15">
@@ -11436,7 +11436,7 @@
       <c r="AI236" s="1"/>
       <c r="AJ236" s="1"/>
       <c r="AN236" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="237" spans="1:40" ht="15">
@@ -11492,7 +11492,7 @@
       <c r="AI237" s="1"/>
       <c r="AJ237" s="1"/>
       <c r="AN237" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="238" spans="1:40" ht="15">
@@ -11554,7 +11554,7 @@
       <c r="AI238" s="1"/>
       <c r="AJ238" s="1"/>
       <c r="AN238" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="239" spans="1:40" ht="15">
@@ -11601,7 +11601,7 @@
       <c r="AI239" s="1"/>
       <c r="AJ239" s="1"/>
       <c r="AN239" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="240" spans="1:40" ht="15">
@@ -11646,7 +11646,7 @@
       <c r="AI240" s="1"/>
       <c r="AJ240" s="1"/>
       <c r="AN240" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="241" spans="1:40" ht="15">
@@ -11691,7 +11691,7 @@
       <c r="AI241" s="1"/>
       <c r="AJ241" s="1"/>
       <c r="AN241" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="242" spans="1:40" ht="15">
@@ -11736,7 +11736,7 @@
       <c r="AI242" s="1"/>
       <c r="AJ242" s="1"/>
       <c r="AN242" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="243" spans="1:40" ht="15">
@@ -11781,7 +11781,7 @@
       <c r="AI243" s="1"/>
       <c r="AJ243" s="1"/>
       <c r="AN243" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="244" spans="1:40" ht="15">
@@ -11826,7 +11826,7 @@
       <c r="AI244" s="1"/>
       <c r="AJ244" s="1"/>
       <c r="AN244" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="245" spans="1:40" ht="15">
@@ -11871,7 +11871,7 @@
       <c r="AI245" s="1"/>
       <c r="AJ245" s="1"/>
       <c r="AN245" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="246" spans="1:40" ht="15">
@@ -11929,7 +11929,7 @@
       <c r="AI246" s="1"/>
       <c r="AJ246" s="1"/>
       <c r="AN246" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="247" spans="1:40" ht="15">
@@ -11987,7 +11987,7 @@
       <c r="AI247" s="1"/>
       <c r="AJ247" s="1"/>
       <c r="AN247" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="248" spans="1:40" ht="15">
@@ -12045,7 +12045,7 @@
       <c r="AI248" s="1"/>
       <c r="AJ248" s="1"/>
       <c r="AN248" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="249" spans="1:40" ht="15">
@@ -12103,7 +12103,7 @@
       <c r="AI249" s="1"/>
       <c r="AJ249" s="1"/>
       <c r="AN249" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="250" spans="1:40" ht="15">
@@ -12161,7 +12161,7 @@
       <c r="AI250" s="1"/>
       <c r="AJ250" s="1"/>
       <c r="AN250" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="251" spans="1:40" ht="15">
@@ -12212,7 +12212,7 @@
       <c r="AI251" s="1"/>
       <c r="AJ251" s="1"/>
       <c r="AN251" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="252" spans="1:40" ht="15">
@@ -12263,7 +12263,7 @@
       <c r="AI252" s="1"/>
       <c r="AJ252" s="1"/>
       <c r="AN252" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="253" spans="1:40" ht="15">
@@ -12313,7 +12313,7 @@
       <c r="AI253" s="1"/>
       <c r="AJ253" s="1"/>
       <c r="AN253" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="254" spans="1:40" ht="15">
@@ -12356,7 +12356,7 @@
       <c r="AI254" s="1"/>
       <c r="AJ254" s="1"/>
       <c r="AN254" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="255" spans="1:40" ht="15">
@@ -12399,7 +12399,7 @@
       <c r="AI255" s="1"/>
       <c r="AJ255" s="1"/>
       <c r="AN255" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="256" spans="1:40" ht="15">
@@ -12442,7 +12442,7 @@
       <c r="AI256" s="1"/>
       <c r="AJ256" s="1"/>
       <c r="AN256" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="257" spans="1:40" ht="15">
@@ -12485,7 +12485,7 @@
       <c r="AI257" s="1"/>
       <c r="AJ257" s="1"/>
       <c r="AN257" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="258" spans="1:40" ht="15">
@@ -12528,7 +12528,7 @@
       <c r="AI258" s="1"/>
       <c r="AJ258" s="1"/>
       <c r="AN258" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="259" spans="1:40" ht="15">
@@ -12571,7 +12571,7 @@
       <c r="AI259" s="1"/>
       <c r="AJ259" s="1"/>
       <c r="AN259" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="260" spans="1:40" ht="15">
@@ -12614,7 +12614,7 @@
       <c r="AI260" s="1"/>
       <c r="AJ260" s="1"/>
       <c r="AN260" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="261" spans="1:40" ht="15">
@@ -12670,7 +12670,7 @@
       <c r="AI261" s="1"/>
       <c r="AJ261" s="1"/>
       <c r="AN261" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="262" spans="1:40" ht="15">
@@ -12726,7 +12726,7 @@
       <c r="AI262" s="1"/>
       <c r="AJ262" s="1"/>
       <c r="AN262" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="263" spans="1:40" ht="15">
@@ -12782,7 +12782,7 @@
       <c r="AI263" s="1"/>
       <c r="AJ263" s="1"/>
       <c r="AN263" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="264" spans="1:40" ht="15">
@@ -12838,7 +12838,7 @@
       <c r="AI264" s="1"/>
       <c r="AJ264" s="1"/>
       <c r="AN264" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="265" spans="1:40" ht="15">
@@ -12894,7 +12894,7 @@
       <c r="AI265" s="1"/>
       <c r="AJ265" s="1"/>
       <c r="AN265" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="266" spans="1:40" ht="15">
@@ -12944,7 +12944,7 @@
       <c r="AI266" s="1"/>
       <c r="AJ266" s="1"/>
       <c r="AN266" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="267" spans="1:40" ht="15">
@@ -12994,7 +12994,7 @@
       <c r="AI267" s="1"/>
       <c r="AJ267" s="1"/>
       <c r="AN267" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="268" spans="1:40" ht="15">
@@ -13046,7 +13046,7 @@
       <c r="AI268" s="1"/>
       <c r="AJ268" s="1"/>
       <c r="AN268" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="269" spans="1:40" ht="15">
@@ -13089,7 +13089,7 @@
       <c r="AI269" s="1"/>
       <c r="AJ269" s="1"/>
       <c r="AN269" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="270" spans="1:40" ht="15">
@@ -13132,7 +13132,7 @@
       <c r="AI270" s="1"/>
       <c r="AJ270" s="1"/>
       <c r="AN270" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="271" spans="1:40" ht="15">
@@ -13175,7 +13175,7 @@
       <c r="AI271" s="1"/>
       <c r="AJ271" s="1"/>
       <c r="AN271" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="272" spans="1:40" ht="15">
@@ -13218,7 +13218,7 @@
       <c r="AI272" s="1"/>
       <c r="AJ272" s="1"/>
       <c r="AN272" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="273" spans="1:40" ht="15">
@@ -13261,7 +13261,7 @@
       <c r="AI273" s="1"/>
       <c r="AJ273" s="1"/>
       <c r="AN273" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="274" spans="1:40" ht="15">
@@ -13304,7 +13304,7 @@
       <c r="AI274" s="1"/>
       <c r="AJ274" s="1"/>
       <c r="AN274" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="275" spans="1:40" ht="15">
@@ -13347,7 +13347,7 @@
       <c r="AI275" s="1"/>
       <c r="AJ275" s="1"/>
       <c r="AN275" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="276" spans="1:40" ht="15">
@@ -27881,7 +27881,7 @@
     </row>
     <row r="828" spans="1:40">
       <c r="A828" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B828" s="16">
         <v>26860</v>
@@ -27901,7 +27901,7 @@
     </row>
     <row r="829" spans="1:40">
       <c r="A829" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B829" s="5">
         <v>27590.484400000001</v>
@@ -27935,7 +27935,7 @@
       <c r="T829" s="39"/>
       <c r="U829" s="39"/>
       <c r="V829" s="28">
-        <v>23.86</v>
+        <v>2.3860000000000001</v>
       </c>
       <c r="W829" s="28"/>
       <c r="AA829" s="17">
@@ -27960,7 +27960,7 @@
     </row>
     <row r="830" spans="1:40">
       <c r="A830" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B830" s="5">
         <v>27955.726600000002</v>
@@ -27994,7 +27994,7 @@
       <c r="T830" s="39"/>
       <c r="U830" s="39"/>
       <c r="V830" s="28">
-        <v>57.77</v>
+        <v>5.777000000000001</v>
       </c>
       <c r="W830" s="28"/>
       <c r="AA830" s="17">
@@ -28019,7 +28019,7 @@
     </row>
     <row r="831" spans="1:40">
       <c r="A831" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B831" s="5">
         <v>28320.968799999999</v>
@@ -28053,7 +28053,7 @@
       <c r="T831" s="39"/>
       <c r="U831" s="39"/>
       <c r="V831" s="28">
-        <v>170.87</v>
+        <v>17.087</v>
       </c>
       <c r="W831" s="28"/>
       <c r="AA831" s="17">
@@ -28078,7 +28078,7 @@
     </row>
     <row r="832" spans="1:40">
       <c r="A832" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B832" s="5">
         <v>28686.210999999999</v>
@@ -28112,7 +28112,7 @@
       <c r="T832" s="39"/>
       <c r="U832" s="39"/>
       <c r="V832" s="28">
-        <v>280.95</v>
+        <v>28.094999999999999</v>
       </c>
       <c r="W832" s="28"/>
       <c r="AA832" s="17">
@@ -28141,7 +28141,7 @@
     </row>
     <row r="833" spans="1:40">
       <c r="A833" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B833" s="5">
         <v>29047.800778000001</v>
@@ -28175,7 +28175,7 @@
       <c r="T833" s="39"/>
       <c r="U833" s="39"/>
       <c r="V833" s="28">
-        <v>367.58</v>
+        <v>36.758000000000003</v>
       </c>
       <c r="W833" s="28"/>
       <c r="AA833" s="17">
@@ -28204,7 +28204,7 @@
     </row>
     <row r="834" spans="1:40">
       <c r="A834" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B834" s="5">
         <v>29051.4532</v>
@@ -28238,7 +28238,7 @@
       <c r="T834" s="39"/>
       <c r="U834" s="39"/>
       <c r="V834" s="28">
-        <v>89.95</v>
+        <v>8.995000000000001</v>
       </c>
       <c r="W834" s="28"/>
       <c r="AA834" s="17">
@@ -28267,7 +28267,7 @@
     </row>
     <row r="835" spans="1:40">
       <c r="A835" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B835" s="5">
         <v>29416.695400000001</v>
@@ -28301,7 +28301,7 @@
       <c r="T835" s="39"/>
       <c r="U835" s="39"/>
       <c r="V835" s="28">
-        <v>155.59</v>
+        <v>15.559000000000001</v>
       </c>
       <c r="W835" s="28"/>
       <c r="AA835" s="17">
@@ -28330,7 +28330,7 @@
     </row>
     <row r="836" spans="1:40">
       <c r="A836" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B836" s="5">
         <v>29781.937600000001</v>
@@ -28364,7 +28364,7 @@
       <c r="T836" s="39"/>
       <c r="U836" s="39"/>
       <c r="V836" s="28">
-        <v>238.24</v>
+        <v>23.824000000000002</v>
       </c>
       <c r="W836" s="28"/>
       <c r="AA836" s="17">
@@ -28393,7 +28393,7 @@
     </row>
     <row r="837" spans="1:40">
       <c r="A837" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B837" s="5">
         <v>30147.179800000002</v>
@@ -28427,7 +28427,7 @@
       <c r="T837" s="39"/>
       <c r="U837" s="39"/>
       <c r="V837" s="28">
-        <v>287.86</v>
+        <v>28.786000000000001</v>
       </c>
       <c r="W837" s="28"/>
       <c r="AA837" s="17">
@@ -28456,7 +28456,7 @@
     </row>
     <row r="838" spans="1:40">
       <c r="A838" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B838" s="5">
         <v>30508.769577999999</v>
@@ -28490,7 +28490,7 @@
       <c r="T838" s="39"/>
       <c r="U838" s="39"/>
       <c r="V838" s="28">
-        <v>327.52</v>
+        <v>32.752000000000002</v>
       </c>
       <c r="W838" s="28"/>
       <c r="AA838" s="17">
@@ -28519,7 +28519,7 @@
     </row>
     <row r="839" spans="1:40">
       <c r="A839" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B839" s="5">
         <v>30512.421999999999</v>
@@ -28553,7 +28553,7 @@
       <c r="T839" s="39"/>
       <c r="U839" s="39"/>
       <c r="V839" s="28">
-        <v>108.8</v>
+        <v>10.88</v>
       </c>
       <c r="W839" s="28"/>
       <c r="AA839" s="17">
@@ -28582,7 +28582,7 @@
     </row>
     <row r="840" spans="1:40">
       <c r="A840" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B840" s="5">
         <v>30877.664199999999</v>
@@ -28616,7 +28616,7 @@
       <c r="T840" s="39"/>
       <c r="U840" s="39"/>
       <c r="V840" s="28">
-        <v>163.93</v>
+        <v>16.393000000000001</v>
       </c>
       <c r="W840" s="28"/>
       <c r="AA840" s="17">
@@ -28645,7 +28645,7 @@
     </row>
     <row r="841" spans="1:40">
       <c r="A841" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B841" s="5">
         <v>31242.9064</v>
@@ -28679,7 +28679,7 @@
       <c r="T841" s="39"/>
       <c r="U841" s="39"/>
       <c r="V841" s="28">
-        <v>213.97</v>
+        <v>21.397000000000002</v>
       </c>
       <c r="W841" s="28"/>
       <c r="AA841" s="17">
@@ -28722,6 +28722,7 @@
       <c r="E842" s="3">
         <v>2220</v>
       </c>
+      <c r="U842" s="39"/>
       <c r="AN842" s="1" t="s">
         <v>24</v>
       </c>
@@ -28743,6 +28744,7 @@
       <c r="E843">
         <v>1975</v>
       </c>
+      <c r="U843" s="39"/>
       <c r="AA843" s="17">
         <v>1.8</v>
       </c>
@@ -28770,6 +28772,7 @@
       <c r="E844">
         <v>1935</v>
       </c>
+      <c r="U844" s="39"/>
       <c r="AA844" s="17">
         <v>2.9</v>
       </c>
@@ -28797,6 +28800,7 @@
       <c r="E845">
         <v>1930</v>
       </c>
+      <c r="U845" s="39"/>
       <c r="AA845" s="17">
         <v>4.3</v>
       </c>
@@ -28824,6 +28828,7 @@
       <c r="E846">
         <v>1930</v>
       </c>
+      <c r="U846" s="39"/>
       <c r="AA846" s="17">
         <v>6.3</v>
       </c>
@@ -28859,6 +28864,7 @@
       <c r="E847">
         <v>1910</v>
       </c>
+      <c r="U847" s="39"/>
       <c r="AA847" s="17">
         <v>8.3000000000000007</v>
       </c>
@@ -28894,6 +28900,7 @@
       <c r="E848">
         <v>1905</v>
       </c>
+      <c r="U848" s="39"/>
       <c r="AA848" s="17">
         <v>9.6</v>
       </c>
@@ -28929,6 +28936,7 @@
       <c r="E849">
         <v>1875</v>
       </c>
+      <c r="U849" s="39"/>
       <c r="AA849" s="17">
         <v>10.9</v>
       </c>
@@ -28964,6 +28972,7 @@
       <c r="E850">
         <v>1750</v>
       </c>
+      <c r="U850" s="39"/>
       <c r="AA850" s="17">
         <v>12.4</v>
       </c>
@@ -28999,6 +29008,7 @@
       <c r="E851">
         <v>1645</v>
       </c>
+      <c r="U851" s="39"/>
       <c r="AA851" s="17">
         <v>13.9</v>
       </c>
@@ -29034,6 +29044,7 @@
       <c r="E852">
         <v>1610</v>
       </c>
+      <c r="U852" s="39"/>
       <c r="AA852" s="17">
         <v>15.3</v>
       </c>
@@ -29087,7 +29098,7 @@
       <c r="T853" s="39"/>
       <c r="U853" s="39"/>
       <c r="V853" s="3">
-        <v>560.6</v>
+        <v>56.06</v>
       </c>
       <c r="AA853" s="17">
         <v>17.8</v>
@@ -29112,7 +29123,7 @@
     </row>
     <row r="854" spans="1:40">
       <c r="A854" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B854" s="5">
         <v>31093</v>
@@ -29124,12 +29135,12 @@
         <v>1260</v>
       </c>
       <c r="AN854" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="855" spans="1:40">
       <c r="A855" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B855" s="5">
         <v>33649.695399999997</v>
@@ -29160,12 +29171,12 @@
         <v>9.8999999999999991E-3</v>
       </c>
       <c r="AN855" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="856" spans="1:40">
       <c r="A856" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B856" s="5">
         <v>34014.937599999997</v>
@@ -29199,12 +29210,12 @@
         <v>9.8999999999999991E-3</v>
       </c>
       <c r="AN856" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="857" spans="1:40">
       <c r="A857" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B857" s="5">
         <v>34380.179799999998</v>
@@ -29238,12 +29249,12 @@
         <v>9.0000000000000011E-3</v>
       </c>
       <c r="AN857" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="858" spans="1:40">
       <c r="A858" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B858" s="5">
         <v>34745.421999999999</v>
@@ -29280,12 +29291,12 @@
         <v>9.4999999999999998E-3</v>
       </c>
       <c r="AN858" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="859" spans="1:40">
       <c r="A859" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B859" s="5">
         <v>35110.664199999999</v>
@@ -29322,12 +29333,12 @@
         <v>9.300000000000001E-3</v>
       </c>
       <c r="AN859" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="860" spans="1:40">
       <c r="A860" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B860" s="5">
         <v>35475.9064</v>
@@ -29364,12 +29375,12 @@
         <v>9.8999999999999991E-3</v>
       </c>
       <c r="AN860" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="861" spans="1:40">
       <c r="A861" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B861" s="5">
         <v>35841.1486</v>
@@ -29403,12 +29414,12 @@
         <v>1.0500000000000001E-2</v>
       </c>
       <c r="AN861" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="862" spans="1:40">
       <c r="A862" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B862" s="5">
         <v>36206.390800000001</v>
@@ -29442,12 +29453,12 @@
         <v>1.03E-2</v>
       </c>
       <c r="AN862" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="863" spans="1:40">
       <c r="A863" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B863" s="5">
         <v>36571.633000000002</v>
@@ -29481,12 +29492,12 @@
         <v>1.03E-2</v>
       </c>
       <c r="AN863" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="864" spans="1:40">
       <c r="A864" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B864" s="5">
         <v>36936.875200000002</v>
@@ -29520,12 +29531,12 @@
         <v>1.0500000000000001E-2</v>
       </c>
       <c r="AN864" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="865" spans="1:40">
       <c r="A865" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B865" s="5">
         <v>31062</v>
@@ -29541,12 +29552,12 @@
         <v>1260</v>
       </c>
       <c r="AN865" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="866" spans="1:40">
       <c r="A866" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B866" s="5">
         <v>33649.695399999997</v>
@@ -29577,12 +29588,12 @@
         <v>9.8999999999999991E-3</v>
       </c>
       <c r="AN866" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="867" spans="1:40">
       <c r="A867" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B867" s="5">
         <v>34014.937599999997</v>
@@ -29616,12 +29627,12 @@
         <v>1.0700000000000001E-2</v>
       </c>
       <c r="AN867" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="868" spans="1:40">
       <c r="A868" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B868" s="5">
         <v>34380.179799999998</v>
@@ -29655,12 +29666,12 @@
         <v>8.8000000000000005E-3</v>
       </c>
       <c r="AN868" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="869" spans="1:40">
       <c r="A869" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B869" s="5">
         <v>34745.421999999999</v>
@@ -29697,12 +29708,12 @@
         <v>9.7000000000000003E-3</v>
       </c>
       <c r="AN869" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="870" spans="1:40">
       <c r="A870" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B870" s="5">
         <v>35110.664199999999</v>
@@ -29739,12 +29750,12 @@
         <v>1.0500000000000001E-2</v>
       </c>
       <c r="AN870" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="871" spans="1:40">
       <c r="A871" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B871" s="5">
         <v>35475.9064</v>
@@ -29781,12 +29792,12 @@
         <v>1.06E-2</v>
       </c>
       <c r="AN871" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="872" spans="1:40">
       <c r="A872" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B872" s="5">
         <v>35841.1486</v>
@@ -29820,12 +29831,12 @@
         <v>1.06E-2</v>
       </c>
       <c r="AN872" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="873" spans="1:40">
       <c r="A873" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B873" s="5">
         <v>36206.390800000001</v>
@@ -29859,12 +29870,12 @@
         <v>1.06E-2</v>
       </c>
       <c r="AN873" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="874" spans="1:40">
       <c r="A874" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B874" s="5">
         <v>36571.633000000002</v>
@@ -29898,12 +29909,12 @@
         <v>1.03E-2</v>
       </c>
       <c r="AN874" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="875" spans="1:40">
       <c r="A875" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B875" s="5">
         <v>36936.875200000002</v>
@@ -29937,12 +29948,12 @@
         <v>1.1000000000000001E-2</v>
       </c>
       <c r="AN875" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="876" spans="1:40">
       <c r="A876" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B876" s="5">
         <v>31062</v>
@@ -29958,12 +29969,12 @@
         <v>1260</v>
       </c>
       <c r="AN876" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="877" spans="1:40">
       <c r="A877" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B877" s="5">
         <v>33649.695399999997</v>
@@ -29994,12 +30005,12 @@
         <v>9.5999999999999992E-3</v>
       </c>
       <c r="AN877" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="878" spans="1:40">
       <c r="A878" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B878" s="5">
         <v>34014.937599999997</v>
@@ -30033,12 +30044,12 @@
         <v>1.3100000000000001E-2</v>
       </c>
       <c r="AN878" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="879" spans="1:40">
       <c r="A879" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B879" s="5">
         <v>34380.179799999998</v>
@@ -30072,12 +30083,12 @@
         <v>1.18E-2</v>
       </c>
       <c r="AN879" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="880" spans="1:40">
       <c r="A880" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B880" s="5">
         <v>34745.421999999999</v>
@@ -30114,12 +30125,12 @@
         <v>1.3100000000000001E-2</v>
       </c>
       <c r="AN880" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="881" spans="1:40">
       <c r="A881" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B881" s="5">
         <v>35110.664199999999</v>
@@ -30156,12 +30167,12 @@
         <v>1.24E-2</v>
       </c>
       <c r="AN881" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="882" spans="1:40">
       <c r="A882" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B882" s="5">
         <v>35475.9064</v>
@@ -30198,12 +30209,12 @@
         <v>1.4499999999999999E-2</v>
       </c>
       <c r="AN882" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="883" spans="1:40">
       <c r="A883" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B883" s="5">
         <v>35841.1486</v>
@@ -30237,12 +30248,12 @@
         <v>1.54E-2</v>
       </c>
       <c r="AN883" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="884" spans="1:40">
       <c r="A884" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B884" s="5">
         <v>36206.390800000001</v>
@@ -30276,12 +30287,12 @@
         <v>1.44E-2</v>
       </c>
       <c r="AN884" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="885" spans="1:40">
       <c r="A885" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B885" s="5">
         <v>36571.633000000002</v>
@@ -30315,12 +30326,12 @@
         <v>1.47E-2</v>
       </c>
       <c r="AN885" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="886" spans="1:40">
       <c r="A886" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B886" s="5">
         <v>36936.875200000002</v>
@@ -30354,12 +30365,12 @@
         <v>1.6200000000000003E-2</v>
       </c>
       <c r="AN886" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="887" spans="1:40">
       <c r="A887" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B887" s="5">
         <v>31093</v>
@@ -30375,12 +30386,12 @@
         <v>1260</v>
       </c>
       <c r="AN887" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="888" spans="1:40">
       <c r="A888" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B888" s="5">
         <v>33649.695399999997</v>
@@ -30411,12 +30422,12 @@
         <v>9.7000000000000003E-3</v>
       </c>
       <c r="AN888" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="889" spans="1:40">
       <c r="A889" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B889" s="5">
         <v>34014.937599999997</v>
@@ -30450,12 +30461,12 @@
         <v>1.29E-2</v>
       </c>
       <c r="AN889" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="890" spans="1:40">
       <c r="A890" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B890" s="5">
         <v>34380.179799999998</v>
@@ -30489,12 +30500,12 @@
         <v>1.11E-2</v>
       </c>
       <c r="AN890" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="891" spans="1:40">
       <c r="A891" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B891" s="5">
         <v>34745.421999999999</v>
@@ -30531,12 +30542,12 @@
         <v>1.3000000000000001E-2</v>
       </c>
       <c r="AN891" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="892" spans="1:40">
       <c r="A892" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B892" s="5">
         <v>35110.664199999999</v>
@@ -30573,12 +30584,12 @@
         <v>1.1299999999999999E-2</v>
       </c>
       <c r="AN892" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="893" spans="1:40">
       <c r="A893" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B893" s="5">
         <v>35475.9064</v>
@@ -30615,12 +30626,12 @@
         <v>1.3999999999999999E-2</v>
       </c>
       <c r="AN893" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="894" spans="1:40">
       <c r="A894" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B894" s="5">
         <v>35841.1486</v>
@@ -30654,12 +30665,12 @@
         <v>1.38E-2</v>
       </c>
       <c r="AN894" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="895" spans="1:40">
       <c r="A895" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B895" s="5">
         <v>36206.390800000001</v>
@@ -30693,12 +30704,12 @@
         <v>1.32E-2</v>
       </c>
       <c r="AN895" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="896" spans="1:40">
       <c r="A896" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B896" s="5">
         <v>36571.633000000002</v>
@@ -30732,12 +30743,12 @@
         <v>1.3600000000000001E-2</v>
       </c>
       <c r="AN896" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="897" spans="1:40" hidden="1">
       <c r="A897" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B897" s="5">
         <v>36936.875200000002</v>
@@ -30771,12 +30782,12 @@
         <v>1.47E-2</v>
       </c>
       <c r="AN897" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="898" spans="1:40" hidden="1">
       <c r="A898" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B898" s="5">
         <v>34014.937604166669</v>
@@ -30813,12 +30824,12 @@
         <v>320</v>
       </c>
       <c r="AN898" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="899" spans="1:40" hidden="1">
       <c r="A899" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B899" s="5">
         <v>34014.937604166669</v>
@@ -30855,12 +30866,12 @@
         <v>270</v>
       </c>
       <c r="AN899" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="900" spans="1:40" hidden="1">
       <c r="A900" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B900" s="5">
         <v>34014.937604166669</v>
@@ -30897,12 +30908,12 @@
         <v>470</v>
       </c>
       <c r="AN900" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="901" spans="1:40" hidden="1">
       <c r="A901" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B901" s="5">
         <v>34014.937604166669</v>
@@ -30939,12 +30950,12 @@
         <v>350</v>
       </c>
       <c r="AN901" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="902" spans="1:40" hidden="1">
       <c r="A902" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B902" s="5">
         <v>35017.937604166669</v>
@@ -30981,12 +30992,12 @@
         <v>610</v>
       </c>
       <c r="AN902" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="903" spans="1:40" hidden="1">
       <c r="A903" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B903" s="5">
         <v>35017.937604166669</v>
@@ -31023,12 +31034,12 @@
         <v>700</v>
       </c>
       <c r="AN903" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="904" spans="1:40" hidden="1">
       <c r="A904" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B904" s="5">
         <v>35017.937604166669</v>
@@ -31065,12 +31076,12 @@
         <v>1239.9999999999998</v>
       </c>
       <c r="AN904" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="905" spans="1:40" hidden="1">
       <c r="A905" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B905" s="5">
         <v>35017.937604166669</v>
@@ -31107,12 +31118,12 @@
         <v>1350</v>
       </c>
       <c r="AN905" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="906" spans="1:40" hidden="1">
       <c r="A906" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B906" s="5">
         <v>36936.875196759262</v>
@@ -31149,12 +31160,12 @@
         <v>1110</v>
       </c>
       <c r="AN906" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="907" spans="1:40" hidden="1">
       <c r="A907" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B907" s="5">
         <v>36936.875196759262</v>
@@ -31191,12 +31202,12 @@
         <v>1250</v>
       </c>
       <c r="AN907" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="908" spans="1:40" hidden="1">
       <c r="A908" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B908" s="5">
         <v>36936.875196759262</v>
@@ -31233,12 +31244,12 @@
         <v>2570</v>
       </c>
       <c r="AN908" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="909" spans="1:40" hidden="1">
       <c r="A909" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B909" s="5">
         <v>36936.875196759262</v>
@@ -31275,12 +31286,12 @@
         <v>2860</v>
       </c>
       <c r="AN909" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="910" spans="1:40" hidden="1">
       <c r="A910" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B910" s="5">
         <v>35581.421999999999</v>
@@ -31301,12 +31312,12 @@
         <v>13.2</v>
       </c>
       <c r="AN910" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="911" spans="1:40" hidden="1">
       <c r="A911" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B911" s="5">
         <v>35581.421999999999</v>
@@ -31327,12 +31338,12 @@
         <v>17.100000000000001</v>
       </c>
       <c r="AN911" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="912" spans="1:40" hidden="1">
       <c r="A912" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B912" s="5">
         <v>35581.421999999999</v>
@@ -31353,12 +31364,12 @@
         <v>20</v>
       </c>
       <c r="AN912" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="913" spans="1:40" hidden="1">
       <c r="A913" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B913" s="5">
         <v>35581.421999999999</v>
@@ -31379,12 +31390,12 @@
         <v>18.899999999999999</v>
       </c>
       <c r="AN913" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="914" spans="1:40" hidden="1">
       <c r="A914" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B914" s="5">
         <v>35534.421999999999</v>
@@ -31405,12 +31416,12 @@
         <v>11.3</v>
       </c>
       <c r="AN914" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="915" spans="1:40" hidden="1">
       <c r="A915" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B915" s="5">
         <v>35534.421999999999</v>
@@ -31431,12 +31442,12 @@
         <v>18.8</v>
       </c>
       <c r="AN915" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="916" spans="1:40" hidden="1">
       <c r="A916" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B916" s="5">
         <v>35534.421999999999</v>
@@ -31457,12 +31468,12 @@
         <v>16.899999999999999</v>
       </c>
       <c r="AN916" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="917" spans="1:40" hidden="1">
       <c r="A917" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B917" s="5">
         <v>35534.421999999999</v>
@@ -31483,12 +31494,12 @@
         <v>16.3</v>
       </c>
       <c r="AN917" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="918" spans="1:40" hidden="1">
       <c r="A918" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B918" s="5">
         <v>35550.421999999999</v>
@@ -31509,12 +31520,12 @@
         <v>10.6</v>
       </c>
       <c r="AN918" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="919" spans="1:40" hidden="1">
       <c r="A919" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B919" s="5">
         <v>35550.421999999999</v>
@@ -31535,12 +31546,12 @@
         <v>14.2</v>
       </c>
       <c r="AN919" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="920" spans="1:40" hidden="1">
       <c r="A920" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B920" s="5">
         <v>35550.421999999999</v>
@@ -31561,12 +31572,12 @@
         <v>14.6</v>
       </c>
       <c r="AN920" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="921" spans="1:40" hidden="1">
       <c r="A921" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B921" s="5">
         <v>35550.421999999999</v>
@@ -31587,12 +31598,12 @@
         <v>13.5</v>
       </c>
       <c r="AN921" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="922" spans="1:40" hidden="1">
       <c r="A922" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B922" s="5">
         <v>37407.633000000002</v>
@@ -31625,12 +31636,12 @@
         <v>18.600000000000001</v>
       </c>
       <c r="AN922" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="923" spans="1:40" hidden="1">
       <c r="A923" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B923" s="5">
         <v>37407.633000000002</v>
@@ -31663,12 +31674,12 @@
         <v>22.7</v>
       </c>
       <c r="AN923" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="924" spans="1:40" hidden="1">
       <c r="A924" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B924" s="5">
         <v>37407.633000000002</v>
@@ -31701,12 +31712,12 @@
         <v>25.4</v>
       </c>
       <c r="AN924" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="925" spans="1:40" hidden="1">
       <c r="A925" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B925" s="5">
         <v>37407.633000000002</v>
@@ -31739,12 +31750,12 @@
         <v>25.1</v>
       </c>
       <c r="AN925" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="926" spans="1:40" hidden="1">
       <c r="A926" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B926" s="5">
         <v>37360.633000000002</v>
@@ -31777,12 +31788,12 @@
         <v>16.8</v>
       </c>
       <c r="AN926" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="927" spans="1:40" hidden="1">
       <c r="A927" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B927" s="5">
         <v>37360.633000000002</v>
@@ -31815,12 +31826,12 @@
         <v>24.9</v>
       </c>
       <c r="AN927" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="928" spans="1:40" hidden="1">
       <c r="A928" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B928" s="5">
         <v>37360.633000000002</v>
@@ -31853,12 +31864,12 @@
         <v>22</v>
       </c>
       <c r="AN928" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="929" spans="1:40" hidden="1">
       <c r="A929" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B929" s="5">
         <v>37360.633000000002</v>
@@ -31891,12 +31902,12 @@
         <v>22.1</v>
       </c>
       <c r="AN929" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="930" spans="1:40" hidden="1">
       <c r="A930" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B930" s="5">
         <v>37376.633000000002</v>
@@ -31929,12 +31940,12 @@
         <v>14.1</v>
       </c>
       <c r="AN930" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="931" spans="1:40" hidden="1">
       <c r="A931" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B931" s="5">
         <v>37376.633000000002</v>
@@ -31967,12 +31978,12 @@
         <v>19.2</v>
       </c>
       <c r="AN931" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="932" spans="1:40" hidden="1">
       <c r="A932" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B932" s="5">
         <v>37376.633000000002</v>
@@ -32005,12 +32016,12 @@
         <v>18.8</v>
       </c>
       <c r="AN932" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="933" spans="1:40" hidden="1">
       <c r="A933" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B933" s="5">
         <v>37376.633000000002</v>
@@ -32043,12 +32054,12 @@
         <v>17.7</v>
       </c>
       <c r="AN933" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="934" spans="1:40" hidden="1">
       <c r="A934" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B934" s="5">
         <v>36022.211000000003</v>
@@ -32065,7 +32076,7 @@
     </row>
     <row r="935" spans="1:40" hidden="1">
       <c r="A935" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B935" s="5">
         <v>36752.695400000004</v>
@@ -32094,7 +32105,7 @@
     </row>
     <row r="936" spans="1:40" hidden="1">
       <c r="A936" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B936" s="5">
         <v>37117.937600000005</v>
@@ -32123,7 +32134,7 @@
     </row>
     <row r="937" spans="1:40" hidden="1">
       <c r="A937" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B937" s="5">
         <v>37483.179800000005</v>
@@ -32152,7 +32163,7 @@
     </row>
     <row r="938" spans="1:40" hidden="1">
       <c r="A938" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B938" s="5">
         <v>37848.422000000006</v>
@@ -32181,7 +32192,7 @@
     </row>
     <row r="939" spans="1:40" hidden="1">
       <c r="A939" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B939" s="5">
         <v>38578.9064</v>
@@ -32210,7 +32221,7 @@
     </row>
     <row r="940" spans="1:40" hidden="1">
       <c r="A940" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B940" s="5">
         <v>38944.1486</v>
@@ -32239,7 +32250,7 @@
     </row>
     <row r="941" spans="1:40" hidden="1">
       <c r="A941" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B941" s="5">
         <v>39309.390800000001</v>
@@ -32268,7 +32279,7 @@
     </row>
     <row r="942" spans="1:40" hidden="1">
       <c r="A942" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B942" s="5">
         <v>39674.633000000002</v>
@@ -32300,7 +32311,7 @@
     <row r="945" spans="1:68" hidden="1"/>
     <row r="946" spans="1:68">
       <c r="A946" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B946" s="5">
         <v>22812</v>
@@ -32317,7 +32328,7 @@
     </row>
     <row r="947" spans="1:68">
       <c r="A947" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B947" s="5">
         <v>29021.117399999999</v>
@@ -32344,7 +32355,7 @@
     </row>
     <row r="948" spans="1:68">
       <c r="A948" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B948" s="5">
         <v>29386.3596</v>
@@ -32371,7 +32382,7 @@
     </row>
     <row r="949" spans="1:68">
       <c r="A949" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B949" s="5">
         <v>29751.6018</v>
@@ -32398,7 +32409,7 @@
     </row>
     <row r="950" spans="1:68">
       <c r="A950" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B950" s="5">
         <v>30116.844000000001</v>
@@ -32425,7 +32436,7 @@
     </row>
     <row r="951" spans="1:68">
       <c r="A951" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B951" s="5">
         <v>30482.086200000002</v>
@@ -32452,7 +32463,7 @@
     </row>
     <row r="952" spans="1:68">
       <c r="A952" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B952" s="5">
         <v>30847.328399999999</v>
@@ -32479,7 +32490,7 @@
     </row>
     <row r="953" spans="1:68">
       <c r="A953" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B953" s="5">
         <v>31212.570599999999</v>
@@ -32506,7 +32517,7 @@
     </row>
     <row r="954" spans="1:68">
       <c r="A954" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B954" s="5">
         <v>31577.8128</v>
@@ -32533,7 +32544,7 @@
     </row>
     <row r="955" spans="1:68">
       <c r="A955" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B955" s="5">
         <v>31943.055</v>
@@ -32626,7 +32637,7 @@
     </row>
     <row r="956" spans="1:68">
       <c r="A956" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B956" s="5">
         <v>32308.297200000001</v>
@@ -32650,7 +32661,7 @@
     </row>
     <row r="957" spans="1:68">
       <c r="A957" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B957" s="5">
         <v>32673.539400000001</v>
@@ -32677,7 +32688,7 @@
     </row>
     <row r="958" spans="1:68">
       <c r="A958" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B958" s="5">
         <v>33038.781600000002</v>
@@ -32704,7 +32715,7 @@
     </row>
     <row r="959" spans="1:68">
       <c r="A959" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B959" s="5">
         <v>33404.023800000003</v>
@@ -32779,7 +32790,7 @@
     </row>
     <row r="960" spans="1:68">
       <c r="A960" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B960" s="5">
         <v>33769.266000000003</v>
@@ -32806,7 +32817,7 @@
     </row>
     <row r="961" spans="1:68">
       <c r="A961" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B961" s="5">
         <v>34134.508199999997</v>
@@ -32833,7 +32844,7 @@
     </row>
     <row r="962" spans="1:68">
       <c r="A962" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B962" s="5">
         <v>34499.750400000004</v>
@@ -32860,7 +32871,7 @@
     </row>
     <row r="963" spans="1:68">
       <c r="A963" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B963" s="5">
         <v>34864.992599999998</v>
@@ -32887,7 +32898,7 @@
     </row>
     <row r="964" spans="1:68">
       <c r="A964" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B964" s="5">
         <v>35230.234799999998</v>
@@ -32962,7 +32973,7 @@
     </row>
     <row r="965" spans="1:68">
       <c r="A965" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B965" s="5">
         <v>29021.117399999999</v>
@@ -32989,7 +33000,7 @@
     </row>
     <row r="966" spans="1:68">
       <c r="A966" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B966" s="5">
         <v>29386.3596</v>
@@ -33016,7 +33027,7 @@
     </row>
     <row r="967" spans="1:68">
       <c r="A967" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B967" s="5">
         <v>29751.6018</v>
@@ -33043,7 +33054,7 @@
     </row>
     <row r="968" spans="1:68">
       <c r="A968" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B968" s="5">
         <v>30116.844000000001</v>
@@ -33070,7 +33081,7 @@
     </row>
     <row r="969" spans="1:68">
       <c r="A969" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B969" s="5">
         <v>30482.086200000002</v>
@@ -33097,7 +33108,7 @@
     </row>
     <row r="970" spans="1:68">
       <c r="A970" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B970" s="5">
         <v>30847.328399999999</v>
@@ -33124,7 +33135,7 @@
     </row>
     <row r="971" spans="1:68">
       <c r="A971" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B971" s="5">
         <v>31212.570599999999</v>
@@ -33151,7 +33162,7 @@
     </row>
     <row r="972" spans="1:68">
       <c r="A972" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B972" s="5">
         <v>31577.8128</v>
@@ -33178,7 +33189,7 @@
     </row>
     <row r="973" spans="1:68">
       <c r="A973" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B973" s="5">
         <v>31943.055</v>
@@ -33271,7 +33282,7 @@
     </row>
     <row r="974" spans="1:68">
       <c r="A974" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B974" s="5">
         <v>32308.297200000001</v>
@@ -33295,7 +33306,7 @@
     </row>
     <row r="975" spans="1:68">
       <c r="A975" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B975" s="5">
         <v>32673.539400000001</v>
@@ -33322,7 +33333,7 @@
     </row>
     <row r="976" spans="1:68">
       <c r="A976" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B976" s="5">
         <v>33038.781600000002</v>
@@ -33349,7 +33360,7 @@
     </row>
     <row r="977" spans="1:68">
       <c r="A977" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B977" s="5">
         <v>33404.023800000003</v>
@@ -33424,7 +33435,7 @@
     </row>
     <row r="978" spans="1:68">
       <c r="A978" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B978" s="5">
         <v>33769.266000000003</v>
@@ -33451,7 +33462,7 @@
     </row>
     <row r="979" spans="1:68">
       <c r="A979" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B979" s="5">
         <v>34134.508199999997</v>
@@ -33478,7 +33489,7 @@
     </row>
     <row r="980" spans="1:68">
       <c r="A980" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B980" s="5">
         <v>34499.750400000004</v>
@@ -33505,7 +33516,7 @@
     </row>
     <row r="981" spans="1:68">
       <c r="A981" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B981" s="5">
         <v>34864.992599999998</v>
@@ -33532,7 +33543,7 @@
     </row>
     <row r="982" spans="1:68">
       <c r="A982" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B982" s="5">
         <v>35230.234799999998</v>

</xml_diff>

<commit_message>
More work on BFG and Pinus model
</commit_message>
<xml_diff>
--- a/Prototypes/Pinus/Observed.xlsx
+++ b/Prototypes/Pinus/Observed.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\APSIMxSourceTree\Prototypes\Pinus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67908916-C8B9-4A41-B15F-B621AC2B2309}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2384AEB9-5B4E-41A4-A274-D50476ECF076}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" tabRatio="653" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -285,24 +285,6 @@
     <t>stemspha</t>
   </si>
   <si>
-    <t xml:space="preserve">Pinus.Fruit.Wt </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pinus.Leaf.Dead.Wt </t>
-  </si>
-  <si>
-    <t xml:space="preserve">WoodTotalWt </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pinus.CoarseRoot.Live.Wt </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pinus.FineRoot.Live.Wt </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pinus.BelowGround.Wt </t>
-  </si>
-  <si>
     <t>Pinus.Stem.Ht</t>
   </si>
   <si>
@@ -324,25 +306,43 @@
     <t>Pinus.Stem.WoodDensity</t>
   </si>
   <si>
-    <t xml:space="preserve">Pinus.Stem.BarkWt </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pinus.Stem.WoodWt </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pinus.Stem.Wt </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pinus.Branch.Wt </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pinus.Leaf.Wt </t>
-  </si>
-  <si>
     <t>Pinus.AboveGround.Wt</t>
   </si>
   <si>
     <t>Pinus.Aboveground.N</t>
+  </si>
+  <si>
+    <t>Pinus.Fruit.Wt</t>
+  </si>
+  <si>
+    <t>Pinus.Leaf.Wt</t>
+  </si>
+  <si>
+    <t>Pinus.Leaf.Dead.Wt</t>
+  </si>
+  <si>
+    <t>Pinus.Branch.Wt</t>
+  </si>
+  <si>
+    <t>Pinus.Stem.BarkWt</t>
+  </si>
+  <si>
+    <t>Pinus.Stem.WoodWt</t>
+  </si>
+  <si>
+    <t>Pinus.Stem.Wt</t>
+  </si>
+  <si>
+    <t>WoodTotalWt</t>
+  </si>
+  <si>
+    <t>Pinus.CoarseRoot.Live.Wt</t>
+  </si>
+  <si>
+    <t>Pinus.FineRoot.Live.Wt</t>
+  </si>
+  <si>
+    <t>Pinus.BelowGround.Wt</t>
   </si>
 </sst>
 </file>
@@ -921,10 +921,10 @@
   <dimension ref="A1:BP982"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D817" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="AG783" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="U829" sqref="U829:U853"/>
+      <selection pane="bottomRight" activeCell="AJ832" sqref="AJ832"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="12.75"/>
@@ -971,21 +971,21 @@
         <v>75</v>
       </c>
       <c r="F1" s="30" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="G1" s="30" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="H1" s="30" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="I1" s="30" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="J1" s="30" t="s">
-        <v>92</v>
-      </c>
-      <c r="K1" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>55</v>
       </c>
       <c r="L1" s="30" t="s">
@@ -998,16 +998,16 @@
         <v>91</v>
       </c>
       <c r="O1" s="30" t="s">
-        <v>78</v>
+        <v>92</v>
       </c>
       <c r="P1" s="30" t="s">
-        <v>79</v>
+        <v>93</v>
       </c>
       <c r="Q1" s="30" t="s">
-        <v>80</v>
+        <v>94</v>
       </c>
       <c r="R1" s="30" t="s">
-        <v>81</v>
+        <v>95</v>
       </c>
       <c r="S1" s="30" t="s">
         <v>3</v>
@@ -1019,9 +1019,9 @@
         <v>31</v>
       </c>
       <c r="V1" s="30" t="s">
-        <v>95</v>
-      </c>
-      <c r="W1" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="W1" s="1" t="s">
         <v>56</v>
       </c>
       <c r="X1" s="30" t="s">
@@ -1034,22 +1034,22 @@
         <v>8</v>
       </c>
       <c r="AA1" s="30" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="AB1" s="30" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="AC1" s="30" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="AD1" s="30" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="AG1" s="30" t="s">
         <v>54</v>
@@ -1061,7 +1061,7 @@
         <v>37</v>
       </c>
       <c r="AJ1" s="30" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="AK1" s="30" t="s">
         <v>74</v>

</xml_diff>

<commit_message>
More on Pinus model and Puruki site
</commit_message>
<xml_diff>
--- a/Prototypes/Pinus/Observed.xlsx
+++ b/Prototypes/Pinus/Observed.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\APSIMxSourceTree\Prototypes\Pinus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B55414AE-ABB0-48B1-86CE-214AB30939B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35DF1E46-5BF1-4887-B80A-C6D280B44B3E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" tabRatio="653" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -294,16 +294,10 @@
     <t>BarkThickness</t>
   </si>
   <si>
-    <t>VolUB</t>
-  </si>
-  <si>
     <t>Pinus.Stem.WoodDensity</t>
   </si>
   <si>
     <t>Pinus.AboveGround.Wt</t>
-  </si>
-  <si>
-    <t>Pinus.Aboveground.N</t>
   </si>
   <si>
     <t>Pinus.Fruit.Wt</t>
@@ -343,6 +337,12 @@
   </si>
   <si>
     <t>PurukiSInviolate</t>
+  </si>
+  <si>
+    <t>Pinus.Stem.Volub</t>
+  </si>
+  <si>
+    <t>Pinus.AboveGround.N</t>
   </si>
 </sst>
 </file>
@@ -420,7 +420,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -445,6 +445,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -461,7 +467,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -531,6 +537,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="0.0" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -913,10 +922,10 @@
   <dimension ref="A1:BP982"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D809" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="U2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A829" sqref="A829"/>
+      <selection pane="bottomRight" activeCell="W1" sqref="W1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="12.75"/>
@@ -963,43 +972,43 @@
         <v>73</v>
       </c>
       <c r="F1" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="G1" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="G1" s="29" t="s">
+      <c r="H1" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="I1" s="29" t="s">
         <v>83</v>
       </c>
-      <c r="H1" s="29" t="s">
+      <c r="J1" s="29" t="s">
         <v>84</v>
-      </c>
-      <c r="I1" s="29" t="s">
-        <v>85</v>
-      </c>
-      <c r="J1" s="29" t="s">
-        <v>86</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>53</v>
       </c>
       <c r="L1" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="M1" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="N1" s="29" t="s">
         <v>87</v>
       </c>
-      <c r="M1" s="29" t="s">
+      <c r="O1" s="29" t="s">
         <v>88</v>
       </c>
-      <c r="N1" s="29" t="s">
+      <c r="P1" s="29" t="s">
         <v>89</v>
       </c>
-      <c r="O1" s="29" t="s">
+      <c r="Q1" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="P1" s="29" t="s">
+      <c r="R1" s="29" t="s">
         <v>91</v>
-      </c>
-      <c r="Q1" s="29" t="s">
-        <v>92</v>
-      </c>
-      <c r="R1" s="29" t="s">
-        <v>93</v>
       </c>
       <c r="S1" s="29" t="s">
         <v>3</v>
@@ -1011,7 +1020,7 @@
         <v>30</v>
       </c>
       <c r="V1" s="29" t="s">
-        <v>82</v>
+        <v>95</v>
       </c>
       <c r="W1" s="1" t="s">
         <v>54</v>
@@ -1041,7 +1050,7 @@
         <v>78</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>79</v>
+        <v>94</v>
       </c>
       <c r="AG1" s="29" t="s">
         <v>52</v>
@@ -1053,7 +1062,7 @@
         <v>36</v>
       </c>
       <c r="AJ1" s="29" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AK1" s="29" t="s">
         <v>72</v>
@@ -27873,7 +27882,7 @@
     </row>
     <row r="828" spans="1:46">
       <c r="A828" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B828" s="16">
         <v>26860</v>
@@ -27933,7 +27942,7 @@
     </row>
     <row r="829" spans="1:46">
       <c r="A829" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B829" s="5">
         <v>27590.484400000001</v>
@@ -27948,16 +27957,24 @@
       <c r="E829" s="2">
         <v>1970</v>
       </c>
-      <c r="F829" s="6"/>
-      <c r="G829" s="6"/>
+      <c r="F829" s="6">
+        <f>G829+H829+J829+N829</f>
+        <v>210</v>
+      </c>
+      <c r="G829" s="6">
+        <v>0</v>
+      </c>
       <c r="H829" s="37">
         <v>90</v>
       </c>
       <c r="I829" s="38"/>
       <c r="J829" s="37">
-        <v>90</v>
-      </c>
-      <c r="K829" s="37"/>
+        <v>50</v>
+      </c>
+      <c r="K829" s="37">
+        <f>J829+G829</f>
+        <v>50</v>
+      </c>
       <c r="L829" s="37">
         <v>20</v>
       </c>
@@ -27967,12 +27984,17 @@
       <c r="N829" s="38">
         <v>70</v>
       </c>
-      <c r="O829" s="38"/>
+      <c r="O829" s="38">
+        <f>N829+J829</f>
+        <v>120</v>
+      </c>
       <c r="P829" s="38"/>
       <c r="Q829" s="38"/>
       <c r="R829" s="38"/>
       <c r="S829" s="38"/>
-      <c r="T829" s="37"/>
+      <c r="T829" s="39">
+        <v>0.57295779513082323</v>
+      </c>
       <c r="U829" s="37"/>
       <c r="V829" s="37">
         <v>2.3860000000000001</v>
@@ -27984,13 +28006,15 @@
       <c r="AA829" s="2">
         <v>1.6</v>
       </c>
-      <c r="AB829" s="6"/>
+      <c r="AB829" s="6">
+        <v>1.3452442528293005</v>
+      </c>
       <c r="AC829" s="2">
         <v>0.28000000000000003</v>
       </c>
       <c r="AD829" s="2"/>
       <c r="AE829" s="2"/>
-      <c r="AF829" s="2"/>
+      <c r="AF829" s="40"/>
       <c r="AG829" s="2"/>
       <c r="AH829" s="2"/>
       <c r="AI829" s="2"/>
@@ -28012,7 +28036,7 @@
     </row>
     <row r="830" spans="1:46">
       <c r="A830" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B830" s="5">
         <v>27955.726600000002</v>
@@ -28027,16 +28051,24 @@
       <c r="E830" s="2">
         <v>1960</v>
       </c>
-      <c r="F830" s="6"/>
-      <c r="G830" s="6"/>
+      <c r="F830" s="6">
+        <f t="shared" ref="F830:F841" si="8">G830+H830+J830+N830</f>
+        <v>700</v>
+      </c>
+      <c r="G830" s="6">
+        <v>0</v>
+      </c>
       <c r="H830" s="37">
         <v>240</v>
       </c>
       <c r="I830" s="38"/>
       <c r="J830" s="37">
-        <v>240</v>
-      </c>
-      <c r="K830" s="37"/>
+        <v>170.00000000000003</v>
+      </c>
+      <c r="K830" s="37">
+        <f t="shared" ref="K830:K841" si="9">J830+G830</f>
+        <v>170.00000000000003</v>
+      </c>
       <c r="L830" s="37">
         <v>40</v>
       </c>
@@ -28046,12 +28078,17 @@
       <c r="N830" s="38">
         <v>290</v>
       </c>
-      <c r="O830" s="38"/>
+      <c r="O830" s="38">
+        <f t="shared" ref="O830:O841" si="10">N830+J830</f>
+        <v>460</v>
+      </c>
       <c r="P830" s="38"/>
       <c r="Q830" s="38"/>
       <c r="R830" s="38"/>
       <c r="S830" s="38"/>
-      <c r="T830" s="37"/>
+      <c r="T830" s="39">
+        <v>1.3369015219719209</v>
+      </c>
       <c r="U830" s="37"/>
       <c r="V830" s="37">
         <v>5.777000000000001</v>
@@ -28063,13 +28100,15 @@
       <c r="AA830" s="2">
         <v>2.6</v>
       </c>
-      <c r="AB830" s="6"/>
+      <c r="AB830" s="6">
+        <v>3.7975516930514694</v>
+      </c>
       <c r="AC830" s="2">
         <v>2.2200000000000002</v>
       </c>
       <c r="AD830" s="2"/>
       <c r="AE830" s="2"/>
-      <c r="AF830" s="2"/>
+      <c r="AF830" s="40"/>
       <c r="AG830" s="2"/>
       <c r="AH830" s="2"/>
       <c r="AI830" s="2"/>
@@ -28091,7 +28130,7 @@
     </row>
     <row r="831" spans="1:46">
       <c r="A831" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B831" s="5">
         <v>28320.968799999999</v>
@@ -28106,16 +28145,24 @@
       <c r="E831" s="2">
         <v>1960</v>
       </c>
-      <c r="F831" s="6"/>
-      <c r="G831" s="6"/>
+      <c r="F831" s="6">
+        <f t="shared" si="8"/>
+        <v>2360</v>
+      </c>
+      <c r="G831" s="6">
+        <v>0</v>
+      </c>
       <c r="H831" s="37">
         <v>800</v>
       </c>
       <c r="I831" s="38"/>
       <c r="J831" s="37">
-        <v>800</v>
-      </c>
-      <c r="K831" s="37"/>
+        <v>700</v>
+      </c>
+      <c r="K831" s="37">
+        <f t="shared" si="9"/>
+        <v>700</v>
+      </c>
       <c r="L831" s="37">
         <v>130</v>
       </c>
@@ -28125,12 +28172,17 @@
       <c r="N831" s="38">
         <v>860</v>
       </c>
-      <c r="O831" s="38"/>
+      <c r="O831" s="38">
+        <f t="shared" si="10"/>
+        <v>1560</v>
+      </c>
       <c r="P831" s="38"/>
       <c r="Q831" s="38"/>
       <c r="R831" s="38"/>
       <c r="S831" s="38"/>
-      <c r="T831" s="37"/>
+      <c r="T831" s="39">
+        <v>4.45633840657307</v>
+      </c>
       <c r="U831" s="37"/>
       <c r="V831" s="37">
         <v>17.087</v>
@@ -28142,13 +28194,15 @@
       <c r="AA831" s="2">
         <v>3.8</v>
       </c>
-      <c r="AB831" s="6"/>
+      <c r="AB831" s="6">
+        <v>6.6316491464530074</v>
+      </c>
       <c r="AC831" s="2">
         <v>6.77</v>
       </c>
       <c r="AD831" s="2"/>
       <c r="AE831" s="2"/>
-      <c r="AF831" s="2"/>
+      <c r="AF831" s="40"/>
       <c r="AG831" s="2"/>
       <c r="AH831" s="2"/>
       <c r="AI831" s="2"/>
@@ -28170,7 +28224,7 @@
     </row>
     <row r="832" spans="1:46">
       <c r="A832" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B832" s="5">
         <v>28686.210999999999</v>
@@ -28185,16 +28239,24 @@
       <c r="E832" s="2">
         <v>1950</v>
       </c>
-      <c r="F832" s="6"/>
-      <c r="G832" s="6"/>
+      <c r="F832" s="6">
+        <f t="shared" si="8"/>
+        <v>4380</v>
+      </c>
+      <c r="G832" s="6">
+        <v>10</v>
+      </c>
       <c r="H832" s="37">
         <v>1250</v>
       </c>
       <c r="I832" s="38"/>
       <c r="J832" s="37">
-        <v>1250</v>
-      </c>
-      <c r="K832" s="37"/>
+        <v>1410</v>
+      </c>
+      <c r="K832" s="37">
+        <f t="shared" si="9"/>
+        <v>1420</v>
+      </c>
       <c r="L832" s="37">
         <v>200</v>
       </c>
@@ -28204,12 +28266,17 @@
       <c r="N832" s="38">
         <v>1710.0000000000002</v>
       </c>
-      <c r="O832" s="38"/>
+      <c r="O832" s="38">
+        <f t="shared" si="10"/>
+        <v>3120</v>
+      </c>
       <c r="P832" s="38"/>
       <c r="Q832" s="38"/>
       <c r="R832" s="38"/>
       <c r="S832" s="38"/>
-      <c r="T832" s="37"/>
+      <c r="T832" s="39">
+        <v>6.3980287122941935</v>
+      </c>
       <c r="U832" s="37"/>
       <c r="V832" s="37">
         <v>28.094999999999999</v>
@@ -28221,15 +28288,17 @@
       <c r="AA832" s="2">
         <v>5.7</v>
       </c>
-      <c r="AB832" s="6"/>
+      <c r="AB832" s="6">
+        <v>10.157024044040933</v>
+      </c>
       <c r="AC832" s="2">
         <v>15.8</v>
       </c>
-      <c r="AD832" s="2">
+      <c r="AD832" s="2"/>
+      <c r="AE832" s="2"/>
+      <c r="AF832" s="41">
         <v>47.7</v>
       </c>
-      <c r="AE832" s="2"/>
-      <c r="AF832" s="2"/>
       <c r="AG832" s="2"/>
       <c r="AH832" s="2"/>
       <c r="AI832" s="2"/>
@@ -28253,7 +28322,7 @@
     </row>
     <row r="833" spans="1:46">
       <c r="A833" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B833" s="5">
         <v>29047.800778000001</v>
@@ -28268,16 +28337,24 @@
       <c r="E833" s="2">
         <v>1950</v>
       </c>
-      <c r="F833" s="6"/>
-      <c r="G833" s="6"/>
+      <c r="F833" s="6">
+        <f t="shared" si="8"/>
+        <v>6860</v>
+      </c>
+      <c r="G833" s="6">
+        <v>0</v>
+      </c>
       <c r="H833" s="37">
         <v>1889.9999999999998</v>
       </c>
       <c r="I833" s="38"/>
       <c r="J833" s="37">
-        <v>1889.9999999999998</v>
-      </c>
-      <c r="K833" s="37"/>
+        <v>2150</v>
+      </c>
+      <c r="K833" s="37">
+        <f t="shared" si="9"/>
+        <v>2150</v>
+      </c>
       <c r="L833" s="37">
         <v>380</v>
       </c>
@@ -28287,12 +28364,17 @@
       <c r="N833" s="38">
         <v>2820</v>
       </c>
-      <c r="O833" s="38"/>
+      <c r="O833" s="38">
+        <f t="shared" si="10"/>
+        <v>4970</v>
+      </c>
       <c r="P833" s="38"/>
       <c r="Q833" s="38"/>
       <c r="R833" s="38"/>
       <c r="S833" s="38"/>
-      <c r="T833" s="37"/>
+      <c r="T833" s="39">
+        <v>9.899437460315891</v>
+      </c>
       <c r="U833" s="37"/>
       <c r="V833" s="37">
         <v>36.758000000000003</v>
@@ -28304,15 +28386,17 @@
       <c r="AA833" s="2">
         <v>8.4</v>
       </c>
-      <c r="AB833" s="6"/>
+      <c r="AB833" s="6">
+        <v>12.570299347501685</v>
+      </c>
       <c r="AC833" s="2">
         <v>24.2</v>
       </c>
-      <c r="AD833" s="2">
+      <c r="AD833" s="2"/>
+      <c r="AE833" s="2"/>
+      <c r="AF833" s="41">
         <v>84.3</v>
       </c>
-      <c r="AE833" s="2"/>
-      <c r="AF833" s="2"/>
       <c r="AG833" s="2"/>
       <c r="AH833" s="2"/>
       <c r="AI833" s="2"/>
@@ -28336,7 +28420,7 @@
     </row>
     <row r="834" spans="1:46">
       <c r="A834" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B834" s="5">
         <v>29051.4532</v>
@@ -28351,16 +28435,24 @@
       <c r="E834" s="2">
         <v>495</v>
       </c>
-      <c r="F834" s="6"/>
-      <c r="G834" s="6"/>
+      <c r="F834" s="6">
+        <f t="shared" si="8"/>
+        <v>1810</v>
+      </c>
+      <c r="G834" s="6">
+        <v>0</v>
+      </c>
       <c r="H834" s="37">
         <v>360</v>
       </c>
       <c r="I834" s="38"/>
       <c r="J834" s="37">
-        <v>360</v>
-      </c>
-      <c r="K834" s="37"/>
+        <v>459.99999999999994</v>
+      </c>
+      <c r="K834" s="37">
+        <f t="shared" si="9"/>
+        <v>459.99999999999994</v>
+      </c>
       <c r="L834" s="37">
         <v>130</v>
       </c>
@@ -28370,12 +28462,17 @@
       <c r="N834" s="38">
         <v>990</v>
       </c>
-      <c r="O834" s="38"/>
+      <c r="O834" s="38">
+        <f t="shared" si="10"/>
+        <v>1450</v>
+      </c>
       <c r="P834" s="38"/>
       <c r="Q834" s="38"/>
       <c r="R834" s="38"/>
       <c r="S834" s="38"/>
-      <c r="T834" s="37"/>
+      <c r="T834" s="39">
+        <v>2.1645072260497766</v>
+      </c>
       <c r="U834" s="37"/>
       <c r="V834" s="37">
         <v>8.995000000000001</v>
@@ -28387,15 +28484,17 @@
       <c r="AA834" s="2">
         <v>8.4</v>
       </c>
-      <c r="AB834" s="6"/>
+      <c r="AB834" s="6">
+        <v>14.838483756073707</v>
+      </c>
       <c r="AC834" s="2">
         <v>8.56</v>
       </c>
-      <c r="AD834" s="2">
+      <c r="AD834" s="2"/>
+      <c r="AE834" s="2"/>
+      <c r="AF834" s="41">
         <v>29.8</v>
       </c>
-      <c r="AE834" s="2"/>
-      <c r="AF834" s="2"/>
       <c r="AG834" s="2"/>
       <c r="AH834" s="2"/>
       <c r="AI834" s="2"/>
@@ -28419,7 +28518,7 @@
     </row>
     <row r="835" spans="1:46">
       <c r="A835" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B835" s="5">
         <v>29416.695400000001</v>
@@ -28434,16 +28533,24 @@
       <c r="E835" s="2">
         <v>495</v>
       </c>
-      <c r="F835" s="6"/>
-      <c r="G835" s="6"/>
+      <c r="F835" s="6">
+        <f t="shared" si="8"/>
+        <v>3120</v>
+      </c>
+      <c r="G835" s="6">
+        <v>10</v>
+      </c>
       <c r="H835" s="37">
         <v>480</v>
       </c>
       <c r="I835" s="38"/>
       <c r="J835" s="37">
-        <v>480</v>
-      </c>
-      <c r="K835" s="37"/>
+        <v>800</v>
+      </c>
+      <c r="K835" s="37">
+        <f t="shared" si="9"/>
+        <v>810</v>
+      </c>
       <c r="L835" s="37">
         <v>200</v>
       </c>
@@ -28453,12 +28560,17 @@
       <c r="N835" s="38">
         <v>1830</v>
       </c>
-      <c r="O835" s="38"/>
+      <c r="O835" s="38">
+        <f t="shared" si="10"/>
+        <v>2630</v>
+      </c>
       <c r="P835" s="38"/>
       <c r="Q835" s="38"/>
       <c r="R835" s="38"/>
       <c r="S835" s="38"/>
-      <c r="T835" s="37"/>
+      <c r="T835" s="39">
+        <v>2.5783100780887045</v>
+      </c>
       <c r="U835" s="37"/>
       <c r="V835" s="37">
         <v>15.559000000000001</v>
@@ -28470,15 +28582,17 @@
       <c r="AA835" s="2">
         <v>9.6</v>
       </c>
-      <c r="AB835" s="6"/>
+      <c r="AB835" s="6">
+        <v>18.426362420514121</v>
+      </c>
       <c r="AC835" s="2">
         <v>13.2</v>
       </c>
-      <c r="AD835" s="2">
+      <c r="AD835" s="2"/>
+      <c r="AE835" s="2"/>
+      <c r="AF835" s="41">
         <v>55.1</v>
       </c>
-      <c r="AE835" s="2"/>
-      <c r="AF835" s="2"/>
       <c r="AG835" s="2"/>
       <c r="AH835" s="2"/>
       <c r="AI835" s="2"/>
@@ -28502,7 +28616,7 @@
     </row>
     <row r="836" spans="1:46">
       <c r="A836" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B836" s="5">
         <v>29781.937600000001</v>
@@ -28517,16 +28631,24 @@
       <c r="E836" s="2">
         <v>495</v>
       </c>
-      <c r="F836" s="6"/>
-      <c r="G836" s="6"/>
+      <c r="F836" s="6">
+        <f t="shared" si="8"/>
+        <v>5560</v>
+      </c>
+      <c r="G836" s="6">
+        <v>0</v>
+      </c>
       <c r="H836" s="37">
         <v>860</v>
       </c>
       <c r="I836" s="38"/>
       <c r="J836" s="37">
-        <v>860</v>
-      </c>
-      <c r="K836" s="37"/>
+        <v>1480</v>
+      </c>
+      <c r="K836" s="37">
+        <f t="shared" si="9"/>
+        <v>1480</v>
+      </c>
       <c r="L836" s="37">
         <v>340</v>
       </c>
@@ -28536,12 +28658,17 @@
       <c r="N836" s="38">
         <v>3220.0000000000005</v>
       </c>
-      <c r="O836" s="38"/>
+      <c r="O836" s="38">
+        <f t="shared" si="10"/>
+        <v>4700</v>
+      </c>
       <c r="P836" s="38"/>
       <c r="Q836" s="38"/>
       <c r="R836" s="38"/>
       <c r="S836" s="38"/>
-      <c r="T836" s="37"/>
+      <c r="T836" s="39">
+        <v>4.5836623610465859</v>
+      </c>
       <c r="U836" s="37"/>
       <c r="V836" s="37">
         <v>23.824000000000002</v>
@@ -28553,15 +28680,17 @@
       <c r="AA836" s="2">
         <v>11.3</v>
       </c>
-      <c r="AB836" s="6"/>
+      <c r="AB836" s="6">
+        <v>22.22302923634555</v>
+      </c>
       <c r="AC836" s="2">
         <v>19.2</v>
       </c>
-      <c r="AD836" s="2">
+      <c r="AD836" s="2"/>
+      <c r="AE836" s="2"/>
+      <c r="AF836" s="41">
         <v>93.9</v>
       </c>
-      <c r="AE836" s="2"/>
-      <c r="AF836" s="2"/>
       <c r="AG836" s="2"/>
       <c r="AH836" s="2"/>
       <c r="AI836" s="2"/>
@@ -28585,7 +28714,7 @@
     </row>
     <row r="837" spans="1:46">
       <c r="A837" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B837" s="5">
         <v>30147.179800000002</v>
@@ -28600,16 +28729,24 @@
       <c r="E837" s="2">
         <v>495</v>
       </c>
-      <c r="F837" s="6"/>
-      <c r="G837" s="6"/>
+      <c r="F837" s="6">
+        <f t="shared" si="8"/>
+        <v>8430</v>
+      </c>
+      <c r="G837" s="6">
+        <v>50</v>
+      </c>
       <c r="H837" s="37">
         <v>1170</v>
       </c>
       <c r="I837" s="38"/>
       <c r="J837" s="37">
-        <v>1170</v>
-      </c>
-      <c r="K837" s="37"/>
+        <v>2150</v>
+      </c>
+      <c r="K837" s="37">
+        <f t="shared" si="9"/>
+        <v>2200</v>
+      </c>
       <c r="L837" s="37">
         <v>500</v>
       </c>
@@ -28619,12 +28756,17 @@
       <c r="N837" s="38">
         <v>5060</v>
       </c>
-      <c r="O837" s="38"/>
+      <c r="O837" s="38">
+        <f t="shared" si="10"/>
+        <v>7210</v>
+      </c>
       <c r="P837" s="38"/>
       <c r="Q837" s="38"/>
       <c r="R837" s="38"/>
       <c r="S837" s="38"/>
-      <c r="T837" s="37"/>
+      <c r="T837" s="39">
+        <v>5.5704230082163368</v>
+      </c>
       <c r="U837" s="37"/>
       <c r="V837" s="37">
         <v>28.786000000000001</v>
@@ -28636,15 +28778,17 @@
       <c r="AA837" s="2">
         <v>13.2</v>
       </c>
-      <c r="AB837" s="6"/>
+      <c r="AB837" s="6">
+        <v>25.205836793512571</v>
+      </c>
       <c r="AC837" s="2">
         <v>24.7</v>
       </c>
-      <c r="AD837" s="2">
+      <c r="AD837" s="2"/>
+      <c r="AE837" s="2"/>
+      <c r="AF837" s="41">
         <v>132.6</v>
       </c>
-      <c r="AE837" s="2"/>
-      <c r="AF837" s="2"/>
       <c r="AG837" s="2"/>
       <c r="AH837" s="2"/>
       <c r="AI837" s="2"/>
@@ -28668,7 +28812,7 @@
     </row>
     <row r="838" spans="1:46">
       <c r="A838" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B838" s="5">
         <v>30508.769577999999</v>
@@ -28683,16 +28827,24 @@
       <c r="E838" s="2">
         <v>495</v>
       </c>
-      <c r="F838" s="6"/>
-      <c r="G838" s="6"/>
+      <c r="F838" s="6">
+        <f t="shared" si="8"/>
+        <v>10560</v>
+      </c>
+      <c r="G838" s="6">
+        <v>60</v>
+      </c>
       <c r="H838" s="37">
         <v>1140</v>
       </c>
       <c r="I838" s="38"/>
       <c r="J838" s="37">
-        <v>1140</v>
-      </c>
-      <c r="K838" s="37"/>
+        <v>3270.0000000000005</v>
+      </c>
+      <c r="K838" s="37">
+        <f t="shared" si="9"/>
+        <v>3330.0000000000005</v>
+      </c>
       <c r="L838" s="37">
         <v>610</v>
       </c>
@@ -28702,12 +28854,17 @@
       <c r="N838" s="38">
         <v>6090</v>
       </c>
-      <c r="O838" s="38"/>
+      <c r="O838" s="38">
+        <f t="shared" si="10"/>
+        <v>9360</v>
+      </c>
       <c r="P838" s="38"/>
       <c r="Q838" s="38"/>
       <c r="R838" s="38"/>
       <c r="S838" s="38"/>
-      <c r="T838" s="37"/>
+      <c r="T838" s="39">
+        <v>5.79323992854499</v>
+      </c>
       <c r="U838" s="37"/>
       <c r="V838" s="37">
         <v>32.752000000000002</v>
@@ -28719,15 +28876,17 @@
       <c r="AA838" s="2">
         <v>15.4</v>
       </c>
-      <c r="AB838" s="6"/>
+      <c r="AB838" s="6">
+        <v>27.871228686279956</v>
+      </c>
       <c r="AC838" s="2">
         <v>30.2</v>
       </c>
-      <c r="AD838" s="2">
+      <c r="AD838" s="2"/>
+      <c r="AE838" s="2"/>
+      <c r="AF838" s="41">
         <v>160.1</v>
       </c>
-      <c r="AE838" s="2"/>
-      <c r="AF838" s="2"/>
       <c r="AG838" s="2"/>
       <c r="AH838" s="2"/>
       <c r="AI838" s="2"/>
@@ -28751,7 +28910,7 @@
     </row>
     <row r="839" spans="1:46">
       <c r="A839" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B839" s="5">
         <v>30512.421999999999</v>
@@ -28766,16 +28925,24 @@
       <c r="E839" s="2">
         <v>159</v>
       </c>
-      <c r="F839" s="6"/>
-      <c r="G839" s="6"/>
+      <c r="F839" s="6">
+        <f t="shared" si="8"/>
+        <v>3510</v>
+      </c>
+      <c r="G839" s="6">
+        <v>20</v>
+      </c>
       <c r="H839" s="37">
         <v>380</v>
       </c>
       <c r="I839" s="38"/>
       <c r="J839" s="37">
-        <v>380</v>
-      </c>
-      <c r="K839" s="37"/>
+        <v>1090</v>
+      </c>
+      <c r="K839" s="37">
+        <f t="shared" si="9"/>
+        <v>1110</v>
+      </c>
       <c r="L839" s="37">
         <v>200</v>
       </c>
@@ -28785,12 +28952,17 @@
       <c r="N839" s="38">
         <v>2020</v>
       </c>
-      <c r="O839" s="38"/>
+      <c r="O839" s="38">
+        <f t="shared" si="10"/>
+        <v>3110</v>
+      </c>
       <c r="P839" s="38"/>
       <c r="Q839" s="38"/>
       <c r="R839" s="38"/>
       <c r="S839" s="38"/>
-      <c r="T839" s="37"/>
+      <c r="T839" s="39">
+        <v>1.941690305721123</v>
+      </c>
       <c r="U839" s="37"/>
       <c r="V839" s="37">
         <v>10.88</v>
@@ -28802,15 +28974,17 @@
       <c r="AA839" s="2">
         <v>15.4</v>
       </c>
-      <c r="AB839" s="6"/>
+      <c r="AB839" s="6">
+        <v>28.298061139836122</v>
+      </c>
       <c r="AC839" s="2">
         <v>10</v>
       </c>
-      <c r="AD839" s="2">
+      <c r="AD839" s="2"/>
+      <c r="AE839" s="2"/>
+      <c r="AF839" s="41">
         <v>53.2</v>
       </c>
-      <c r="AE839" s="2"/>
-      <c r="AF839" s="2"/>
       <c r="AG839" s="2"/>
       <c r="AH839" s="2"/>
       <c r="AI839" s="2"/>
@@ -28834,7 +29008,7 @@
     </row>
     <row r="840" spans="1:46">
       <c r="A840" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B840" s="5">
         <v>30877.664199999999</v>
@@ -28849,16 +29023,24 @@
       <c r="E840" s="2">
         <v>156</v>
       </c>
-      <c r="F840" s="6"/>
-      <c r="G840" s="6"/>
+      <c r="F840" s="6">
+        <f t="shared" si="8"/>
+        <v>5340</v>
+      </c>
+      <c r="G840" s="6">
+        <v>50</v>
+      </c>
       <c r="H840" s="37">
         <v>440.00000000000006</v>
       </c>
       <c r="I840" s="38"/>
       <c r="J840" s="37">
-        <v>440.00000000000006</v>
-      </c>
-      <c r="K840" s="37"/>
+        <v>1520</v>
+      </c>
+      <c r="K840" s="37">
+        <f t="shared" si="9"/>
+        <v>1570</v>
+      </c>
       <c r="L840" s="37">
         <v>300</v>
       </c>
@@ -28868,12 +29050,17 @@
       <c r="N840" s="38">
         <v>3329.9999999999995</v>
       </c>
-      <c r="O840" s="38"/>
+      <c r="O840" s="38">
+        <f t="shared" si="10"/>
+        <v>4850</v>
+      </c>
       <c r="P840" s="38"/>
       <c r="Q840" s="38"/>
       <c r="R840" s="38"/>
       <c r="S840" s="38"/>
-      <c r="T840" s="37"/>
+      <c r="T840" s="39">
+        <v>1.9735212943395024</v>
+      </c>
       <c r="U840" s="37"/>
       <c r="V840" s="37">
         <v>16.393000000000001</v>
@@ -28885,15 +29072,17 @@
       <c r="AA840" s="2">
         <v>17.399999999999999</v>
       </c>
-      <c r="AB840" s="6"/>
+      <c r="AB840" s="6">
+        <v>32.573514550366255</v>
+      </c>
       <c r="AC840" s="2">
         <v>13</v>
       </c>
-      <c r="AD840" s="2">
+      <c r="AD840" s="2"/>
+      <c r="AE840" s="2"/>
+      <c r="AF840" s="41">
         <v>86.7</v>
       </c>
-      <c r="AE840" s="2"/>
-      <c r="AF840" s="2"/>
       <c r="AG840" s="2"/>
       <c r="AH840" s="2"/>
       <c r="AI840" s="2"/>
@@ -28917,7 +29106,7 @@
     </row>
     <row r="841" spans="1:46">
       <c r="A841" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B841" s="5">
         <v>31242.9064</v>
@@ -28932,16 +29121,24 @@
       <c r="E841" s="2">
         <v>156</v>
       </c>
-      <c r="F841" s="6"/>
-      <c r="G841" s="6"/>
+      <c r="F841" s="6">
+        <f t="shared" si="8"/>
+        <v>7200</v>
+      </c>
+      <c r="G841" s="6">
+        <v>80</v>
+      </c>
       <c r="H841" s="37">
         <v>700</v>
       </c>
       <c r="I841" s="38"/>
       <c r="J841" s="37">
-        <v>700</v>
-      </c>
-      <c r="K841" s="37"/>
+        <v>1940.0000000000002</v>
+      </c>
+      <c r="K841" s="37">
+        <f t="shared" si="9"/>
+        <v>2020.0000000000002</v>
+      </c>
       <c r="L841" s="37">
         <v>450</v>
       </c>
@@ -28951,12 +29148,17 @@
       <c r="N841" s="38">
         <v>4480</v>
       </c>
-      <c r="O841" s="38"/>
+      <c r="O841" s="38">
+        <f t="shared" si="10"/>
+        <v>6420</v>
+      </c>
       <c r="P841" s="38"/>
       <c r="Q841" s="38"/>
       <c r="R841" s="38"/>
       <c r="S841" s="38"/>
-      <c r="T841" s="37"/>
+      <c r="T841" s="39">
+        <v>3.3740847935481812</v>
+      </c>
       <c r="U841" s="37"/>
       <c r="V841" s="37">
         <v>21.397000000000002</v>
@@ -28968,15 +29170,17 @@
       <c r="AA841" s="2">
         <v>19.3</v>
       </c>
-      <c r="AB841" s="6"/>
+      <c r="AB841" s="6">
+        <v>36.585994738079251</v>
+      </c>
       <c r="AC841" s="2">
         <v>16.399999999999999</v>
       </c>
-      <c r="AD841" s="2">
+      <c r="AD841" s="2"/>
+      <c r="AE841" s="2"/>
+      <c r="AF841" s="41">
         <v>111.6</v>
       </c>
-      <c r="AE841" s="2"/>
-      <c r="AF841" s="2"/>
       <c r="AG841" s="2"/>
       <c r="AH841" s="2"/>
       <c r="AI841" s="2"/>
@@ -29000,7 +29204,7 @@
     </row>
     <row r="842" spans="1:46">
       <c r="A842" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B842" s="16">
         <v>26860</v>
@@ -29015,10 +29219,9 @@
         <v>2220</v>
       </c>
       <c r="F842" s="6"/>
-      <c r="G842" s="6"/>
       <c r="H842" s="38"/>
       <c r="I842" s="38"/>
-      <c r="J842" s="38"/>
+      <c r="J842" s="37"/>
       <c r="K842" s="38"/>
       <c r="L842" s="38"/>
       <c r="M842" s="38"/>
@@ -29028,7 +29231,6 @@
       <c r="Q842" s="38"/>
       <c r="R842" s="38"/>
       <c r="S842" s="38"/>
-      <c r="T842" s="38"/>
       <c r="U842" s="37"/>
       <c r="V842" s="38"/>
       <c r="W842" s="38"/>
@@ -29060,7 +29262,7 @@
     </row>
     <row r="843" spans="1:46">
       <c r="A843" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B843" s="5">
         <v>27590.484400000001</v>
@@ -29069,14 +29271,13 @@
         <v>2</v>
       </c>
       <c r="D843" s="6">
-        <f t="shared" ref="D843:D853" si="8">E843*100/2220</f>
+        <f t="shared" ref="D843:D853" si="11">E843*100/2220</f>
         <v>88.963963963963963</v>
       </c>
       <c r="E843" s="2">
         <v>1975</v>
       </c>
       <c r="F843" s="6"/>
-      <c r="G843" s="6"/>
       <c r="H843" s="38"/>
       <c r="I843" s="38"/>
       <c r="J843" s="38"/>
@@ -29099,7 +29300,9 @@
       <c r="AA843" s="2">
         <v>1.8</v>
       </c>
-      <c r="AB843" s="6"/>
+      <c r="AB843" s="6">
+        <v>1.9169426521686781</v>
+      </c>
       <c r="AC843" s="2">
         <v>0.56999999999999995</v>
       </c>
@@ -29125,7 +29328,7 @@
     </row>
     <row r="844" spans="1:46">
       <c r="A844" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B844" s="5">
         <v>27955.726600000002</v>
@@ -29134,14 +29337,13 @@
         <v>3</v>
       </c>
       <c r="D844" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>87.162162162162161</v>
       </c>
       <c r="E844" s="2">
         <v>1935</v>
       </c>
       <c r="F844" s="6"/>
-      <c r="G844" s="6"/>
       <c r="H844" s="38"/>
       <c r="I844" s="38"/>
       <c r="J844" s="38"/>
@@ -29164,7 +29366,9 @@
       <c r="AA844" s="2">
         <v>2.9</v>
       </c>
-      <c r="AB844" s="6"/>
+      <c r="AB844" s="6">
+        <v>4.7714767002648442</v>
+      </c>
       <c r="AC844" s="2">
         <v>3.46</v>
       </c>
@@ -29190,7 +29394,7 @@
     </row>
     <row r="845" spans="1:46">
       <c r="A845" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B845" s="5">
         <v>28320.968799999999</v>
@@ -29199,14 +29403,13 @@
         <v>4</v>
       </c>
       <c r="D845" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>86.936936936936931</v>
       </c>
       <c r="E845" s="2">
         <v>1930</v>
       </c>
       <c r="F845" s="6"/>
-      <c r="G845" s="6"/>
       <c r="H845" s="38"/>
       <c r="I845" s="38"/>
       <c r="J845" s="38"/>
@@ -29229,7 +29432,9 @@
       <c r="AA845" s="2">
         <v>4.3</v>
       </c>
-      <c r="AB845" s="6"/>
+      <c r="AB845" s="6">
+        <v>8.0488221679828911</v>
+      </c>
       <c r="AC845" s="2">
         <v>9.82</v>
       </c>
@@ -29255,7 +29460,7 @@
     </row>
     <row r="846" spans="1:46">
       <c r="A846" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B846" s="5">
         <v>28686.210999999999</v>
@@ -29264,14 +29469,13 @@
         <v>5</v>
       </c>
       <c r="D846" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>86.936936936936931</v>
       </c>
       <c r="E846" s="2">
         <v>1930</v>
       </c>
       <c r="F846" s="6"/>
-      <c r="G846" s="6"/>
       <c r="H846" s="38"/>
       <c r="I846" s="38"/>
       <c r="J846" s="38"/>
@@ -29294,15 +29498,16 @@
       <c r="AA846" s="2">
         <v>6.3</v>
       </c>
-      <c r="AB846" s="6"/>
+      <c r="AB846" s="6">
+        <v>11.543892476660128</v>
+      </c>
       <c r="AC846" s="2">
         <v>20.2</v>
       </c>
-      <c r="AD846" s="2">
+      <c r="AE846" s="2"/>
+      <c r="AF846" s="2">
         <v>69.5</v>
       </c>
-      <c r="AE846" s="2"/>
-      <c r="AF846" s="2"/>
       <c r="AG846" s="2"/>
       <c r="AH846" s="2"/>
       <c r="AI846" s="2"/>
@@ -29322,7 +29527,7 @@
     </row>
     <row r="847" spans="1:46">
       <c r="A847" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B847" s="5">
         <v>29051.4532</v>
@@ -29331,14 +29536,13 @@
         <v>6</v>
       </c>
       <c r="D847" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>86.036036036036037</v>
       </c>
       <c r="E847" s="2">
         <v>1910</v>
       </c>
       <c r="F847" s="6"/>
-      <c r="G847" s="6"/>
       <c r="H847" s="38"/>
       <c r="I847" s="38"/>
       <c r="J847" s="38"/>
@@ -29361,15 +29565,16 @@
       <c r="AA847" s="2">
         <v>8.3000000000000007</v>
       </c>
-      <c r="AB847" s="6"/>
+      <c r="AB847" s="6">
+        <v>13.975661374215719</v>
+      </c>
       <c r="AC847" s="2">
         <v>29.3</v>
       </c>
-      <c r="AD847" s="2">
+      <c r="AE847" s="2"/>
+      <c r="AF847" s="2">
         <v>119.6</v>
       </c>
-      <c r="AE847" s="2"/>
-      <c r="AF847" s="2"/>
       <c r="AG847" s="2"/>
       <c r="AH847" s="2"/>
       <c r="AI847" s="2"/>
@@ -29389,7 +29594,7 @@
     </row>
     <row r="848" spans="1:46">
       <c r="A848" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B848" s="5">
         <v>29416.695400000001</v>
@@ -29398,14 +29603,13 @@
         <v>7</v>
       </c>
       <c r="D848" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>85.810810810810807</v>
       </c>
       <c r="E848" s="2">
         <v>1905</v>
       </c>
       <c r="F848" s="6"/>
-      <c r="G848" s="6"/>
       <c r="H848" s="38"/>
       <c r="I848" s="38"/>
       <c r="J848" s="38"/>
@@ -29428,15 +29632,16 @@
       <c r="AA848" s="2">
         <v>9.6</v>
       </c>
-      <c r="AB848" s="6"/>
+      <c r="AB848" s="6">
+        <v>15.915759123580655</v>
+      </c>
       <c r="AC848" s="2">
         <v>37.9</v>
       </c>
-      <c r="AD848" s="2">
+      <c r="AE848" s="2"/>
+      <c r="AF848" s="2">
         <v>172.5</v>
       </c>
-      <c r="AE848" s="2"/>
-      <c r="AF848" s="2"/>
       <c r="AG848" s="2"/>
       <c r="AH848" s="2"/>
       <c r="AI848" s="2"/>
@@ -29456,7 +29661,7 @@
     </row>
     <row r="849" spans="1:46">
       <c r="A849" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B849" s="5">
         <v>29781.937600000001</v>
@@ -29465,14 +29670,13 @@
         <v>8</v>
       </c>
       <c r="D849" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>84.459459459459453</v>
       </c>
       <c r="E849" s="2">
         <v>1875</v>
       </c>
       <c r="F849" s="6"/>
-      <c r="G849" s="6"/>
       <c r="H849" s="38"/>
       <c r="I849" s="38"/>
       <c r="J849" s="38"/>
@@ -29495,15 +29699,16 @@
       <c r="AA849" s="2">
         <v>10.9</v>
       </c>
-      <c r="AB849" s="6"/>
+      <c r="AB849" s="6">
+        <v>17.048119903280465</v>
+      </c>
       <c r="AC849" s="2">
         <v>42.8</v>
       </c>
-      <c r="AD849" s="2">
+      <c r="AE849" s="2"/>
+      <c r="AF849" s="2">
         <v>217.3</v>
       </c>
-      <c r="AE849" s="2"/>
-      <c r="AF849" s="2"/>
       <c r="AG849" s="2"/>
       <c r="AH849" s="2"/>
       <c r="AI849" s="2"/>
@@ -29523,7 +29728,7 @@
     </row>
     <row r="850" spans="1:46">
       <c r="A850" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B850" s="5">
         <v>30147.179800000002</v>
@@ -29532,14 +29737,13 @@
         <v>9</v>
       </c>
       <c r="D850" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>78.828828828828833</v>
       </c>
       <c r="E850" s="2">
         <v>1750</v>
       </c>
       <c r="F850" s="6"/>
-      <c r="G850" s="6"/>
       <c r="H850" s="38"/>
       <c r="I850" s="38"/>
       <c r="J850" s="38"/>
@@ -29562,15 +29766,16 @@
       <c r="AA850" s="2">
         <v>12.4</v>
       </c>
-      <c r="AB850" s="6"/>
+      <c r="AB850" s="6">
+        <v>18.353830384971328</v>
+      </c>
       <c r="AC850" s="2">
         <v>46.3</v>
       </c>
-      <c r="AD850" s="2">
+      <c r="AE850" s="2"/>
+      <c r="AF850" s="2">
         <v>259.89999999999998</v>
       </c>
-      <c r="AE850" s="2"/>
-      <c r="AF850" s="2"/>
       <c r="AG850" s="2"/>
       <c r="AH850" s="2"/>
       <c r="AI850" s="2"/>
@@ -29590,7 +29795,7 @@
     </row>
     <row r="851" spans="1:46">
       <c r="A851" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B851" s="5">
         <v>30512.421999999999</v>
@@ -29599,14 +29804,13 @@
         <v>10</v>
       </c>
       <c r="D851" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>74.099099099099092</v>
       </c>
       <c r="E851" s="2">
         <v>1645</v>
       </c>
       <c r="F851" s="6"/>
-      <c r="G851" s="6"/>
       <c r="H851" s="38"/>
       <c r="I851" s="38"/>
       <c r="J851" s="38"/>
@@ -29629,15 +29833,16 @@
       <c r="AA851" s="2">
         <v>13.9</v>
       </c>
-      <c r="AB851" s="6"/>
+      <c r="AB851" s="6">
+        <v>19.984677413450651</v>
+      </c>
       <c r="AC851" s="2">
         <v>51.6</v>
       </c>
-      <c r="AD851" s="2">
+      <c r="AE851" s="2"/>
+      <c r="AF851" s="2">
         <v>318.8</v>
       </c>
-      <c r="AE851" s="2"/>
-      <c r="AF851" s="2"/>
       <c r="AG851" s="2"/>
       <c r="AH851" s="2"/>
       <c r="AI851" s="2"/>
@@ -29657,7 +29862,7 @@
     </row>
     <row r="852" spans="1:46">
       <c r="A852" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B852" s="5">
         <v>30877.664199999999</v>
@@ -29666,14 +29871,13 @@
         <v>11</v>
       </c>
       <c r="D852" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>72.522522522522522</v>
       </c>
       <c r="E852" s="2">
         <v>1610</v>
       </c>
       <c r="F852" s="6"/>
-      <c r="G852" s="6"/>
       <c r="H852" s="38"/>
       <c r="I852" s="38"/>
       <c r="J852" s="38"/>
@@ -29696,15 +29900,16 @@
       <c r="AA852" s="2">
         <v>15.3</v>
       </c>
-      <c r="AB852" s="6"/>
+      <c r="AB852" s="6">
+        <v>20.987944268713981</v>
+      </c>
       <c r="AC852" s="2">
         <v>55.7</v>
       </c>
-      <c r="AD852" s="2">
+      <c r="AE852" s="2"/>
+      <c r="AF852" s="2">
         <v>365.2</v>
       </c>
-      <c r="AE852" s="2"/>
-      <c r="AF852" s="2"/>
       <c r="AG852" s="2"/>
       <c r="AH852" s="2"/>
       <c r="AI852" s="2"/>
@@ -29724,7 +29929,7 @@
     </row>
     <row r="853" spans="1:46">
       <c r="A853" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B853" s="5">
         <v>31242.9064</v>
@@ -29733,20 +29938,30 @@
         <v>12</v>
       </c>
       <c r="D853" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>69.819819819819813</v>
       </c>
       <c r="E853" s="2">
         <v>1550</v>
       </c>
-      <c r="F853" s="6"/>
-      <c r="G853" s="6"/>
+      <c r="F853" s="6">
+        <f t="shared" ref="F853" si="12">G853+H853+J853+N853</f>
+        <v>23020</v>
+      </c>
+      <c r="G853" s="6">
+        <v>110.00000000000001</v>
+      </c>
       <c r="H853" s="37">
         <v>1350</v>
       </c>
       <c r="I853" s="38"/>
-      <c r="J853" s="37"/>
-      <c r="K853" s="37"/>
+      <c r="J853" s="37">
+        <v>5290</v>
+      </c>
+      <c r="K853" s="37">
+        <f t="shared" ref="K853" si="13">J853+G853</f>
+        <v>5400</v>
+      </c>
       <c r="L853" s="37">
         <v>1500</v>
       </c>
@@ -29756,12 +29971,17 @@
       <c r="N853" s="38">
         <v>16269.999999999998</v>
       </c>
-      <c r="O853" s="38"/>
+      <c r="O853" s="38">
+        <f t="shared" ref="O853" si="14">N853+J853</f>
+        <v>21560</v>
+      </c>
       <c r="P853" s="38"/>
       <c r="Q853" s="38"/>
       <c r="R853" s="38"/>
       <c r="S853" s="38"/>
-      <c r="T853" s="37"/>
+      <c r="T853" s="39">
+        <v>6.6208456326228466</v>
+      </c>
       <c r="U853" s="37"/>
       <c r="V853" s="38">
         <v>56.06</v>
@@ -29773,15 +29993,16 @@
       <c r="AA853" s="2">
         <v>17.8</v>
       </c>
-      <c r="AB853" s="6"/>
+      <c r="AB853" s="6">
+        <v>22.014833209354752</v>
+      </c>
       <c r="AC853" s="2">
         <v>59</v>
       </c>
-      <c r="AD853" s="2">
+      <c r="AE853" s="2"/>
+      <c r="AF853" s="2">
         <v>427.4</v>
       </c>
-      <c r="AE853" s="2"/>
-      <c r="AF853" s="2"/>
       <c r="AG853" s="2"/>
       <c r="AH853" s="2"/>
       <c r="AI853" s="2"/>
@@ -29814,6 +30035,7 @@
       <c r="E854" s="3">
         <v>1260</v>
       </c>
+      <c r="G854" s="6"/>
       <c r="AN854" s="1" t="s">
         <v>35</v>
       </c>
@@ -29829,12 +30051,13 @@
         <v>7</v>
       </c>
       <c r="D855" s="20">
-        <f t="shared" ref="D855:D897" si="9">E855/E$854*100</f>
+        <f t="shared" ref="D855:D897" si="15">E855/E$854*100</f>
         <v>92.393650793650806</v>
       </c>
       <c r="E855" s="3">
         <v>1164.1600000000001</v>
       </c>
+      <c r="G855" s="6"/>
       <c r="M855" s="1">
         <v>288</v>
       </c>
@@ -29865,12 +30088,13 @@
         <v>8</v>
       </c>
       <c r="D856" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>92.392857142857153</v>
       </c>
       <c r="E856" s="3">
         <v>1164.1500000000001</v>
       </c>
+      <c r="G856" s="6"/>
       <c r="M856" s="3">
         <v>429</v>
       </c>
@@ -29904,12 +30128,13 @@
         <v>9</v>
       </c>
       <c r="D857" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>92.257936507936506</v>
       </c>
       <c r="E857" s="3">
         <v>1162.45</v>
       </c>
+      <c r="G857" s="6"/>
       <c r="M857" s="3">
         <v>630</v>
       </c>
@@ -29943,12 +30168,13 @@
         <v>10</v>
       </c>
       <c r="D858" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>91.326190476190476</v>
       </c>
       <c r="E858" s="3">
         <v>1150.71</v>
       </c>
+      <c r="G858" s="6"/>
       <c r="M858" s="3">
         <v>877.99999999999989</v>
       </c>
@@ -29985,12 +30211,13 @@
         <v>11</v>
       </c>
       <c r="D859" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>91.325396825396837</v>
       </c>
       <c r="E859" s="3">
         <v>1150.7</v>
       </c>
+      <c r="G859" s="6"/>
       <c r="M859" s="3">
         <v>1112</v>
       </c>
@@ -30027,12 +30254,13 @@
         <v>12</v>
       </c>
       <c r="D860" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>90.381746031746019</v>
       </c>
       <c r="E860" s="3">
         <v>1138.81</v>
       </c>
+      <c r="G860" s="6"/>
       <c r="M860" s="3">
         <v>1374</v>
       </c>
@@ -30069,12 +30297,13 @@
         <v>13</v>
       </c>
       <c r="D861" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>90.381746031746019</v>
       </c>
       <c r="E861" s="3">
         <v>1138.81</v>
       </c>
+      <c r="G861" s="6"/>
       <c r="M861" s="3">
         <v>1709</v>
       </c>
@@ -30108,12 +30337,13 @@
         <v>14</v>
       </c>
       <c r="D862" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>89.927777777777777</v>
       </c>
       <c r="E862" s="3">
         <v>1133.0899999999999</v>
       </c>
+      <c r="G862" s="6"/>
       <c r="M862" s="3">
         <v>1923</v>
       </c>
@@ -30147,12 +30377,13 @@
         <v>15</v>
       </c>
       <c r="D863" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>89.547619047619037</v>
       </c>
       <c r="E863" s="3">
         <v>1128.3</v>
       </c>
+      <c r="G863" s="6"/>
       <c r="M863" s="3">
         <v>2191</v>
       </c>
@@ -30186,12 +30417,13 @@
         <v>16</v>
       </c>
       <c r="D864" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>89.547619047619037</v>
       </c>
       <c r="E864" s="3">
         <v>1128.3</v>
       </c>
+      <c r="G864" s="6"/>
       <c r="M864" s="3">
         <v>2600</v>
       </c>
@@ -30225,7 +30457,7 @@
         <v>0</v>
       </c>
       <c r="D865" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>100</v>
       </c>
       <c r="E865" s="3">
@@ -30246,7 +30478,7 @@
         <v>7</v>
       </c>
       <c r="D866" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>94.30396825396825</v>
       </c>
       <c r="E866" s="3">
@@ -30282,7 +30514,7 @@
         <v>8</v>
       </c>
       <c r="D867" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>94.315873015873024</v>
       </c>
       <c r="E867" s="3">
@@ -30321,7 +30553,7 @@
         <v>9</v>
       </c>
       <c r="D868" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>94.315079365079356</v>
       </c>
       <c r="E868" s="3">
@@ -30360,7 +30592,7 @@
         <v>10</v>
       </c>
       <c r="D869" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>93.481746031746027</v>
       </c>
       <c r="E869" s="3">
@@ -30402,7 +30634,7 @@
         <v>11</v>
       </c>
       <c r="D870" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>93.248412698412707</v>
       </c>
       <c r="E870" s="3">
@@ -30444,7 +30676,7 @@
         <v>12</v>
       </c>
       <c r="D871" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>91.93730158730159</v>
       </c>
       <c r="E871" s="3">
@@ -30486,7 +30718,7 @@
         <v>13</v>
       </c>
       <c r="D872" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>91.715873015873001</v>
       </c>
       <c r="E872" s="3">
@@ -30525,7 +30757,7 @@
         <v>14</v>
       </c>
       <c r="D873" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>91.017460317460305</v>
       </c>
       <c r="E873" s="3">
@@ -30564,7 +30796,7 @@
         <v>15</v>
       </c>
       <c r="D874" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>90.575396825396822</v>
       </c>
       <c r="E874" s="3">
@@ -30603,7 +30835,7 @@
         <v>16</v>
       </c>
       <c r="D875" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>90.183333333333323</v>
       </c>
       <c r="E875" s="3">
@@ -30642,7 +30874,7 @@
         <v>0</v>
       </c>
       <c r="D876" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>100</v>
       </c>
       <c r="E876" s="3">
@@ -30663,7 +30895,7 @@
         <v>7</v>
       </c>
       <c r="D877" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>95.075396825396837</v>
       </c>
       <c r="E877" s="3">
@@ -30699,7 +30931,7 @@
         <v>8</v>
       </c>
       <c r="D878" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>94.842063492063488</v>
       </c>
       <c r="E878" s="3">
@@ -30738,7 +30970,7 @@
         <v>9</v>
       </c>
       <c r="D879" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>94.841269841269835</v>
       </c>
       <c r="E879" s="3">
@@ -30777,7 +31009,7 @@
         <v>10</v>
       </c>
       <c r="D880" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>93.933333333333323</v>
       </c>
       <c r="E880" s="3">
@@ -30819,7 +31051,7 @@
         <v>11</v>
       </c>
       <c r="D881" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>93.932539682539684</v>
       </c>
       <c r="E881" s="3">
@@ -30861,7 +31093,7 @@
         <v>12</v>
       </c>
       <c r="D882" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>93.098412698412687</v>
       </c>
       <c r="E882" s="3">
@@ -30903,7 +31135,7 @@
         <v>13</v>
       </c>
       <c r="D883" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>92.619841269841274</v>
       </c>
       <c r="E883" s="3">
@@ -30942,7 +31174,7 @@
         <v>14</v>
       </c>
       <c r="D884" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>92.385714285714286</v>
       </c>
       <c r="E884" s="3">
@@ -30981,7 +31213,7 @@
         <v>15</v>
       </c>
       <c r="D885" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>91.760317460317466</v>
       </c>
       <c r="E885" s="3">
@@ -31020,7 +31252,7 @@
         <v>16</v>
       </c>
       <c r="D886" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>90.865873015873021</v>
       </c>
       <c r="E886" s="3">
@@ -31059,7 +31291,7 @@
         <v>0</v>
       </c>
       <c r="D887" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>100</v>
       </c>
       <c r="E887" s="3">
@@ -31080,7 +31312,7 @@
         <v>7</v>
       </c>
       <c r="D888" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>91.487301587301587</v>
       </c>
       <c r="E888" s="3">
@@ -31116,7 +31348,7 @@
         <v>8</v>
       </c>
       <c r="D889" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>91.265873015873026</v>
       </c>
       <c r="E889" s="3">
@@ -31155,7 +31387,7 @@
         <v>9</v>
       </c>
       <c r="D890" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>91.031746031746025</v>
       </c>
       <c r="E890" s="3">
@@ -31194,7 +31426,7 @@
         <v>10</v>
       </c>
       <c r="D891" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>90.123809523809513</v>
       </c>
       <c r="E891" s="3">
@@ -31236,7 +31468,7 @@
         <v>11</v>
       </c>
       <c r="D892" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>89.730952380952374</v>
       </c>
       <c r="E892" s="3">
@@ -31278,7 +31510,7 @@
         <v>12</v>
       </c>
       <c r="D893" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>88.811111111111103</v>
       </c>
       <c r="E893" s="3">
@@ -31320,7 +31552,7 @@
         <v>13</v>
       </c>
       <c r="D894" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>88.810317460317449</v>
       </c>
       <c r="E894" s="3">
@@ -31359,7 +31591,7 @@
         <v>14</v>
       </c>
       <c r="D895" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>87.890476190476193</v>
       </c>
       <c r="E895" s="3">
@@ -31398,7 +31630,7 @@
         <v>15</v>
       </c>
       <c r="D896" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>87.876984126984127</v>
       </c>
       <c r="E896" s="3">
@@ -31437,7 +31669,7 @@
         <v>16</v>
       </c>
       <c r="D897" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>87.656349206349205</v>
       </c>
       <c r="E897" s="3">
@@ -33044,7 +33276,7 @@
         <v>18</v>
       </c>
       <c r="D948" s="20">
-        <f t="shared" ref="D948:D982" si="10">E948/E$946*100</f>
+        <f t="shared" ref="D948:D982" si="16">E948/E$946*100</f>
         <v>41.80602006688963</v>
       </c>
       <c r="E948" s="3">
@@ -33071,7 +33303,7 @@
         <v>19</v>
       </c>
       <c r="D949" s="20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>41.80602006688963</v>
       </c>
       <c r="E949" s="3">
@@ -33098,7 +33330,7 @@
         <v>20</v>
       </c>
       <c r="D950" s="20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>41.80602006688963</v>
       </c>
       <c r="E950" s="3">
@@ -33125,7 +33357,7 @@
         <v>21</v>
       </c>
       <c r="D951" s="20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>41.80602006688963</v>
       </c>
       <c r="E951" s="3">
@@ -33152,7 +33384,7 @@
         <v>22</v>
       </c>
       <c r="D952" s="20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>41.80602006688963</v>
       </c>
       <c r="E952" s="3">
@@ -33179,7 +33411,7 @@
         <v>23</v>
       </c>
       <c r="D953" s="20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>41.80602006688963</v>
       </c>
       <c r="E953" s="3">
@@ -33206,7 +33438,7 @@
         <v>24</v>
       </c>
       <c r="D954" s="20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>41.80602006688963</v>
       </c>
       <c r="E954" s="3">
@@ -33233,7 +33465,7 @@
         <v>25</v>
       </c>
       <c r="D955" s="20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>41.80602006688963</v>
       </c>
       <c r="E955" s="3">
@@ -33326,7 +33558,7 @@
         <v>26</v>
       </c>
       <c r="D956" s="20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>41.80602006688963</v>
       </c>
       <c r="E956" s="3">
@@ -33350,7 +33582,7 @@
         <v>27</v>
       </c>
       <c r="D957" s="20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>41.80602006688963</v>
       </c>
       <c r="E957" s="3">
@@ -33377,7 +33609,7 @@
         <v>28</v>
       </c>
       <c r="D958" s="20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>41.80602006688963</v>
       </c>
       <c r="E958" s="3">
@@ -33404,7 +33636,7 @@
         <v>29</v>
       </c>
       <c r="D959" s="20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>41.80602006688963</v>
       </c>
       <c r="E959" s="3">
@@ -33479,7 +33711,7 @@
         <v>30</v>
       </c>
       <c r="D960" s="20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>41.80602006688963</v>
       </c>
       <c r="E960" s="3">
@@ -33506,7 +33738,7 @@
         <v>31</v>
       </c>
       <c r="D961" s="20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>41.80602006688963</v>
       </c>
       <c r="E961" s="3">
@@ -33533,7 +33765,7 @@
         <v>32</v>
       </c>
       <c r="D962" s="20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>41.80602006688963</v>
       </c>
       <c r="E962" s="3">
@@ -33560,7 +33792,7 @@
         <v>33</v>
       </c>
       <c r="D963" s="20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>41.80602006688963</v>
       </c>
       <c r="E963" s="3">
@@ -33587,7 +33819,7 @@
         <v>34</v>
       </c>
       <c r="D964" s="20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>41.80602006688963</v>
       </c>
       <c r="E964" s="3">
@@ -33662,7 +33894,7 @@
         <v>17</v>
       </c>
       <c r="D965" s="20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>41.80602006688963</v>
       </c>
       <c r="E965" s="3">
@@ -33689,7 +33921,7 @@
         <v>18</v>
       </c>
       <c r="D966" s="20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>41.80602006688963</v>
       </c>
       <c r="E966" s="3">
@@ -33716,7 +33948,7 @@
         <v>19</v>
       </c>
       <c r="D967" s="20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>41.80602006688963</v>
       </c>
       <c r="E967" s="3">
@@ -33743,7 +33975,7 @@
         <v>20</v>
       </c>
       <c r="D968" s="20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>41.80602006688963</v>
       </c>
       <c r="E968" s="3">
@@ -33770,7 +34002,7 @@
         <v>21</v>
       </c>
       <c r="D969" s="20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>41.80602006688963</v>
       </c>
       <c r="E969" s="3">
@@ -33797,7 +34029,7 @@
         <v>22</v>
       </c>
       <c r="D970" s="20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>41.80602006688963</v>
       </c>
       <c r="E970" s="3">
@@ -33824,7 +34056,7 @@
         <v>23</v>
       </c>
       <c r="D971" s="20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>41.80602006688963</v>
       </c>
       <c r="E971" s="3">
@@ -33851,7 +34083,7 @@
         <v>24</v>
       </c>
       <c r="D972" s="20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>41.80602006688963</v>
       </c>
       <c r="E972" s="3">
@@ -33878,7 +34110,7 @@
         <v>25</v>
       </c>
       <c r="D973" s="20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>41.80602006688963</v>
       </c>
       <c r="E973" s="3">
@@ -33971,7 +34203,7 @@
         <v>26</v>
       </c>
       <c r="D974" s="20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>41.80602006688963</v>
       </c>
       <c r="E974" s="3">
@@ -33995,7 +34227,7 @@
         <v>27</v>
       </c>
       <c r="D975" s="20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>41.80602006688963</v>
       </c>
       <c r="E975" s="3">
@@ -34022,7 +34254,7 @@
         <v>28</v>
       </c>
       <c r="D976" s="20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>41.80602006688963</v>
       </c>
       <c r="E976" s="3">
@@ -34049,7 +34281,7 @@
         <v>29</v>
       </c>
       <c r="D977" s="20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>41.80602006688963</v>
       </c>
       <c r="E977" s="3">
@@ -34124,7 +34356,7 @@
         <v>30</v>
       </c>
       <c r="D978" s="20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>41.80602006688963</v>
       </c>
       <c r="E978" s="3">
@@ -34151,7 +34383,7 @@
         <v>31</v>
       </c>
       <c r="D979" s="20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>41.80602006688963</v>
       </c>
       <c r="E979" s="3">
@@ -34178,7 +34410,7 @@
         <v>32</v>
       </c>
       <c r="D980" s="20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>41.80602006688963</v>
       </c>
       <c r="E980" s="3">
@@ -34205,7 +34437,7 @@
         <v>33</v>
       </c>
       <c r="D981" s="20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>41.80602006688963</v>
       </c>
       <c r="E981" s="3">
@@ -34232,7 +34464,7 @@
         <v>34</v>
       </c>
       <c r="D982" s="20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>41.80602006688963</v>
       </c>
       <c r="E982" s="3">

</xml_diff>

<commit_message>
Added TowerHill and SETRES sites
</commit_message>
<xml_diff>
--- a/Prototypes/Pinus/Observed.xlsx
+++ b/Prototypes/Pinus/Observed.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\APSIMxSourceTree\Prototypes\Pinus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35DF1E46-5BF1-4887-B80A-C6D280B44B3E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B6BB5BB-BEE1-42CB-93F2-BDFF3E26C351}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" tabRatio="653" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -270,9 +270,6 @@
     <t>TowerHillC</t>
   </si>
   <si>
-    <t>TowerHillF</t>
-  </si>
-  <si>
     <t>Pinus.Foliar.Nconc (g/g)</t>
   </si>
   <si>
@@ -333,16 +330,19 @@
     <t>Pinus.BelowGround.Wt</t>
   </si>
   <si>
-    <t>PurukiSTahi</t>
-  </si>
-  <si>
-    <t>PurukiSInviolate</t>
-  </si>
-  <si>
     <t>Pinus.Stem.Volub</t>
   </si>
   <si>
     <t>Pinus.AboveGround.N</t>
+  </si>
+  <si>
+    <t>PurukiTahi</t>
+  </si>
+  <si>
+    <t>PurukiInviolate</t>
+  </si>
+  <si>
+    <t>TowerHillN</t>
   </si>
 </sst>
 </file>
@@ -354,7 +354,7 @@
     <numFmt numFmtId="165" formatCode="[$-C09]dd\-mmm\-yy;@"/>
     <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -419,6 +419,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -467,7 +474,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -540,6 +547,7 @@
     <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="0.0" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -922,10 +930,10 @@
   <dimension ref="A1:BP982"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="U2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D886" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="W1" sqref="W1"/>
+      <selection pane="bottomRight" activeCell="V982" sqref="V982"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="12.75"/>
@@ -969,46 +977,46 @@
         <v>24</v>
       </c>
       <c r="E1" s="29" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F1" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="G1" s="29" t="s">
         <v>80</v>
       </c>
-      <c r="G1" s="29" t="s">
+      <c r="H1" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="H1" s="29" t="s">
+      <c r="I1" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="I1" s="29" t="s">
+      <c r="J1" s="29" t="s">
         <v>83</v>
-      </c>
-      <c r="J1" s="29" t="s">
-        <v>84</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>53</v>
       </c>
       <c r="L1" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="M1" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="M1" s="29" t="s">
+      <c r="N1" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="N1" s="29" t="s">
+      <c r="O1" s="29" t="s">
         <v>87</v>
       </c>
-      <c r="O1" s="29" t="s">
+      <c r="P1" s="29" t="s">
         <v>88</v>
       </c>
-      <c r="P1" s="29" t="s">
+      <c r="Q1" s="29" t="s">
         <v>89</v>
       </c>
-      <c r="Q1" s="29" t="s">
+      <c r="R1" s="29" t="s">
         <v>90</v>
-      </c>
-      <c r="R1" s="29" t="s">
-        <v>91</v>
       </c>
       <c r="S1" s="29" t="s">
         <v>3</v>
@@ -1020,7 +1028,7 @@
         <v>30</v>
       </c>
       <c r="V1" s="29" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="W1" s="1" t="s">
         <v>54</v>
@@ -1035,22 +1043,22 @@
         <v>8</v>
       </c>
       <c r="AA1" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="AB1" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="AB1" s="29" t="s">
+      <c r="AC1" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="AC1" s="29" t="s">
+      <c r="AD1" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="AD1" s="29" t="s">
+      <c r="AE1" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="AE1" s="1" t="s">
-        <v>78</v>
-      </c>
       <c r="AF1" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="AG1" s="29" t="s">
         <v>52</v>
@@ -1062,10 +1070,10 @@
         <v>36</v>
       </c>
       <c r="AJ1" s="29" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AK1" s="29" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AL1" s="29" t="s">
         <v>26</v>
@@ -27882,7 +27890,7 @@
     </row>
     <row r="828" spans="1:46">
       <c r="A828" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B828" s="16">
         <v>26860</v>
@@ -27942,7 +27950,7 @@
     </row>
     <row r="829" spans="1:46">
       <c r="A829" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B829" s="5">
         <v>27590.484400000001</v>
@@ -28036,7 +28044,7 @@
     </row>
     <row r="830" spans="1:46">
       <c r="A830" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B830" s="5">
         <v>27955.726600000002</v>
@@ -28130,7 +28138,7 @@
     </row>
     <row r="831" spans="1:46">
       <c r="A831" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B831" s="5">
         <v>28320.968799999999</v>
@@ -28224,7 +28232,7 @@
     </row>
     <row r="832" spans="1:46">
       <c r="A832" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B832" s="5">
         <v>28686.210999999999</v>
@@ -28322,7 +28330,7 @@
     </row>
     <row r="833" spans="1:46">
       <c r="A833" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B833" s="5">
         <v>29047.800778000001</v>
@@ -28420,7 +28428,7 @@
     </row>
     <row r="834" spans="1:46">
       <c r="A834" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B834" s="5">
         <v>29051.4532</v>
@@ -28518,7 +28526,7 @@
     </row>
     <row r="835" spans="1:46">
       <c r="A835" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B835" s="5">
         <v>29416.695400000001</v>
@@ -28616,7 +28624,7 @@
     </row>
     <row r="836" spans="1:46">
       <c r="A836" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B836" s="5">
         <v>29781.937600000001</v>
@@ -28714,7 +28722,7 @@
     </row>
     <row r="837" spans="1:46">
       <c r="A837" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B837" s="5">
         <v>30147.179800000002</v>
@@ -28812,7 +28820,7 @@
     </row>
     <row r="838" spans="1:46">
       <c r="A838" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B838" s="5">
         <v>30508.769577999999</v>
@@ -28910,7 +28918,7 @@
     </row>
     <row r="839" spans="1:46">
       <c r="A839" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B839" s="5">
         <v>30512.421999999999</v>
@@ -29008,7 +29016,7 @@
     </row>
     <row r="840" spans="1:46">
       <c r="A840" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B840" s="5">
         <v>30877.664199999999</v>
@@ -29106,7 +29114,7 @@
     </row>
     <row r="841" spans="1:46">
       <c r="A841" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B841" s="5">
         <v>31242.9064</v>
@@ -29204,7 +29212,7 @@
     </row>
     <row r="842" spans="1:46">
       <c r="A842" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B842" s="16">
         <v>26860</v>
@@ -29262,7 +29270,7 @@
     </row>
     <row r="843" spans="1:46">
       <c r="A843" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B843" s="5">
         <v>27590.484400000001</v>
@@ -29328,7 +29336,7 @@
     </row>
     <row r="844" spans="1:46">
       <c r="A844" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B844" s="5">
         <v>27955.726600000002</v>
@@ -29394,7 +29402,7 @@
     </row>
     <row r="845" spans="1:46">
       <c r="A845" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B845" s="5">
         <v>28320.968799999999</v>
@@ -29460,7 +29468,7 @@
     </row>
     <row r="846" spans="1:46">
       <c r="A846" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B846" s="5">
         <v>28686.210999999999</v>
@@ -29527,7 +29535,7 @@
     </row>
     <row r="847" spans="1:46">
       <c r="A847" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B847" s="5">
         <v>29051.4532</v>
@@ -29594,7 +29602,7 @@
     </row>
     <row r="848" spans="1:46">
       <c r="A848" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B848" s="5">
         <v>29416.695400000001</v>
@@ -29661,7 +29669,7 @@
     </row>
     <row r="849" spans="1:46">
       <c r="A849" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B849" s="5">
         <v>29781.937600000001</v>
@@ -29728,7 +29736,7 @@
     </row>
     <row r="850" spans="1:46">
       <c r="A850" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B850" s="5">
         <v>30147.179800000002</v>
@@ -29795,7 +29803,7 @@
     </row>
     <row r="851" spans="1:46">
       <c r="A851" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B851" s="5">
         <v>30512.421999999999</v>
@@ -29862,7 +29870,7 @@
     </row>
     <row r="852" spans="1:46">
       <c r="A852" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B852" s="5">
         <v>30877.664199999999</v>
@@ -29929,7 +29937,7 @@
     </row>
     <row r="853" spans="1:46">
       <c r="A853" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B853" s="5">
         <v>31242.9064</v>
@@ -33235,7 +33243,7 @@
         <v>100</v>
       </c>
       <c r="E946" s="3">
-        <v>1495</v>
+        <v>1496</v>
       </c>
     </row>
     <row r="947" spans="1:68">
@@ -33250,12 +33258,12 @@
       </c>
       <c r="D947" s="20">
         <f>E947/E$946*100</f>
-        <v>41.80602006688963</v>
+        <v>41.778074866310163</v>
       </c>
       <c r="E947" s="3">
         <v>625</v>
       </c>
-      <c r="AF947" s="3">
+      <c r="AD947" s="3">
         <v>110.6</v>
       </c>
       <c r="AG947" s="3">
@@ -33277,12 +33285,12 @@
       </c>
       <c r="D948" s="20">
         <f t="shared" ref="D948:D982" si="16">E948/E$946*100</f>
-        <v>41.80602006688963</v>
+        <v>41.778074866310163</v>
       </c>
       <c r="E948" s="3">
         <v>625</v>
       </c>
-      <c r="AF948" s="3">
+      <c r="AD948" s="3">
         <v>119.16</v>
       </c>
       <c r="AG948" s="3">
@@ -33304,12 +33312,12 @@
       </c>
       <c r="D949" s="20">
         <f t="shared" si="16"/>
-        <v>41.80602006688963</v>
+        <v>41.778074866310163</v>
       </c>
       <c r="E949" s="3">
         <v>625</v>
       </c>
-      <c r="AF949" s="3">
+      <c r="AD949" s="3">
         <v>127.61</v>
       </c>
       <c r="AG949" s="3">
@@ -33331,12 +33339,12 @@
       </c>
       <c r="D950" s="20">
         <f t="shared" si="16"/>
-        <v>41.80602006688963</v>
+        <v>41.778074866310163</v>
       </c>
       <c r="E950" s="3">
         <v>625</v>
       </c>
-      <c r="AF950" s="3">
+      <c r="AD950" s="3">
         <v>136.59</v>
       </c>
       <c r="AG950" s="3">
@@ -33358,12 +33366,12 @@
       </c>
       <c r="D951" s="20">
         <f t="shared" si="16"/>
-        <v>41.80602006688963</v>
+        <v>41.778074866310163</v>
       </c>
       <c r="E951" s="3">
         <v>625</v>
       </c>
-      <c r="AF951" s="3">
+      <c r="AD951" s="3">
         <v>147.47</v>
       </c>
       <c r="AG951" s="3">
@@ -33385,12 +33393,12 @@
       </c>
       <c r="D952" s="20">
         <f t="shared" si="16"/>
-        <v>41.80602006688963</v>
+        <v>41.778074866310163</v>
       </c>
       <c r="E952" s="3">
         <v>625</v>
       </c>
-      <c r="AF952" s="3">
+      <c r="AD952" s="3">
         <v>156.59</v>
       </c>
       <c r="AG952" s="3">
@@ -33412,12 +33420,12 @@
       </c>
       <c r="D953" s="20">
         <f t="shared" si="16"/>
-        <v>41.80602006688963</v>
+        <v>41.778074866310163</v>
       </c>
       <c r="E953" s="3">
         <v>625</v>
       </c>
-      <c r="AF953" s="3">
+      <c r="AD953" s="3">
         <v>165.34</v>
       </c>
       <c r="AG953" s="3">
@@ -33439,12 +33447,12 @@
       </c>
       <c r="D954" s="20">
         <f t="shared" si="16"/>
-        <v>41.80602006688963</v>
+        <v>41.778074866310163</v>
       </c>
       <c r="E954" s="3">
         <v>625</v>
       </c>
-      <c r="AF954" s="3">
+      <c r="AD954" s="3">
         <v>175.29</v>
       </c>
       <c r="AG954" s="3">
@@ -33466,7 +33474,7 @@
       </c>
       <c r="D955" s="20">
         <f t="shared" si="16"/>
-        <v>41.80602006688963</v>
+        <v>41.778074866310163</v>
       </c>
       <c r="E955" s="3">
         <v>625</v>
@@ -33477,12 +33485,16 @@
       <c r="G955" s="3">
         <v>631</v>
       </c>
-      <c r="I955" s="3">
+      <c r="H955" s="3">
         <v>545</v>
       </c>
       <c r="J955" s="3">
         <v>1205</v>
       </c>
+      <c r="K955" s="3">
+        <f>G955+J955</f>
+        <v>1836</v>
+      </c>
       <c r="L955" s="3">
         <v>1518</v>
       </c>
@@ -33492,10 +33504,17 @@
       <c r="N955" s="3">
         <v>10602</v>
       </c>
+      <c r="O955" s="3">
+        <f>N955+J955</f>
+        <v>11807</v>
+      </c>
+      <c r="V955" s="3">
+        <v>12.965</v>
+      </c>
       <c r="W955" s="3">
         <v>1457</v>
       </c>
-      <c r="AF955" s="3">
+      <c r="AD955" s="3">
         <v>184.82999999999998</v>
       </c>
       <c r="AG955" s="3">
@@ -33547,7 +33566,7 @@
         <v>15.000000000000002</v>
       </c>
     </row>
-    <row r="956" spans="1:68">
+    <row r="956" spans="1:68" ht="15">
       <c r="A956" s="3" t="s">
         <v>70</v>
       </c>
@@ -33559,19 +33578,20 @@
       </c>
       <c r="D956" s="20">
         <f t="shared" si="16"/>
-        <v>41.80602006688963</v>
+        <v>41.778074866310163</v>
       </c>
       <c r="E956" s="3">
         <v>625</v>
       </c>
-      <c r="AF956" s="3">
+      <c r="K956" s="42"/>
+      <c r="AD956" s="3">
         <v>193.64</v>
       </c>
       <c r="AG956" s="3">
         <v>7.4476923076923072</v>
       </c>
     </row>
-    <row r="957" spans="1:68">
+    <row r="957" spans="1:68" ht="15">
       <c r="A957" s="3" t="s">
         <v>70</v>
       </c>
@@ -33583,12 +33603,13 @@
       </c>
       <c r="D957" s="20">
         <f t="shared" si="16"/>
-        <v>41.80602006688963</v>
+        <v>41.778074866310163</v>
       </c>
       <c r="E957" s="3">
         <v>625</v>
       </c>
-      <c r="AF957" s="3">
+      <c r="K957" s="42"/>
+      <c r="AD957" s="3">
         <v>201.92</v>
       </c>
       <c r="AG957" s="3">
@@ -33610,12 +33631,13 @@
       </c>
       <c r="D958" s="20">
         <f t="shared" si="16"/>
-        <v>41.80602006688963</v>
+        <v>41.778074866310163</v>
       </c>
       <c r="E958" s="3">
         <v>625</v>
       </c>
-      <c r="AF958" s="3">
+      <c r="V958"/>
+      <c r="AD958" s="3">
         <v>205.76</v>
       </c>
       <c r="AG958" s="3">
@@ -33637,7 +33659,7 @@
       </c>
       <c r="D959" s="20">
         <f t="shared" si="16"/>
-        <v>41.80602006688963</v>
+        <v>41.778074866310163</v>
       </c>
       <c r="E959" s="3">
         <v>625</v>
@@ -33645,7 +33667,7 @@
       <c r="F959" s="3">
         <v>13777</v>
       </c>
-      <c r="I959" s="3">
+      <c r="H959" s="3">
         <v>423.00000000000006</v>
       </c>
       <c r="K959" s="3">
@@ -33660,10 +33682,13 @@
       <c r="N959" s="3">
         <v>11145</v>
       </c>
+      <c r="V959">
+        <v>11.751000000000001</v>
+      </c>
       <c r="W959" s="3">
         <v>3927.0000000000005</v>
       </c>
-      <c r="AF959" s="3">
+      <c r="AD959" s="3">
         <v>215.7</v>
       </c>
       <c r="AG959" s="3">
@@ -33712,12 +33737,12 @@
       </c>
       <c r="D960" s="20">
         <f t="shared" si="16"/>
-        <v>41.80602006688963</v>
+        <v>41.778074866310163</v>
       </c>
       <c r="E960" s="3">
         <v>625</v>
       </c>
-      <c r="AF960" s="3">
+      <c r="AD960" s="3">
         <v>227.14999999999998</v>
       </c>
       <c r="AG960" s="3">
@@ -33739,12 +33764,12 @@
       </c>
       <c r="D961" s="20">
         <f t="shared" si="16"/>
-        <v>41.80602006688963</v>
+        <v>41.778074866310163</v>
       </c>
       <c r="E961" s="3">
         <v>625</v>
       </c>
-      <c r="AF961" s="3">
+      <c r="AD961" s="3">
         <v>233.27999999999997</v>
       </c>
       <c r="AG961" s="3">
@@ -33766,12 +33791,12 @@
       </c>
       <c r="D962" s="20">
         <f t="shared" si="16"/>
-        <v>41.80602006688963</v>
+        <v>41.778074866310163</v>
       </c>
       <c r="E962" s="3">
         <v>625</v>
       </c>
-      <c r="AF962" s="3">
+      <c r="AD962" s="3">
         <v>240.28999999999996</v>
       </c>
       <c r="AG962" s="3">
@@ -33793,12 +33818,12 @@
       </c>
       <c r="D963" s="20">
         <f t="shared" si="16"/>
-        <v>41.80602006688963</v>
+        <v>41.778074866310163</v>
       </c>
       <c r="E963" s="3">
         <v>625</v>
       </c>
-      <c r="AF963" s="3">
+      <c r="AD963" s="3">
         <v>245.75999999999996</v>
       </c>
       <c r="AG963" s="3">
@@ -33820,7 +33845,7 @@
       </c>
       <c r="D964" s="20">
         <f t="shared" si="16"/>
-        <v>41.80602006688963</v>
+        <v>41.778074866310163</v>
       </c>
       <c r="E964" s="3">
         <v>625</v>
@@ -33828,7 +33853,7 @@
       <c r="F964" s="3">
         <v>17651</v>
       </c>
-      <c r="I964" s="3">
+      <c r="H964" s="3">
         <v>528</v>
       </c>
       <c r="K964" s="3">
@@ -33843,10 +33868,13 @@
       <c r="N964" s="3">
         <v>13838</v>
       </c>
+      <c r="V964">
+        <v>15.704000000000001</v>
+      </c>
       <c r="W964" s="3">
         <v>3336.9999999999995</v>
       </c>
-      <c r="AF964" s="3">
+      <c r="AD964" s="3">
         <v>256.16999999999996</v>
       </c>
       <c r="AG964" s="3">
@@ -33885,7 +33913,7 @@
     </row>
     <row r="965" spans="1:68">
       <c r="A965" s="3" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="B965" s="5">
         <v>29021.117399999999</v>
@@ -33895,12 +33923,12 @@
       </c>
       <c r="D965" s="20">
         <f t="shared" si="16"/>
-        <v>41.80602006688963</v>
+        <v>41.778074866310163</v>
       </c>
       <c r="E965" s="3">
         <v>625</v>
       </c>
-      <c r="AF965" s="3">
+      <c r="AD965" s="3">
         <v>110.3</v>
       </c>
       <c r="AG965" s="3">
@@ -33912,7 +33940,7 @@
     </row>
     <row r="966" spans="1:68">
       <c r="A966" s="3" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="B966" s="5">
         <v>29386.3596</v>
@@ -33922,12 +33950,12 @@
       </c>
       <c r="D966" s="20">
         <f t="shared" si="16"/>
-        <v>41.80602006688963</v>
+        <v>41.778074866310163</v>
       </c>
       <c r="E966" s="3">
         <v>625</v>
       </c>
-      <c r="AF966" s="3">
+      <c r="AD966" s="3">
         <v>121.94</v>
       </c>
       <c r="AG966" s="3">
@@ -33939,7 +33967,7 @@
     </row>
     <row r="967" spans="1:68">
       <c r="A967" s="3" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="B967" s="5">
         <v>29751.6018</v>
@@ -33949,12 +33977,12 @@
       </c>
       <c r="D967" s="20">
         <f t="shared" si="16"/>
-        <v>41.80602006688963</v>
+        <v>41.778074866310163</v>
       </c>
       <c r="E967" s="3">
         <v>625</v>
       </c>
-      <c r="AF967" s="3">
+      <c r="AD967" s="3">
         <v>135.66</v>
       </c>
       <c r="AG967" s="3">
@@ -33966,7 +33994,7 @@
     </row>
     <row r="968" spans="1:68">
       <c r="A968" s="3" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="B968" s="5">
         <v>30116.844000000001</v>
@@ -33976,12 +34004,12 @@
       </c>
       <c r="D968" s="20">
         <f t="shared" si="16"/>
-        <v>41.80602006688963</v>
+        <v>41.778074866310163</v>
       </c>
       <c r="E968" s="3">
         <v>625</v>
       </c>
-      <c r="AF968" s="3">
+      <c r="AD968" s="3">
         <v>152.26999999999998</v>
       </c>
       <c r="AG968" s="3">
@@ -33993,7 +34021,7 @@
     </row>
     <row r="969" spans="1:68">
       <c r="A969" s="3" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="B969" s="5">
         <v>30482.086200000002</v>
@@ -34003,12 +34031,12 @@
       </c>
       <c r="D969" s="20">
         <f t="shared" si="16"/>
-        <v>41.80602006688963</v>
+        <v>41.778074866310163</v>
       </c>
       <c r="E969" s="3">
         <v>625</v>
       </c>
-      <c r="AF969" s="3">
+      <c r="AD969" s="3">
         <v>174.11999999999998</v>
       </c>
       <c r="AG969" s="3">
@@ -34020,7 +34048,7 @@
     </row>
     <row r="970" spans="1:68">
       <c r="A970" s="3" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="B970" s="5">
         <v>30847.328399999999</v>
@@ -34030,12 +34058,12 @@
       </c>
       <c r="D970" s="20">
         <f t="shared" si="16"/>
-        <v>41.80602006688963</v>
+        <v>41.778074866310163</v>
       </c>
       <c r="E970" s="3">
         <v>625</v>
       </c>
-      <c r="AF970" s="3">
+      <c r="AD970" s="3">
         <v>192.77999999999997</v>
       </c>
       <c r="AG970" s="3">
@@ -34047,7 +34075,7 @@
     </row>
     <row r="971" spans="1:68">
       <c r="A971" s="3" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="B971" s="5">
         <v>31212.570599999999</v>
@@ -34057,12 +34085,12 @@
       </c>
       <c r="D971" s="20">
         <f t="shared" si="16"/>
-        <v>41.80602006688963</v>
+        <v>41.778074866310163</v>
       </c>
       <c r="E971" s="3">
         <v>625</v>
       </c>
-      <c r="AF971" s="3">
+      <c r="AD971" s="3">
         <v>219.14</v>
       </c>
       <c r="AG971" s="3">
@@ -34074,7 +34102,7 @@
     </row>
     <row r="972" spans="1:68">
       <c r="A972" s="3" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="B972" s="5">
         <v>31577.8128</v>
@@ -34084,12 +34112,12 @@
       </c>
       <c r="D972" s="20">
         <f t="shared" si="16"/>
-        <v>41.80602006688963</v>
+        <v>41.778074866310163</v>
       </c>
       <c r="E972" s="3">
         <v>625</v>
       </c>
-      <c r="AF972" s="3">
+      <c r="AD972" s="3">
         <v>252.42999999999998</v>
       </c>
       <c r="AG972" s="3">
@@ -34101,7 +34129,7 @@
     </row>
     <row r="973" spans="1:68">
       <c r="A973" s="3" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="B973" s="5">
         <v>31943.055</v>
@@ -34111,7 +34139,7 @@
       </c>
       <c r="D973" s="20">
         <f t="shared" si="16"/>
-        <v>41.80602006688963</v>
+        <v>41.778074866310163</v>
       </c>
       <c r="E973" s="3">
         <v>625</v>
@@ -34122,12 +34150,16 @@
       <c r="G973" s="3">
         <v>667</v>
       </c>
-      <c r="I973" s="3">
+      <c r="H973" s="3">
         <v>1057</v>
       </c>
       <c r="J973" s="3">
         <v>1805</v>
       </c>
+      <c r="K973" s="3">
+        <f>G973+J973</f>
+        <v>2472</v>
+      </c>
       <c r="L973" s="3">
         <v>2456</v>
       </c>
@@ -34137,10 +34169,17 @@
       <c r="N973" s="3">
         <v>15190</v>
       </c>
+      <c r="O973" s="3">
+        <f>N973+J973</f>
+        <v>16995</v>
+      </c>
+      <c r="V973" s="3">
+        <v>26.013000000000005</v>
+      </c>
       <c r="W973" s="3">
         <v>1257</v>
       </c>
-      <c r="AF973" s="3">
+      <c r="AD973" s="3">
         <v>283.27999999999997</v>
       </c>
       <c r="AG973" s="3">
@@ -34194,7 +34233,7 @@
     </row>
     <row r="974" spans="1:68">
       <c r="A974" s="3" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="B974" s="5">
         <v>32308.297200000001</v>
@@ -34204,12 +34243,12 @@
       </c>
       <c r="D974" s="20">
         <f t="shared" si="16"/>
-        <v>41.80602006688963</v>
+        <v>41.778074866310163</v>
       </c>
       <c r="E974" s="3">
         <v>625</v>
       </c>
-      <c r="AF974" s="3">
+      <c r="AD974" s="3">
         <v>310.58999999999997</v>
       </c>
       <c r="AG974" s="3">
@@ -34218,7 +34257,7 @@
     </row>
     <row r="975" spans="1:68">
       <c r="A975" s="3" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="B975" s="5">
         <v>32673.539400000001</v>
@@ -34228,12 +34267,12 @@
       </c>
       <c r="D975" s="20">
         <f t="shared" si="16"/>
-        <v>41.80602006688963</v>
+        <v>41.778074866310163</v>
       </c>
       <c r="E975" s="3">
         <v>625</v>
       </c>
-      <c r="AF975" s="3">
+      <c r="AD975" s="3">
         <v>344</v>
       </c>
       <c r="AG975" s="3">
@@ -34245,7 +34284,7 @@
     </row>
     <row r="976" spans="1:68">
       <c r="A976" s="3" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="B976" s="5">
         <v>33038.781600000002</v>
@@ -34255,12 +34294,12 @@
       </c>
       <c r="D976" s="20">
         <f t="shared" si="16"/>
-        <v>41.80602006688963</v>
+        <v>41.778074866310163</v>
       </c>
       <c r="E976" s="3">
         <v>625</v>
       </c>
-      <c r="AF976" s="3">
+      <c r="AD976" s="3">
         <v>374.32</v>
       </c>
       <c r="AG976" s="3">
@@ -34272,7 +34311,7 @@
     </row>
     <row r="977" spans="1:68">
       <c r="A977" s="3" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="B977" s="5">
         <v>33404.023800000003</v>
@@ -34282,7 +34321,7 @@
       </c>
       <c r="D977" s="20">
         <f t="shared" si="16"/>
-        <v>41.80602006688963</v>
+        <v>41.778074866310163</v>
       </c>
       <c r="E977" s="3">
         <v>625</v>
@@ -34290,7 +34329,7 @@
       <c r="F977" s="3">
         <v>25530</v>
       </c>
-      <c r="I977" s="3">
+      <c r="H977" s="3">
         <v>1050</v>
       </c>
       <c r="K977" s="3">
@@ -34305,10 +34344,13 @@
       <c r="N977" s="3">
         <v>21086</v>
       </c>
+      <c r="V977" s="3">
+        <v>35.235999999999997</v>
+      </c>
       <c r="W977" s="3">
         <v>4821</v>
       </c>
-      <c r="AF977" s="3">
+      <c r="AD977" s="3">
         <v>407.74</v>
       </c>
       <c r="AG977" s="3">
@@ -34347,7 +34389,7 @@
     </row>
     <row r="978" spans="1:68">
       <c r="A978" s="3" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="B978" s="5">
         <v>33769.266000000003</v>
@@ -34357,12 +34399,12 @@
       </c>
       <c r="D978" s="20">
         <f t="shared" si="16"/>
-        <v>41.80602006688963</v>
+        <v>41.778074866310163</v>
       </c>
       <c r="E978" s="3">
         <v>625</v>
       </c>
-      <c r="AF978" s="3">
+      <c r="AD978" s="3">
         <v>438.73</v>
       </c>
       <c r="AG978" s="3">
@@ -34374,7 +34416,7 @@
     </row>
     <row r="979" spans="1:68">
       <c r="A979" s="3" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="B979" s="5">
         <v>34134.508199999997</v>
@@ -34384,12 +34426,12 @@
       </c>
       <c r="D979" s="20">
         <f t="shared" si="16"/>
-        <v>41.80602006688963</v>
+        <v>41.778074866310163</v>
       </c>
       <c r="E979" s="3">
         <v>625</v>
       </c>
-      <c r="AF979" s="3">
+      <c r="AD979" s="3">
         <v>468.61</v>
       </c>
       <c r="AG979" s="3">
@@ -34401,7 +34443,7 @@
     </row>
     <row r="980" spans="1:68">
       <c r="A980" s="3" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="B980" s="5">
         <v>34499.750400000004</v>
@@ -34411,12 +34453,12 @@
       </c>
       <c r="D980" s="20">
         <f t="shared" si="16"/>
-        <v>41.80602006688963</v>
+        <v>41.778074866310163</v>
       </c>
       <c r="E980" s="3">
         <v>625</v>
       </c>
-      <c r="AF980" s="3">
+      <c r="AD980" s="3">
         <v>495.43</v>
       </c>
       <c r="AG980" s="3">
@@ -34428,7 +34470,7 @@
     </row>
     <row r="981" spans="1:68">
       <c r="A981" s="3" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="B981" s="5">
         <v>34864.992599999998</v>
@@ -34438,12 +34480,12 @@
       </c>
       <c r="D981" s="20">
         <f t="shared" si="16"/>
-        <v>41.80602006688963</v>
+        <v>41.778074866310163</v>
       </c>
       <c r="E981" s="3">
         <v>625</v>
       </c>
-      <c r="AF981" s="3">
+      <c r="AD981" s="3">
         <v>512.85</v>
       </c>
       <c r="AG981" s="3">
@@ -34455,7 +34497,7 @@
     </row>
     <row r="982" spans="1:68">
       <c r="A982" s="3" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="B982" s="5">
         <v>35230.234799999998</v>
@@ -34465,7 +34507,7 @@
       </c>
       <c r="D982" s="20">
         <f t="shared" si="16"/>
-        <v>41.80602006688963</v>
+        <v>41.778074866310163</v>
       </c>
       <c r="E982" s="3">
         <v>625</v>
@@ -34473,7 +34515,7 @@
       <c r="F982" s="3">
         <v>34106</v>
       </c>
-      <c r="I982" s="3">
+      <c r="H982" s="3">
         <v>1071</v>
       </c>
       <c r="K982" s="3">
@@ -34488,10 +34530,13 @@
       <c r="N982" s="3">
         <v>28390</v>
       </c>
+      <c r="V982" s="3">
+        <v>30.543000000000003</v>
+      </c>
       <c r="W982" s="3">
         <v>4924</v>
       </c>
-      <c r="AF982" s="3">
+      <c r="AD982" s="3">
         <v>528.84</v>
       </c>
       <c r="AG982" s="3">

</xml_diff>

<commit_message>
More work on SETRES site
</commit_message>
<xml_diff>
--- a/Prototypes/Pinus/Observed.xlsx
+++ b/Prototypes/Pinus/Observed.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\APSIMxSourceTree\Prototypes\Pinus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B6BB5BB-BEE1-42CB-93F2-BDFF3E26C351}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDF8F4F9-7FBC-46B8-9827-C3A12CF4C9B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" tabRatio="653" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -930,10 +930,10 @@
   <dimension ref="A1:BP982"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D886" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="AF854" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="V982" sqref="V982"/>
+      <selection pane="bottomRight" activeCell="AI858" sqref="AI858:AI894"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="12.75"/>
@@ -30041,7 +30041,7 @@
         <v>0</v>
       </c>
       <c r="E854" s="3">
-        <v>1260</v>
+        <v>1667</v>
       </c>
       <c r="G854" s="6"/>
       <c r="AN854" s="1" t="s">
@@ -30060,7 +30060,7 @@
       </c>
       <c r="D855" s="20">
         <f t="shared" ref="D855:D897" si="15">E855/E$854*100</f>
-        <v>92.393650793650806</v>
+        <v>69.835632873425325</v>
       </c>
       <c r="E855" s="3">
         <v>1164.1600000000001</v>
@@ -30097,7 +30097,7 @@
       </c>
       <c r="D856" s="20">
         <f t="shared" si="15"/>
-        <v>92.392857142857153</v>
+        <v>69.835032993401327</v>
       </c>
       <c r="E856" s="3">
         <v>1164.1500000000001</v>
@@ -30137,7 +30137,7 @@
       </c>
       <c r="D857" s="20">
         <f t="shared" si="15"/>
-        <v>92.257936507936506</v>
+        <v>69.733053389322137</v>
       </c>
       <c r="E857" s="3">
         <v>1162.45</v>
@@ -30177,7 +30177,7 @@
       </c>
       <c r="D858" s="20">
         <f t="shared" si="15"/>
-        <v>91.326190476190476</v>
+        <v>69.028794241151772</v>
       </c>
       <c r="E858" s="3">
         <v>1150.71</v>
@@ -30199,7 +30199,7 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="AJ858" s="3">
-        <v>0.49</v>
+        <v>490</v>
       </c>
       <c r="AK858" s="3">
         <v>9.4999999999999998E-3</v>
@@ -30220,7 +30220,7 @@
       </c>
       <c r="D859" s="20">
         <f t="shared" si="15"/>
-        <v>91.325396825396837</v>
+        <v>69.028194361127788</v>
       </c>
       <c r="E859" s="3">
         <v>1150.7</v>
@@ -30242,7 +30242,7 @@
         <v>10.1</v>
       </c>
       <c r="AJ859" s="3">
-        <v>0.5</v>
+        <v>500</v>
       </c>
       <c r="AK859" s="3">
         <v>9.300000000000001E-3</v>
@@ -30263,7 +30263,7 @@
       </c>
       <c r="D860" s="20">
         <f t="shared" si="15"/>
-        <v>90.381746031746019</v>
+        <v>68.314937012597483</v>
       </c>
       <c r="E860" s="3">
         <v>1138.81</v>
@@ -30285,7 +30285,7 @@
         <v>11.7</v>
       </c>
       <c r="AJ860" s="3">
-        <v>0.53</v>
+        <v>530</v>
       </c>
       <c r="AK860" s="3">
         <v>9.8999999999999991E-3</v>
@@ -30306,7 +30306,7 @@
       </c>
       <c r="D861" s="20">
         <f t="shared" si="15"/>
-        <v>90.381746031746019</v>
+        <v>68.314937012597483</v>
       </c>
       <c r="E861" s="3">
         <v>1138.81</v>
@@ -30346,7 +30346,7 @@
       </c>
       <c r="D862" s="20">
         <f t="shared" si="15"/>
-        <v>89.927777777777777</v>
+        <v>67.971805638872212</v>
       </c>
       <c r="E862" s="3">
         <v>1133.0899999999999</v>
@@ -30386,7 +30386,7 @@
       </c>
       <c r="D863" s="20">
         <f t="shared" si="15"/>
-        <v>89.547619047619037</v>
+        <v>67.684463107378519</v>
       </c>
       <c r="E863" s="3">
         <v>1128.3</v>
@@ -30426,7 +30426,7 @@
       </c>
       <c r="D864" s="20">
         <f t="shared" si="15"/>
-        <v>89.547619047619037</v>
+        <v>67.684463107378519</v>
       </c>
       <c r="E864" s="3">
         <v>1128.3</v>
@@ -30469,7 +30469,7 @@
         <v>100</v>
       </c>
       <c r="E865" s="3">
-        <v>1260</v>
+        <v>1667</v>
       </c>
       <c r="AN865" s="1" t="s">
         <v>35</v>
@@ -30487,7 +30487,7 @@
       </c>
       <c r="D866" s="20">
         <f t="shared" si="15"/>
-        <v>94.30396825396825</v>
+        <v>71.279544091181762</v>
       </c>
       <c r="E866" s="3">
         <v>1188.23</v>
@@ -30523,7 +30523,7 @@
       </c>
       <c r="D867" s="20">
         <f t="shared" si="15"/>
-        <v>94.315873015873024</v>
+        <v>71.288542291541702</v>
       </c>
       <c r="E867" s="3">
         <v>1188.3800000000001</v>
@@ -30562,7 +30562,7 @@
       </c>
       <c r="D868" s="20">
         <f t="shared" si="15"/>
-        <v>94.315079365079356</v>
+        <v>71.28794241151769</v>
       </c>
       <c r="E868" s="3">
         <v>1188.3699999999999</v>
@@ -30601,7 +30601,7 @@
       </c>
       <c r="D869" s="20">
         <f t="shared" si="15"/>
-        <v>93.481746031746027</v>
+        <v>70.658068386322725</v>
       </c>
       <c r="E869" s="3">
         <v>1177.8699999999999</v>
@@ -30622,7 +30622,7 @@
         <v>8.5</v>
       </c>
       <c r="AJ869" s="3">
-        <v>0.5</v>
+        <v>500</v>
       </c>
       <c r="AK869" s="3">
         <v>9.7000000000000003E-3</v>
@@ -30643,7 +30643,7 @@
       </c>
       <c r="D870" s="20">
         <f t="shared" si="15"/>
-        <v>93.248412698412707</v>
+        <v>70.481703659268149</v>
       </c>
       <c r="E870" s="3">
         <v>1174.93</v>
@@ -30664,7 +30664,7 @@
         <v>11</v>
       </c>
       <c r="AJ870" s="3">
-        <v>0.49</v>
+        <v>490</v>
       </c>
       <c r="AK870" s="3">
         <v>1.0500000000000001E-2</v>
@@ -30685,7 +30685,7 @@
       </c>
       <c r="D871" s="20">
         <f t="shared" si="15"/>
-        <v>91.93730158730159</v>
+        <v>69.490701859628075</v>
       </c>
       <c r="E871" s="3">
         <v>1158.4100000000001</v>
@@ -30706,7 +30706,7 @@
         <v>12.9</v>
       </c>
       <c r="AJ871" s="3">
-        <v>0.54</v>
+        <v>540</v>
       </c>
       <c r="AK871" s="3">
         <v>1.06E-2</v>
@@ -30727,7 +30727,7 @@
       </c>
       <c r="D872" s="20">
         <f t="shared" si="15"/>
-        <v>91.715873015873001</v>
+        <v>69.323335332933411</v>
       </c>
       <c r="E872" s="3">
         <v>1155.6199999999999</v>
@@ -30766,7 +30766,7 @@
       </c>
       <c r="D873" s="20">
         <f t="shared" si="15"/>
-        <v>91.017460317460305</v>
+        <v>68.795440911817636</v>
       </c>
       <c r="E873" s="3">
         <v>1146.82</v>
@@ -30805,7 +30805,7 @@
       </c>
       <c r="D874" s="20">
         <f t="shared" si="15"/>
-        <v>90.575396825396822</v>
+        <v>68.461307738452319</v>
       </c>
       <c r="E874" s="3">
         <v>1141.25</v>
@@ -30844,7 +30844,7 @@
       </c>
       <c r="D875" s="20">
         <f t="shared" si="15"/>
-        <v>90.183333333333323</v>
+        <v>68.164967006598673</v>
       </c>
       <c r="E875" s="3">
         <v>1136.31</v>
@@ -30886,7 +30886,7 @@
         <v>100</v>
       </c>
       <c r="E876" s="3">
-        <v>1260</v>
+        <v>1667</v>
       </c>
       <c r="AN876" s="1" t="s">
         <v>35</v>
@@ -30904,7 +30904,7 @@
       </c>
       <c r="D877" s="20">
         <f t="shared" si="15"/>
-        <v>95.075396825396837</v>
+        <v>71.862627474505103</v>
       </c>
       <c r="E877" s="3">
         <v>1197.95</v>
@@ -30940,7 +30940,7 @@
       </c>
       <c r="D878" s="20">
         <f t="shared" si="15"/>
-        <v>94.842063492063488</v>
+        <v>71.686262747450513</v>
       </c>
       <c r="E878" s="3">
         <v>1195.01</v>
@@ -30979,7 +30979,7 @@
       </c>
       <c r="D879" s="20">
         <f t="shared" si="15"/>
-        <v>94.841269841269835</v>
+        <v>71.685662867426515</v>
       </c>
       <c r="E879" s="3">
         <v>1195</v>
@@ -31018,7 +31018,7 @@
       </c>
       <c r="D880" s="20">
         <f t="shared" si="15"/>
-        <v>93.933333333333323</v>
+        <v>70.999400119976002</v>
       </c>
       <c r="E880" s="3">
         <v>1183.56</v>
@@ -31039,7 +31039,7 @@
         <v>13.1</v>
       </c>
       <c r="AJ880" s="3">
-        <v>0.45</v>
+        <v>450</v>
       </c>
       <c r="AK880" s="3">
         <v>1.3100000000000001E-2</v>
@@ -31060,7 +31060,7 @@
       </c>
       <c r="D881" s="20">
         <f t="shared" si="15"/>
-        <v>93.932539682539684</v>
+        <v>70.998800239952004</v>
       </c>
       <c r="E881" s="3">
         <v>1183.55</v>
@@ -31081,7 +31081,7 @@
         <v>17.100000000000001</v>
       </c>
       <c r="AJ881" s="3">
-        <v>0.46</v>
+        <v>460</v>
       </c>
       <c r="AK881" s="3">
         <v>1.24E-2</v>
@@ -31102,7 +31102,7 @@
       </c>
       <c r="D882" s="20">
         <f t="shared" si="15"/>
-        <v>93.098412698412687</v>
+        <v>70.368326334733055</v>
       </c>
       <c r="E882" s="3">
         <v>1173.04</v>
@@ -31123,7 +31123,7 @@
         <v>20.3</v>
       </c>
       <c r="AJ882" s="3">
-        <v>0.49</v>
+        <v>490</v>
       </c>
       <c r="AK882" s="3">
         <v>1.4499999999999999E-2</v>
@@ -31144,7 +31144,7 @@
       </c>
       <c r="D883" s="20">
         <f t="shared" si="15"/>
-        <v>92.619841269841274</v>
+        <v>70.006598680263949</v>
       </c>
       <c r="E883" s="3">
         <v>1167.01</v>
@@ -31183,7 +31183,7 @@
       </c>
       <c r="D884" s="20">
         <f t="shared" si="15"/>
-        <v>92.385714285714286</v>
+        <v>69.82963407318536</v>
       </c>
       <c r="E884" s="3">
         <v>1164.06</v>
@@ -31222,7 +31222,7 @@
       </c>
       <c r="D885" s="20">
         <f t="shared" si="15"/>
-        <v>91.760317460317466</v>
+        <v>69.356928614277152</v>
       </c>
       <c r="E885" s="3">
         <v>1156.18</v>
@@ -31261,7 +31261,7 @@
       </c>
       <c r="D886" s="20">
         <f t="shared" si="15"/>
-        <v>90.865873015873021</v>
+        <v>68.68086382723456</v>
       </c>
       <c r="E886" s="3">
         <v>1144.9100000000001</v>
@@ -31303,7 +31303,7 @@
         <v>100</v>
       </c>
       <c r="E887" s="3">
-        <v>1260</v>
+        <v>1667</v>
       </c>
       <c r="AN887" s="1" t="s">
         <v>35</v>
@@ -31321,7 +31321,7 @@
       </c>
       <c r="D888" s="20">
         <f t="shared" si="15"/>
-        <v>91.487301587301587</v>
+        <v>69.150569886022794</v>
       </c>
       <c r="E888" s="3">
         <v>1152.74</v>
@@ -31357,7 +31357,7 @@
       </c>
       <c r="D889" s="20">
         <f t="shared" si="15"/>
-        <v>91.265873015873026</v>
+        <v>68.983203359328144</v>
       </c>
       <c r="E889" s="3">
         <v>1149.95</v>
@@ -31396,7 +31396,7 @@
       </c>
       <c r="D890" s="20">
         <f t="shared" si="15"/>
-        <v>91.031746031746025</v>
+        <v>68.806238752249556</v>
       </c>
       <c r="E890" s="3">
         <v>1147</v>
@@ -31435,7 +31435,7 @@
       </c>
       <c r="D891" s="20">
         <f t="shared" si="15"/>
-        <v>90.123809523809513</v>
+        <v>68.119976004799028</v>
       </c>
       <c r="E891" s="3">
         <v>1135.56</v>
@@ -31456,7 +31456,7 @@
         <v>13.9</v>
       </c>
       <c r="AJ891" s="3">
-        <v>0.45</v>
+        <v>450</v>
       </c>
       <c r="AK891" s="3">
         <v>1.3000000000000001E-2</v>
@@ -31477,7 +31477,7 @@
       </c>
       <c r="D892" s="20">
         <f t="shared" si="15"/>
-        <v>89.730952380952374</v>
+        <v>67.823035392921412</v>
       </c>
       <c r="E892" s="3">
         <v>1130.6099999999999</v>
@@ -31498,7 +31498,7 @@
         <v>18.3</v>
       </c>
       <c r="AJ892" s="3">
-        <v>0.46</v>
+        <v>460</v>
       </c>
       <c r="AK892" s="3">
         <v>1.1299999999999999E-2</v>
@@ -31519,7 +31519,7 @@
       </c>
       <c r="D893" s="20">
         <f t="shared" si="15"/>
-        <v>88.811111111111103</v>
+        <v>67.127774445110973</v>
       </c>
       <c r="E893" s="3">
         <v>1119.02</v>
@@ -31540,7 +31540,7 @@
         <v>21.7</v>
       </c>
       <c r="AJ893" s="3">
-        <v>0.51</v>
+        <v>510</v>
       </c>
       <c r="AK893" s="3">
         <v>1.3999999999999999E-2</v>
@@ -31561,7 +31561,7 @@
       </c>
       <c r="D894" s="20">
         <f t="shared" si="15"/>
-        <v>88.810317460317449</v>
+        <v>67.127174565086975</v>
       </c>
       <c r="E894" s="3">
         <v>1119.01</v>
@@ -31600,7 +31600,7 @@
       </c>
       <c r="D895" s="20">
         <f t="shared" si="15"/>
-        <v>87.890476190476193</v>
+        <v>66.43191361727655</v>
       </c>
       <c r="E895" s="3">
         <v>1107.42</v>
@@ -31639,7 +31639,7 @@
       </c>
       <c r="D896" s="20">
         <f t="shared" si="15"/>
-        <v>87.876984126984127</v>
+        <v>66.421715656868628</v>
       </c>
       <c r="E896" s="3">
         <v>1107.25</v>
@@ -31678,7 +31678,7 @@
       </c>
       <c r="D897" s="20">
         <f t="shared" si="15"/>
-        <v>87.656349206349205</v>
+        <v>66.254949010197961</v>
       </c>
       <c r="E897" s="3">
         <v>1104.47</v>

</xml_diff>

<commit_message>
Worked on BFG and Puruki sites and Pinus model
</commit_message>
<xml_diff>
--- a/Prototypes/Pinus/Observed.xlsx
+++ b/Prototypes/Pinus/Observed.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\APSIMxSourceTree\Prototypes\Pinus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E31F4BF-70A7-4569-AEC5-24D203ABBDCA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B85D0538-A8CB-42FC-A3F7-1ECDEA1501E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" tabRatio="653" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -366,7 +366,7 @@
     <t>Pinus.Leaf.Live.NConc</t>
   </si>
   <si>
-    <t>PAWmmTotal</t>
+    <t>SWmmTotal</t>
   </si>
 </sst>
 </file>
@@ -960,10 +960,10 @@
   <dimension ref="A1:BO1436"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="AC2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="U2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AL1" sqref="AL1"/>
+      <selection pane="bottomRight" activeCell="Y1" sqref="Y1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="12.75"/>

</xml_diff>

<commit_message>
Worked on SE Qld sites and cultivars
</commit_message>
<xml_diff>
--- a/Prototypes/Pinus/Observed.xlsx
+++ b/Prototypes/Pinus/Observed.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\APSIMxSourceTree\Prototypes\Pinus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47DFB8C7-8076-4026-A7E6-470949AB3D4E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4552B3E-B55C-4F5E-A9BC-2E71EC1F40D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17670" tabRatio="653" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" tabRatio="653" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Observed" sheetId="6" r:id="rId1"/>
@@ -987,49 +987,49 @@
   <dimension ref="A1:BT1438"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="XEG1148" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="AC1146" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A1169" sqref="A1169:A1171"/>
+      <selection pane="bottomRight" activeCell="AC1148" sqref="AC1148:AD1159"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9.26953125" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="9.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" style="3"/>
-    <col min="5" max="5" width="9.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.42578125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="9.28515625" style="3"/>
-    <col min="8" max="8" width="9.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.28515625" style="3"/>
-    <col min="10" max="10" width="9.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="9.28515625" style="3"/>
-    <col min="14" max="14" width="10.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="9.28515625" style="3"/>
-    <col min="17" max="17" width="10.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.28515625" style="3"/>
-    <col min="19" max="19" width="5.28515625" style="3" customWidth="1"/>
-    <col min="20" max="21" width="9.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="9.28515625" style="3"/>
-    <col min="24" max="24" width="14.85546875" style="3" customWidth="1"/>
-    <col min="25" max="25" width="9.28515625" style="3"/>
-    <col min="26" max="26" width="17.28515625" style="3" customWidth="1"/>
-    <col min="27" max="27" width="16.140625" style="3" customWidth="1"/>
-    <col min="28" max="28" width="15.7109375" style="3" customWidth="1"/>
-    <col min="29" max="29" width="17.140625" style="3" customWidth="1"/>
-    <col min="30" max="35" width="23.7109375" style="3" customWidth="1"/>
-    <col min="36" max="41" width="17.7109375" style="3" customWidth="1"/>
-    <col min="42" max="42" width="15.7109375" style="3" customWidth="1"/>
-    <col min="43" max="44" width="25.5703125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="17.7265625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="12.26953125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="9.54296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.26953125" style="3"/>
+    <col min="5" max="5" width="9.54296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.453125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="9.26953125" style="3"/>
+    <col min="8" max="8" width="9.54296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.26953125" style="3"/>
+    <col min="10" max="10" width="9.54296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="9.26953125" style="3"/>
+    <col min="14" max="14" width="10.54296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="9.26953125" style="3"/>
+    <col min="17" max="17" width="10.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.26953125" style="3"/>
+    <col min="19" max="19" width="5.26953125" style="3" customWidth="1"/>
+    <col min="20" max="21" width="9.54296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="9.26953125" style="3"/>
+    <col min="24" max="24" width="14.81640625" style="3" customWidth="1"/>
+    <col min="25" max="25" width="9.26953125" style="3"/>
+    <col min="26" max="26" width="17.26953125" style="3" customWidth="1"/>
+    <col min="27" max="27" width="16.1796875" style="3" customWidth="1"/>
+    <col min="28" max="28" width="15.7265625" style="3" customWidth="1"/>
+    <col min="29" max="29" width="17.1796875" style="3" customWidth="1"/>
+    <col min="30" max="35" width="23.7265625" style="3" customWidth="1"/>
+    <col min="36" max="41" width="17.7265625" style="3" customWidth="1"/>
+    <col min="42" max="42" width="15.7265625" style="3" customWidth="1"/>
+    <col min="43" max="44" width="25.54296875" style="3" customWidth="1"/>
     <col min="45" max="45" width="20" style="3" bestFit="1" customWidth="1"/>
     <col min="46" max="46" width="20" style="3" customWidth="1"/>
-    <col min="47" max="47" width="10.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="48" max="16384" width="9.28515625" style="3"/>
+    <col min="47" max="47" width="10.26953125" style="3" bestFit="1" customWidth="1"/>
+    <col min="48" max="16384" width="9.26953125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:72" ht="33.75">
+    <row r="1" spans="1:72" ht="30">
       <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
@@ -14087,7 +14087,7 @@
       <c r="AS237" s="1"/>
       <c r="AT237" s="1"/>
     </row>
-    <row r="238" spans="1:46" ht="15">
+    <row r="238" spans="1:46" ht="14.5">
       <c r="A238" s="1" t="s">
         <v>4</v>
       </c>
@@ -14123,7 +14123,7 @@
       <c r="AS238" s="9"/>
       <c r="AT238" s="9"/>
     </row>
-    <row r="239" spans="1:46" ht="15">
+    <row r="239" spans="1:46" ht="14.5">
       <c r="A239" s="1" t="s">
         <v>4</v>
       </c>
@@ -14159,7 +14159,7 @@
       <c r="AS239" s="9"/>
       <c r="AT239" s="9"/>
     </row>
-    <row r="240" spans="1:46" ht="15">
+    <row r="240" spans="1:46" ht="14.5">
       <c r="A240" s="1" t="s">
         <v>4</v>
       </c>
@@ -14195,7 +14195,7 @@
       <c r="AS240" s="9"/>
       <c r="AT240" s="9"/>
     </row>
-    <row r="241" spans="1:46" ht="15">
+    <row r="241" spans="1:46" ht="14.5">
       <c r="A241" s="1" t="s">
         <v>4</v>
       </c>
@@ -14236,7 +14236,7 @@
       <c r="AS241" s="9"/>
       <c r="AT241" s="9"/>
     </row>
-    <row r="242" spans="1:46" ht="15">
+    <row r="242" spans="1:46" ht="14.5">
       <c r="A242" s="1" t="s">
         <v>4</v>
       </c>
@@ -14272,7 +14272,7 @@
       <c r="AS242" s="9"/>
       <c r="AT242" s="9"/>
     </row>
-    <row r="243" spans="1:46" ht="15">
+    <row r="243" spans="1:46" ht="14.5">
       <c r="A243" s="1" t="s">
         <v>4</v>
       </c>
@@ -14308,7 +14308,7 @@
       <c r="AS243" s="9"/>
       <c r="AT243" s="9"/>
     </row>
-    <row r="244" spans="1:46" ht="15">
+    <row r="244" spans="1:46" ht="14.5">
       <c r="A244" s="1" t="s">
         <v>4</v>
       </c>
@@ -14344,7 +14344,7 @@
       <c r="AS244" s="9"/>
       <c r="AT244" s="9"/>
     </row>
-    <row r="245" spans="1:46" ht="15">
+    <row r="245" spans="1:46" ht="14.5">
       <c r="A245" s="1" t="s">
         <v>4</v>
       </c>
@@ -14380,7 +14380,7 @@
       <c r="AS245" s="9"/>
       <c r="AT245" s="9"/>
     </row>
-    <row r="246" spans="1:46" ht="15">
+    <row r="246" spans="1:46" ht="14.5">
       <c r="A246" s="1" t="s">
         <v>4</v>
       </c>
@@ -14422,7 +14422,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="247" spans="1:46" ht="15">
+    <row r="247" spans="1:46" ht="14.5">
       <c r="A247" s="1" t="s">
         <v>4</v>
       </c>
@@ -14455,7 +14455,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="248" spans="1:46" ht="15">
+    <row r="248" spans="1:46" ht="14.5">
       <c r="A248" s="1" t="s">
         <v>4</v>
       </c>
@@ -14488,7 +14488,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="249" spans="1:46" ht="15">
+    <row r="249" spans="1:46" ht="14.5">
       <c r="A249" s="1" t="s">
         <v>4</v>
       </c>
@@ -14521,7 +14521,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="250" spans="1:46" ht="15">
+    <row r="250" spans="1:46" ht="14.5">
       <c r="A250" s="1" t="s">
         <v>4</v>
       </c>
@@ -14563,7 +14563,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="251" spans="1:46" ht="15">
+    <row r="251" spans="1:46" ht="14.5">
       <c r="A251" s="1" t="s">
         <v>4</v>
       </c>
@@ -14596,7 +14596,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="252" spans="1:46" ht="15">
+    <row r="252" spans="1:46" ht="14.5">
       <c r="A252" s="1" t="s">
         <v>4</v>
       </c>
@@ -14629,7 +14629,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="253" spans="1:46" ht="15">
+    <row r="253" spans="1:46" ht="14.5">
       <c r="A253" s="1" t="s">
         <v>4</v>
       </c>
@@ -14662,7 +14662,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="254" spans="1:46" ht="15">
+    <row r="254" spans="1:46" ht="14.5">
       <c r="A254" s="1" t="s">
         <v>4</v>
       </c>
@@ -14704,7 +14704,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="255" spans="1:46" ht="15">
+    <row r="255" spans="1:46" ht="14.5">
       <c r="A255" s="1" t="s">
         <v>4</v>
       </c>
@@ -14737,7 +14737,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="256" spans="1:46" ht="15">
+    <row r="256" spans="1:46" ht="14.5">
       <c r="A256" s="1" t="s">
         <v>4</v>
       </c>
@@ -14770,7 +14770,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="257" spans="1:44" ht="15">
+    <row r="257" spans="1:44" ht="14.5">
       <c r="A257" s="1" t="s">
         <v>4</v>
       </c>
@@ -14803,7 +14803,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="258" spans="1:44" ht="15">
+    <row r="258" spans="1:44" ht="14.5">
       <c r="A258" s="1" t="s">
         <v>4</v>
       </c>
@@ -14842,7 +14842,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="259" spans="1:44" ht="15">
+    <row r="259" spans="1:44" ht="14.5">
       <c r="A259" s="1" t="s">
         <v>5</v>
       </c>
@@ -14875,7 +14875,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="260" spans="1:44" ht="15">
+    <row r="260" spans="1:44" ht="14.5">
       <c r="A260" s="1" t="s">
         <v>5</v>
       </c>
@@ -14908,7 +14908,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="261" spans="1:44" ht="15">
+    <row r="261" spans="1:44" ht="14.5">
       <c r="A261" s="1" t="s">
         <v>5</v>
       </c>
@@ -14941,7 +14941,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="262" spans="1:44" ht="15">
+    <row r="262" spans="1:44" ht="14.5">
       <c r="A262" s="1" t="s">
         <v>5</v>
       </c>
@@ -14979,7 +14979,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="263" spans="1:44" ht="15">
+    <row r="263" spans="1:44" ht="14.5">
       <c r="A263" s="1" t="s">
         <v>5</v>
       </c>
@@ -15012,7 +15012,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="264" spans="1:44" ht="15">
+    <row r="264" spans="1:44" ht="14.5">
       <c r="A264" s="1" t="s">
         <v>5</v>
       </c>
@@ -15045,7 +15045,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="265" spans="1:44" ht="15">
+    <row r="265" spans="1:44" ht="14.5">
       <c r="A265" s="1" t="s">
         <v>5</v>
       </c>
@@ -15078,7 +15078,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="266" spans="1:44" ht="15">
+    <row r="266" spans="1:44" ht="14.5">
       <c r="A266" s="1" t="s">
         <v>5</v>
       </c>
@@ -15111,7 +15111,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="267" spans="1:44" ht="15">
+    <row r="267" spans="1:44" ht="14.5">
       <c r="A267" s="1" t="s">
         <v>5</v>
       </c>
@@ -15153,7 +15153,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="268" spans="1:44" ht="15">
+    <row r="268" spans="1:44" ht="14.5">
       <c r="A268" s="1" t="s">
         <v>5</v>
       </c>
@@ -15186,7 +15186,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="269" spans="1:44" ht="15">
+    <row r="269" spans="1:44" ht="14.5">
       <c r="A269" s="1" t="s">
         <v>5</v>
       </c>
@@ -15219,7 +15219,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="270" spans="1:44" ht="15">
+    <row r="270" spans="1:44" ht="14.5">
       <c r="A270" s="1" t="s">
         <v>5</v>
       </c>
@@ -15252,7 +15252,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="271" spans="1:44" ht="15">
+    <row r="271" spans="1:44" ht="14.5">
       <c r="A271" s="1" t="s">
         <v>5</v>
       </c>
@@ -15294,7 +15294,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="272" spans="1:44" ht="15">
+    <row r="272" spans="1:44" ht="14.5">
       <c r="A272" s="1" t="s">
         <v>5</v>
       </c>
@@ -15327,7 +15327,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="273" spans="1:44" ht="15">
+    <row r="273" spans="1:44" ht="14.5">
       <c r="A273" s="1" t="s">
         <v>5</v>
       </c>
@@ -15360,7 +15360,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="274" spans="1:44" ht="15">
+    <row r="274" spans="1:44" ht="14.5">
       <c r="A274" s="1" t="s">
         <v>5</v>
       </c>
@@ -15393,7 +15393,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="275" spans="1:44" ht="15">
+    <row r="275" spans="1:44" ht="14.5">
       <c r="A275" s="1" t="s">
         <v>5</v>
       </c>
@@ -15435,7 +15435,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="276" spans="1:44" ht="15">
+    <row r="276" spans="1:44" ht="14.5">
       <c r="A276" s="1" t="s">
         <v>5</v>
       </c>
@@ -15468,7 +15468,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="277" spans="1:44" ht="15">
+    <row r="277" spans="1:44" ht="14.5">
       <c r="A277" s="1" t="s">
         <v>5</v>
       </c>
@@ -15501,7 +15501,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="278" spans="1:44" ht="15">
+    <row r="278" spans="1:44" ht="14.5">
       <c r="A278" s="1" t="s">
         <v>5</v>
       </c>
@@ -15534,7 +15534,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="279" spans="1:44" ht="15">
+    <row r="279" spans="1:44" ht="14.5">
       <c r="A279" s="1" t="s">
         <v>5</v>
       </c>
@@ -15573,7 +15573,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="280" spans="1:44" ht="15">
+    <row r="280" spans="1:44" ht="14.5">
       <c r="A280" s="1" t="s">
         <v>6</v>
       </c>
@@ -15606,7 +15606,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="281" spans="1:44" ht="15">
+    <row r="281" spans="1:44" ht="14.5">
       <c r="A281" s="1" t="s">
         <v>6</v>
       </c>
@@ -15639,7 +15639,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="282" spans="1:44" ht="15">
+    <row r="282" spans="1:44" ht="14.5">
       <c r="A282" s="1" t="s">
         <v>6</v>
       </c>
@@ -15672,7 +15672,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="283" spans="1:44" ht="15">
+    <row r="283" spans="1:44" ht="14.5">
       <c r="A283" s="1" t="s">
         <v>6</v>
       </c>
@@ -15710,7 +15710,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="284" spans="1:44" ht="15">
+    <row r="284" spans="1:44" ht="14.5">
       <c r="A284" s="1" t="s">
         <v>6</v>
       </c>
@@ -15743,7 +15743,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="285" spans="1:44" ht="15">
+    <row r="285" spans="1:44" ht="14.5">
       <c r="A285" s="1" t="s">
         <v>6</v>
       </c>
@@ -15776,7 +15776,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="286" spans="1:44" ht="15">
+    <row r="286" spans="1:44" ht="14.5">
       <c r="A286" s="1" t="s">
         <v>6</v>
       </c>
@@ -15809,7 +15809,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="287" spans="1:44" ht="15">
+    <row r="287" spans="1:44" ht="14.5">
       <c r="A287" s="1" t="s">
         <v>6</v>
       </c>
@@ -15842,7 +15842,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="288" spans="1:44" ht="15">
+    <row r="288" spans="1:44" ht="14.5">
       <c r="A288" s="1" t="s">
         <v>6</v>
       </c>
@@ -15884,7 +15884,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="289" spans="1:44" ht="15">
+    <row r="289" spans="1:44" ht="14.5">
       <c r="A289" s="1" t="s">
         <v>6</v>
       </c>
@@ -15917,7 +15917,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="290" spans="1:44" ht="15">
+    <row r="290" spans="1:44" ht="14.5">
       <c r="A290" s="1" t="s">
         <v>6</v>
       </c>
@@ -15950,7 +15950,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="291" spans="1:44" ht="15">
+    <row r="291" spans="1:44" ht="14.5">
       <c r="A291" s="1" t="s">
         <v>6</v>
       </c>
@@ -15983,7 +15983,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="292" spans="1:44" ht="15">
+    <row r="292" spans="1:44" ht="14.5">
       <c r="A292" s="1" t="s">
         <v>6</v>
       </c>
@@ -16025,7 +16025,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="293" spans="1:44" ht="15">
+    <row r="293" spans="1:44" ht="14.5">
       <c r="A293" s="1" t="s">
         <v>6</v>
       </c>
@@ -16058,7 +16058,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="294" spans="1:44" ht="15">
+    <row r="294" spans="1:44" ht="14.5">
       <c r="A294" s="1" t="s">
         <v>6</v>
       </c>
@@ -16091,7 +16091,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="295" spans="1:44" ht="15">
+    <row r="295" spans="1:44" ht="14.5">
       <c r="A295" s="1" t="s">
         <v>6</v>
       </c>
@@ -16124,7 +16124,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="296" spans="1:44" ht="15">
+    <row r="296" spans="1:44" ht="14.5">
       <c r="A296" s="1" t="s">
         <v>6</v>
       </c>
@@ -16166,7 +16166,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="297" spans="1:44" ht="15">
+    <row r="297" spans="1:44" ht="14.5">
       <c r="A297" s="1" t="s">
         <v>6</v>
       </c>
@@ -16199,7 +16199,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="298" spans="1:44" ht="15">
+    <row r="298" spans="1:44" ht="14.5">
       <c r="A298" s="1" t="s">
         <v>6</v>
       </c>
@@ -16232,7 +16232,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="299" spans="1:44" ht="15">
+    <row r="299" spans="1:44" ht="14.5">
       <c r="A299" s="1" t="s">
         <v>6</v>
       </c>
@@ -16265,7 +16265,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="300" spans="1:44" ht="15">
+    <row r="300" spans="1:44" ht="14.5">
       <c r="A300" s="1" t="s">
         <v>6</v>
       </c>
@@ -16304,7 +16304,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="301" spans="1:44" ht="15">
+    <row r="301" spans="1:44" ht="14.5">
       <c r="A301" s="1" t="s">
         <v>9</v>
       </c>
@@ -16337,7 +16337,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="302" spans="1:44" ht="15">
+    <row r="302" spans="1:44" ht="14.5">
       <c r="A302" s="1" t="s">
         <v>9</v>
       </c>
@@ -16370,7 +16370,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="303" spans="1:44" ht="15">
+    <row r="303" spans="1:44" ht="14.5">
       <c r="A303" s="1" t="s">
         <v>9</v>
       </c>
@@ -16403,7 +16403,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="304" spans="1:44" ht="15">
+    <row r="304" spans="1:44" ht="14.5">
       <c r="A304" s="1" t="s">
         <v>9</v>
       </c>
@@ -16436,7 +16436,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="305" spans="1:44" ht="15">
+    <row r="305" spans="1:44" ht="14.5">
       <c r="A305" s="1" t="s">
         <v>9</v>
       </c>
@@ -16469,7 +16469,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="306" spans="1:44" ht="15">
+    <row r="306" spans="1:44" ht="14.5">
       <c r="A306" s="1" t="s">
         <v>9</v>
       </c>
@@ -16502,7 +16502,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="307" spans="1:44" ht="15">
+    <row r="307" spans="1:44" ht="14.5">
       <c r="A307" s="1" t="s">
         <v>9</v>
       </c>
@@ -16535,7 +16535,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="308" spans="1:44" ht="15">
+    <row r="308" spans="1:44" ht="14.5">
       <c r="A308" s="1" t="s">
         <v>9</v>
       </c>
@@ -16573,7 +16573,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="309" spans="1:44" ht="15">
+    <row r="309" spans="1:44" ht="14.5">
       <c r="A309" s="1" t="s">
         <v>9</v>
       </c>
@@ -16615,7 +16615,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="310" spans="1:44" ht="15">
+    <row r="310" spans="1:44" ht="14.5">
       <c r="A310" s="1" t="s">
         <v>9</v>
       </c>
@@ -16648,7 +16648,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="311" spans="1:44" ht="15">
+    <row r="311" spans="1:44" ht="14.5">
       <c r="A311" s="1" t="s">
         <v>9</v>
       </c>
@@ -16681,7 +16681,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="312" spans="1:44" ht="15">
+    <row r="312" spans="1:44" ht="14.5">
       <c r="A312" s="1" t="s">
         <v>9</v>
       </c>
@@ -16714,7 +16714,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="313" spans="1:44" ht="15">
+    <row r="313" spans="1:44" ht="14.5">
       <c r="A313" s="1" t="s">
         <v>9</v>
       </c>
@@ -16756,7 +16756,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="314" spans="1:44" ht="15">
+    <row r="314" spans="1:44" ht="14.5">
       <c r="A314" s="1" t="s">
         <v>9</v>
       </c>
@@ -16789,7 +16789,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="315" spans="1:44" ht="15">
+    <row r="315" spans="1:44" ht="14.5">
       <c r="A315" s="1" t="s">
         <v>9</v>
       </c>
@@ -16822,7 +16822,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="316" spans="1:44" ht="15">
+    <row r="316" spans="1:44" ht="14.5">
       <c r="A316" s="1" t="s">
         <v>9</v>
       </c>
@@ -16855,7 +16855,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="317" spans="1:44" ht="15">
+    <row r="317" spans="1:44" ht="14.5">
       <c r="A317" s="1" t="s">
         <v>9</v>
       </c>
@@ -16897,7 +16897,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="318" spans="1:44" ht="15">
+    <row r="318" spans="1:44" ht="14.5">
       <c r="A318" s="1" t="s">
         <v>9</v>
       </c>
@@ -16930,7 +16930,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="319" spans="1:44" ht="15">
+    <row r="319" spans="1:44" ht="14.5">
       <c r="A319" s="1" t="s">
         <v>9</v>
       </c>
@@ -16963,7 +16963,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="320" spans="1:44" ht="15">
+    <row r="320" spans="1:44" ht="14.5">
       <c r="A320" s="1" t="s">
         <v>9</v>
       </c>
@@ -16996,7 +16996,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="321" spans="1:44" ht="15">
+    <row r="321" spans="1:44" ht="14.5">
       <c r="A321" s="1" t="s">
         <v>9</v>
       </c>
@@ -17035,7 +17035,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="322" spans="1:44" ht="15">
+    <row r="322" spans="1:44" ht="14.5">
       <c r="A322" s="1" t="s">
         <v>10</v>
       </c>
@@ -17068,7 +17068,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="323" spans="1:44" ht="15">
+    <row r="323" spans="1:44" ht="14.5">
       <c r="A323" s="1" t="s">
         <v>10</v>
       </c>
@@ -17101,7 +17101,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="324" spans="1:44" ht="15">
+    <row r="324" spans="1:44" ht="14.5">
       <c r="A324" s="1" t="s">
         <v>10</v>
       </c>
@@ -17134,7 +17134,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="325" spans="1:44" ht="15">
+    <row r="325" spans="1:44" ht="14.5">
       <c r="A325" s="1" t="s">
         <v>10</v>
       </c>
@@ -17167,7 +17167,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="326" spans="1:44" ht="15">
+    <row r="326" spans="1:44" ht="14.5">
       <c r="A326" s="1" t="s">
         <v>10</v>
       </c>
@@ -17200,7 +17200,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="327" spans="1:44" ht="15">
+    <row r="327" spans="1:44" ht="14.5">
       <c r="A327" s="1" t="s">
         <v>10</v>
       </c>
@@ -17233,7 +17233,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="328" spans="1:44" ht="15">
+    <row r="328" spans="1:44" ht="14.5">
       <c r="A328" s="1" t="s">
         <v>10</v>
       </c>
@@ -17266,7 +17266,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="329" spans="1:44" ht="15">
+    <row r="329" spans="1:44" ht="14.5">
       <c r="A329" s="1" t="s">
         <v>10</v>
       </c>
@@ -17300,7 +17300,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="330" spans="1:44" ht="15">
+    <row r="330" spans="1:44" ht="14.5">
       <c r="A330" s="1" t="s">
         <v>10</v>
       </c>
@@ -17343,7 +17343,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="331" spans="1:44" ht="15">
+    <row r="331" spans="1:44" ht="14.5">
       <c r="A331" s="1" t="s">
         <v>10</v>
       </c>
@@ -17377,7 +17377,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="332" spans="1:44" ht="15">
+    <row r="332" spans="1:44" ht="14.5">
       <c r="A332" s="1" t="s">
         <v>10</v>
       </c>
@@ -17411,7 +17411,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="333" spans="1:44" ht="15">
+    <row r="333" spans="1:44" ht="14.5">
       <c r="A333" s="1" t="s">
         <v>10</v>
       </c>
@@ -17445,7 +17445,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="334" spans="1:44" ht="15">
+    <row r="334" spans="1:44" ht="14.5">
       <c r="A334" s="1" t="s">
         <v>10</v>
       </c>
@@ -17488,7 +17488,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="335" spans="1:44" ht="15">
+    <row r="335" spans="1:44" ht="14.5">
       <c r="A335" s="1" t="s">
         <v>10</v>
       </c>
@@ -17522,7 +17522,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="336" spans="1:44" ht="15">
+    <row r="336" spans="1:44" ht="14.5">
       <c r="A336" s="1" t="s">
         <v>10</v>
       </c>
@@ -17556,7 +17556,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="337" spans="1:44" ht="15">
+    <row r="337" spans="1:44" ht="14.5">
       <c r="A337" s="1" t="s">
         <v>10</v>
       </c>
@@ -17590,7 +17590,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="338" spans="1:44" ht="15">
+    <row r="338" spans="1:44" ht="14.5">
       <c r="A338" s="1" t="s">
         <v>10</v>
       </c>
@@ -17633,7 +17633,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="339" spans="1:44" ht="15">
+    <row r="339" spans="1:44" ht="14.5">
       <c r="A339" s="1" t="s">
         <v>10</v>
       </c>
@@ -17667,7 +17667,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="340" spans="1:44" ht="15">
+    <row r="340" spans="1:44" ht="14.5">
       <c r="A340" s="1" t="s">
         <v>10</v>
       </c>
@@ -17701,7 +17701,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="341" spans="1:44" ht="15">
+    <row r="341" spans="1:44" ht="14.5">
       <c r="A341" s="1" t="s">
         <v>10</v>
       </c>
@@ -17740,7 +17740,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="342" spans="1:44" ht="15">
+    <row r="342" spans="1:44" ht="14.5">
       <c r="A342" s="1" t="s">
         <v>10</v>
       </c>
@@ -17780,7 +17780,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="343" spans="1:44" ht="15">
+    <row r="343" spans="1:44" ht="14.5">
       <c r="A343" s="1" t="s">
         <v>4</v>
       </c>
@@ -17839,7 +17839,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="344" spans="1:44" ht="15">
+    <row r="344" spans="1:44" ht="14.5">
       <c r="A344" s="1" t="s">
         <v>4</v>
       </c>
@@ -17898,7 +17898,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="345" spans="1:44" ht="15">
+    <row r="345" spans="1:44" ht="14.5">
       <c r="A345" s="1" t="s">
         <v>4</v>
       </c>
@@ -17957,7 +17957,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="346" spans="1:44" ht="15">
+    <row r="346" spans="1:44" ht="14.5">
       <c r="A346" s="1" t="s">
         <v>4</v>
       </c>
@@ -18016,7 +18016,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="347" spans="1:44" ht="15">
+    <row r="347" spans="1:44" ht="14.5">
       <c r="A347" s="1" t="s">
         <v>4</v>
       </c>
@@ -18075,7 +18075,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="348" spans="1:44" ht="15">
+    <row r="348" spans="1:44" ht="14.5">
       <c r="A348" s="1" t="s">
         <v>5</v>
       </c>
@@ -18129,7 +18129,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="349" spans="1:44" ht="15">
+    <row r="349" spans="1:44" ht="14.5">
       <c r="A349" s="1" t="s">
         <v>5</v>
       </c>
@@ -18183,7 +18183,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="350" spans="1:44" ht="15">
+    <row r="350" spans="1:44" ht="14.5">
       <c r="A350" s="1" t="s">
         <v>5</v>
       </c>
@@ -18237,7 +18237,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="351" spans="1:44" ht="15">
+    <row r="351" spans="1:44" ht="14.5">
       <c r="A351" s="1" t="s">
         <v>5</v>
       </c>
@@ -18291,7 +18291,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="352" spans="1:44" ht="15">
+    <row r="352" spans="1:44" ht="14.5">
       <c r="A352" s="1" t="s">
         <v>5</v>
       </c>
@@ -18345,7 +18345,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="353" spans="1:44" ht="15">
+    <row r="353" spans="1:44" ht="14.5">
       <c r="A353" s="1" t="s">
         <v>6</v>
       </c>
@@ -18399,7 +18399,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="354" spans="1:44" ht="15">
+    <row r="354" spans="1:44" ht="14.5">
       <c r="A354" s="1" t="s">
         <v>6</v>
       </c>
@@ -18453,7 +18453,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="355" spans="1:44" ht="15">
+    <row r="355" spans="1:44" ht="14.5">
       <c r="A355" s="1" t="s">
         <v>6</v>
       </c>
@@ -18507,7 +18507,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="356" spans="1:44" ht="15">
+    <row r="356" spans="1:44" ht="14.5">
       <c r="A356" s="1" t="s">
         <v>6</v>
       </c>
@@ -18561,7 +18561,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="357" spans="1:44" ht="15">
+    <row r="357" spans="1:44" ht="14.5">
       <c r="A357" s="1" t="s">
         <v>6</v>
       </c>
@@ -18615,7 +18615,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="358" spans="1:44" ht="15">
+    <row r="358" spans="1:44" ht="14.5">
       <c r="A358" s="1" t="s">
         <v>9</v>
       </c>
@@ -18669,7 +18669,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="359" spans="1:44" ht="15">
+    <row r="359" spans="1:44" ht="14.5">
       <c r="A359" s="1" t="s">
         <v>9</v>
       </c>
@@ -18723,7 +18723,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="360" spans="1:44" ht="15">
+    <row r="360" spans="1:44" ht="14.5">
       <c r="A360" s="1" t="s">
         <v>9</v>
       </c>
@@ -18777,7 +18777,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="361" spans="1:44" ht="15">
+    <row r="361" spans="1:44" ht="14.5">
       <c r="A361" s="1" t="s">
         <v>9</v>
       </c>
@@ -18831,7 +18831,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="362" spans="1:44" ht="15">
+    <row r="362" spans="1:44" ht="14.5">
       <c r="A362" s="1" t="s">
         <v>9</v>
       </c>
@@ -18885,7 +18885,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="363" spans="1:44" ht="15">
+    <row r="363" spans="1:44" ht="14.5">
       <c r="A363" s="1" t="s">
         <v>11</v>
       </c>
@@ -18939,7 +18939,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="364" spans="1:44" ht="15">
+    <row r="364" spans="1:44" ht="14.5">
       <c r="A364" s="1" t="s">
         <v>11</v>
       </c>
@@ -18993,7 +18993,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="365" spans="1:44" ht="15">
+    <row r="365" spans="1:44" ht="14.5">
       <c r="A365" s="1" t="s">
         <v>11</v>
       </c>
@@ -19043,7 +19043,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="366" spans="1:44" ht="15">
+    <row r="366" spans="1:44" ht="14.5">
       <c r="A366" s="1" t="s">
         <v>11</v>
       </c>
@@ -19093,7 +19093,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="367" spans="1:44" ht="15">
+    <row r="367" spans="1:44" ht="14.5">
       <c r="A367" s="1" t="s">
         <v>11</v>
       </c>
@@ -19143,7 +19143,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="368" spans="1:44" ht="15">
+    <row r="368" spans="1:44" ht="14.5">
       <c r="A368" s="1" t="s">
         <v>10</v>
       </c>
@@ -19193,7 +19193,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="369" spans="1:44" ht="15">
+    <row r="369" spans="1:44" ht="14.5">
       <c r="A369" s="1" t="s">
         <v>10</v>
       </c>
@@ -19243,7 +19243,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="370" spans="1:44" ht="15">
+    <row r="370" spans="1:44" ht="14.5">
       <c r="A370" s="1" t="s">
         <v>10</v>
       </c>
@@ -19293,7 +19293,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="371" spans="1:44" ht="15">
+    <row r="371" spans="1:44" ht="14.5">
       <c r="A371" s="1" t="s">
         <v>10</v>
       </c>
@@ -19343,7 +19343,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="372" spans="1:44" ht="15">
+    <row r="372" spans="1:44" ht="14.5">
       <c r="A372" s="1" t="s">
         <v>10</v>
       </c>
@@ -19393,7 +19393,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="373" spans="1:44" ht="15">
+    <row r="373" spans="1:44" ht="14.5">
       <c r="A373" s="1" t="s">
         <v>12</v>
       </c>
@@ -19443,7 +19443,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="374" spans="1:44" ht="15">
+    <row r="374" spans="1:44" ht="14.5">
       <c r="A374" s="1" t="s">
         <v>12</v>
       </c>
@@ -19493,7 +19493,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="375" spans="1:44" ht="15">
+    <row r="375" spans="1:44" ht="14.5">
       <c r="A375" s="1" t="s">
         <v>12</v>
       </c>
@@ -19543,7 +19543,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="376" spans="1:44" ht="15">
+    <row r="376" spans="1:44" ht="14.5">
       <c r="A376" s="1" t="s">
         <v>12</v>
       </c>
@@ -19593,7 +19593,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="377" spans="1:44" ht="15">
+    <row r="377" spans="1:44" ht="14.5">
       <c r="A377" s="1" t="s">
         <v>12</v>
       </c>
@@ -19643,7 +19643,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="378" spans="1:44" ht="15">
+    <row r="378" spans="1:44" ht="14.5">
       <c r="A378" t="s">
         <v>4</v>
       </c>
@@ -19702,7 +19702,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="379" spans="1:44" ht="15">
+    <row r="379" spans="1:44" ht="14.5">
       <c r="A379" t="s">
         <v>4</v>
       </c>
@@ -19761,7 +19761,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="380" spans="1:44" ht="15">
+    <row r="380" spans="1:44" ht="14.5">
       <c r="A380" t="s">
         <v>4</v>
       </c>
@@ -19820,7 +19820,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="381" spans="1:44" ht="15">
+    <row r="381" spans="1:44" ht="14.5">
       <c r="A381" t="s">
         <v>4</v>
       </c>
@@ -19879,7 +19879,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="382" spans="1:44" ht="15">
+    <row r="382" spans="1:44" ht="14.5">
       <c r="A382" t="s">
         <v>4</v>
       </c>
@@ -19938,7 +19938,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="383" spans="1:44" ht="15">
+    <row r="383" spans="1:44" ht="14.5">
       <c r="A383" t="s">
         <v>4</v>
       </c>
@@ -19990,7 +19990,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="384" spans="1:44" ht="15">
+    <row r="384" spans="1:44" ht="14.5">
       <c r="A384" t="s">
         <v>4</v>
       </c>
@@ -20044,7 +20044,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="385" spans="1:44" ht="15">
+    <row r="385" spans="1:44" ht="14.5">
       <c r="A385" t="s">
         <v>4</v>
       </c>
@@ -20105,7 +20105,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="386" spans="1:44" ht="15">
+    <row r="386" spans="1:44" ht="14.5">
       <c r="A386" t="s">
         <v>4</v>
       </c>
@@ -20149,7 +20149,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="387" spans="1:44" ht="15">
+    <row r="387" spans="1:44" ht="14.5">
       <c r="A387" t="s">
         <v>4</v>
       </c>
@@ -20193,7 +20193,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="388" spans="1:44" ht="15">
+    <row r="388" spans="1:44" ht="14.5">
       <c r="A388" t="s">
         <v>4</v>
       </c>
@@ -20237,7 +20237,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="389" spans="1:44" ht="15">
+    <row r="389" spans="1:44" ht="14.5">
       <c r="A389" t="s">
         <v>4</v>
       </c>
@@ -20281,7 +20281,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="390" spans="1:44" ht="15">
+    <row r="390" spans="1:44" ht="14.5">
       <c r="A390" t="s">
         <v>4</v>
       </c>
@@ -20325,7 +20325,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="391" spans="1:44" ht="15">
+    <row r="391" spans="1:44" ht="14.5">
       <c r="A391" t="s">
         <v>4</v>
       </c>
@@ -20369,7 +20369,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="392" spans="1:44" ht="15">
+    <row r="392" spans="1:44" ht="14.5">
       <c r="A392" t="s">
         <v>4</v>
       </c>
@@ -20413,7 +20413,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="393" spans="1:44" ht="15">
+    <row r="393" spans="1:44" ht="14.5">
       <c r="A393" t="s">
         <v>5</v>
       </c>
@@ -20472,7 +20472,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="394" spans="1:44" ht="15">
+    <row r="394" spans="1:44" ht="14.5">
       <c r="A394" t="s">
         <v>5</v>
       </c>
@@ -20531,7 +20531,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="395" spans="1:44" ht="15">
+    <row r="395" spans="1:44" ht="14.5">
       <c r="A395" t="s">
         <v>5</v>
       </c>
@@ -20590,7 +20590,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="396" spans="1:44" ht="15">
+    <row r="396" spans="1:44" ht="14.5">
       <c r="A396" t="s">
         <v>5</v>
       </c>
@@ -20649,7 +20649,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="397" spans="1:44" ht="15">
+    <row r="397" spans="1:44" ht="14.5">
       <c r="A397" t="s">
         <v>5</v>
       </c>
@@ -20708,7 +20708,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="398" spans="1:44" ht="15">
+    <row r="398" spans="1:44" ht="14.5">
       <c r="A398" t="s">
         <v>5</v>
       </c>
@@ -20760,7 +20760,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="399" spans="1:44" ht="15">
+    <row r="399" spans="1:44" ht="14.5">
       <c r="A399" t="s">
         <v>5</v>
       </c>
@@ -20812,7 +20812,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="400" spans="1:44" ht="15">
+    <row r="400" spans="1:44" ht="14.5">
       <c r="A400" t="s">
         <v>5</v>
       </c>
@@ -20866,7 +20866,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="401" spans="1:44" ht="15">
+    <row r="401" spans="1:44" ht="14.5">
       <c r="A401" t="s">
         <v>5</v>
       </c>
@@ -20910,7 +20910,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="402" spans="1:44" ht="15">
+    <row r="402" spans="1:44" ht="14.5">
       <c r="A402" t="s">
         <v>5</v>
       </c>
@@ -20954,7 +20954,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="403" spans="1:44" ht="15">
+    <row r="403" spans="1:44" ht="14.5">
       <c r="A403" t="s">
         <v>5</v>
       </c>
@@ -20998,7 +20998,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="404" spans="1:44" ht="15">
+    <row r="404" spans="1:44" ht="14.5">
       <c r="A404" t="s">
         <v>5</v>
       </c>
@@ -21042,7 +21042,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="405" spans="1:44" ht="15">
+    <row r="405" spans="1:44" ht="14.5">
       <c r="A405" t="s">
         <v>5</v>
       </c>
@@ -21086,7 +21086,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="406" spans="1:44" ht="15">
+    <row r="406" spans="1:44" ht="14.5">
       <c r="A406" t="s">
         <v>5</v>
       </c>
@@ -21130,7 +21130,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="407" spans="1:44" ht="15">
+    <row r="407" spans="1:44" ht="14.5">
       <c r="A407" t="s">
         <v>5</v>
       </c>
@@ -21174,7 +21174,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="408" spans="1:44" ht="15">
+    <row r="408" spans="1:44" ht="14.5">
       <c r="A408" t="s">
         <v>6</v>
       </c>
@@ -21233,7 +21233,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="409" spans="1:44" ht="15">
+    <row r="409" spans="1:44" ht="14.5">
       <c r="A409" t="s">
         <v>6</v>
       </c>
@@ -21292,7 +21292,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="410" spans="1:44" ht="15">
+    <row r="410" spans="1:44" ht="14.5">
       <c r="A410" t="s">
         <v>6</v>
       </c>
@@ -21351,7 +21351,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="411" spans="1:44" ht="15">
+    <row r="411" spans="1:44" ht="14.5">
       <c r="A411" t="s">
         <v>6</v>
       </c>
@@ -21410,7 +21410,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="412" spans="1:44" ht="15">
+    <row r="412" spans="1:44" ht="14.5">
       <c r="A412" t="s">
         <v>6</v>
       </c>
@@ -21469,7 +21469,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="413" spans="1:44" ht="15">
+    <row r="413" spans="1:44" ht="14.5">
       <c r="A413" t="s">
         <v>6</v>
       </c>
@@ -21522,7 +21522,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="414" spans="1:44" ht="15">
+    <row r="414" spans="1:44" ht="14.5">
       <c r="A414" t="s">
         <v>6</v>
       </c>
@@ -21577,7 +21577,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="415" spans="1:44" ht="15">
+    <row r="415" spans="1:44" ht="14.5">
       <c r="A415" t="s">
         <v>6</v>
       </c>
@@ -21638,7 +21638,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="416" spans="1:44" ht="15">
+    <row r="416" spans="1:44" ht="14.5">
       <c r="A416" t="s">
         <v>6</v>
       </c>
@@ -21682,7 +21682,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="417" spans="1:44" ht="15">
+    <row r="417" spans="1:44" ht="14.5">
       <c r="A417" t="s">
         <v>6</v>
       </c>
@@ -21726,7 +21726,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="418" spans="1:44" ht="15">
+    <row r="418" spans="1:44" ht="14.5">
       <c r="A418" t="s">
         <v>6</v>
       </c>
@@ -21770,7 +21770,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="419" spans="1:44" ht="15">
+    <row r="419" spans="1:44" ht="14.5">
       <c r="A419" t="s">
         <v>6</v>
       </c>
@@ -21814,7 +21814,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="420" spans="1:44" ht="15">
+    <row r="420" spans="1:44" ht="14.5">
       <c r="A420" t="s">
         <v>6</v>
       </c>
@@ -21858,7 +21858,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="421" spans="1:44" ht="15">
+    <row r="421" spans="1:44" ht="14.5">
       <c r="A421" t="s">
         <v>6</v>
       </c>
@@ -21902,7 +21902,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="422" spans="1:44" ht="15">
+    <row r="422" spans="1:44" ht="14.5">
       <c r="A422" t="s">
         <v>6</v>
       </c>
@@ -21946,7 +21946,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="423" spans="1:44" ht="15">
+    <row r="423" spans="1:44" ht="14.5">
       <c r="A423" t="s">
         <v>11</v>
       </c>
@@ -22003,7 +22003,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="424" spans="1:44" ht="15">
+    <row r="424" spans="1:44" ht="14.5">
       <c r="A424" t="s">
         <v>11</v>
       </c>
@@ -22060,7 +22060,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="425" spans="1:44" ht="15">
+    <row r="425" spans="1:44" ht="14.5">
       <c r="A425" t="s">
         <v>11</v>
       </c>
@@ -22117,7 +22117,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="426" spans="1:44" ht="15">
+    <row r="426" spans="1:44" ht="14.5">
       <c r="A426" t="s">
         <v>11</v>
       </c>
@@ -22174,7 +22174,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="427" spans="1:44" ht="15">
+    <row r="427" spans="1:44" ht="14.5">
       <c r="A427" t="s">
         <v>11</v>
       </c>
@@ -22231,7 +22231,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="428" spans="1:44" ht="15">
+    <row r="428" spans="1:44" ht="14.5">
       <c r="A428" t="s">
         <v>11</v>
       </c>
@@ -22282,7 +22282,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="429" spans="1:44" ht="15">
+    <row r="429" spans="1:44" ht="14.5">
       <c r="A429" t="s">
         <v>11</v>
       </c>
@@ -22332,7 +22332,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="430" spans="1:44" ht="15">
+    <row r="430" spans="1:44" ht="14.5">
       <c r="A430" t="s">
         <v>11</v>
       </c>
@@ -22384,7 +22384,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="431" spans="1:44" ht="15">
+    <row r="431" spans="1:44" ht="14.5">
       <c r="A431" t="s">
         <v>11</v>
       </c>
@@ -22427,7 +22427,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="432" spans="1:44" ht="15">
+    <row r="432" spans="1:44" ht="14.5">
       <c r="A432" t="s">
         <v>11</v>
       </c>
@@ -22469,7 +22469,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="433" spans="1:44" ht="15">
+    <row r="433" spans="1:44" ht="14.5">
       <c r="A433" t="s">
         <v>11</v>
       </c>
@@ -22511,7 +22511,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="434" spans="1:44" ht="15">
+    <row r="434" spans="1:44" ht="14.5">
       <c r="A434" t="s">
         <v>11</v>
       </c>
@@ -22553,7 +22553,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="435" spans="1:44" ht="15">
+    <row r="435" spans="1:44" ht="14.5">
       <c r="A435" t="s">
         <v>11</v>
       </c>
@@ -22595,7 +22595,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="436" spans="1:44" ht="15">
+    <row r="436" spans="1:44" ht="14.5">
       <c r="A436" t="s">
         <v>11</v>
       </c>
@@ -22637,7 +22637,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="437" spans="1:44" ht="15">
+    <row r="437" spans="1:44" ht="14.5">
       <c r="A437" t="s">
         <v>11</v>
       </c>
@@ -22679,7 +22679,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="438" spans="1:44" ht="15">
+    <row r="438" spans="1:44" ht="14.5">
       <c r="A438" t="s">
         <v>9</v>
       </c>
@@ -22736,7 +22736,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="439" spans="1:44" ht="15">
+    <row r="439" spans="1:44" ht="14.5">
       <c r="A439" t="s">
         <v>9</v>
       </c>
@@ -22793,7 +22793,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="440" spans="1:44" ht="15">
+    <row r="440" spans="1:44" ht="14.5">
       <c r="A440" t="s">
         <v>9</v>
       </c>
@@ -22850,7 +22850,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="441" spans="1:44" ht="15">
+    <row r="441" spans="1:44" ht="14.5">
       <c r="A441" t="s">
         <v>9</v>
       </c>
@@ -22907,7 +22907,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="442" spans="1:44" ht="15">
+    <row r="442" spans="1:44" ht="14.5">
       <c r="A442" t="s">
         <v>9</v>
       </c>
@@ -22964,7 +22964,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="443" spans="1:44" ht="15">
+    <row r="443" spans="1:44" ht="14.5">
       <c r="A443" t="s">
         <v>9</v>
       </c>
@@ -23014,7 +23014,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="444" spans="1:44" ht="15">
+    <row r="444" spans="1:44" ht="14.5">
       <c r="A444" t="s">
         <v>9</v>
       </c>
@@ -23064,7 +23064,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="445" spans="1:44" ht="15">
+    <row r="445" spans="1:44" ht="14.5">
       <c r="A445" t="s">
         <v>9</v>
       </c>
@@ -23114,7 +23114,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="446" spans="1:44" ht="15">
+    <row r="446" spans="1:44" ht="14.5">
       <c r="A446" t="s">
         <v>9</v>
       </c>
@@ -23156,7 +23156,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="447" spans="1:44" ht="15">
+    <row r="447" spans="1:44" ht="14.5">
       <c r="A447" t="s">
         <v>9</v>
       </c>
@@ -23198,7 +23198,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="448" spans="1:44" ht="15">
+    <row r="448" spans="1:44" ht="14.5">
       <c r="A448" t="s">
         <v>9</v>
       </c>
@@ -23240,7 +23240,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="449" spans="1:44" ht="15">
+    <row r="449" spans="1:44" ht="14.5">
       <c r="A449" t="s">
         <v>9</v>
       </c>
@@ -23282,7 +23282,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="450" spans="1:44" ht="15">
+    <row r="450" spans="1:44" ht="14.5">
       <c r="A450" t="s">
         <v>9</v>
       </c>
@@ -23324,7 +23324,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="451" spans="1:44" ht="15">
+    <row r="451" spans="1:44" ht="14.5">
       <c r="A451" t="s">
         <v>9</v>
       </c>
@@ -23366,7 +23366,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="452" spans="1:44" ht="15">
+    <row r="452" spans="1:44" ht="14.5">
       <c r="A452" t="s">
         <v>9</v>
       </c>
@@ -23408,7 +23408,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="453" spans="1:44" ht="15">
+    <row r="453" spans="1:44" ht="14.5">
       <c r="A453" t="s">
         <v>12</v>
       </c>
@@ -23467,7 +23467,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="454" spans="1:44" ht="15">
+    <row r="454" spans="1:44" ht="14.5">
       <c r="A454" t="s">
         <v>12</v>
       </c>
@@ -23526,7 +23526,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="455" spans="1:44" ht="15">
+    <row r="455" spans="1:44" ht="14.5">
       <c r="A455" t="s">
         <v>12</v>
       </c>
@@ -23585,7 +23585,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="456" spans="1:44" ht="15">
+    <row r="456" spans="1:44" ht="14.5">
       <c r="A456" t="s">
         <v>12</v>
       </c>
@@ -23644,7 +23644,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="457" spans="1:44" ht="15">
+    <row r="457" spans="1:44" ht="14.5">
       <c r="A457" t="s">
         <v>12</v>
       </c>
@@ -23703,7 +23703,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="458" spans="1:44" ht="15">
+    <row r="458" spans="1:44" ht="14.5">
       <c r="A458" t="s">
         <v>12</v>
       </c>
@@ -23756,7 +23756,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="459" spans="1:44" ht="15">
+    <row r="459" spans="1:44" ht="14.5">
       <c r="A459" t="s">
         <v>12</v>
       </c>
@@ -23811,7 +23811,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="460" spans="1:44" ht="15">
+    <row r="460" spans="1:44" ht="14.5">
       <c r="A460" t="s">
         <v>12</v>
       </c>
@@ -23872,7 +23872,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="461" spans="1:44" ht="15">
+    <row r="461" spans="1:44" ht="14.5">
       <c r="A461" t="s">
         <v>12</v>
       </c>
@@ -23918,7 +23918,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="462" spans="1:44" ht="15">
+    <row r="462" spans="1:44" ht="14.5">
       <c r="A462" t="s">
         <v>12</v>
       </c>
@@ -23962,7 +23962,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="463" spans="1:44" ht="15">
+    <row r="463" spans="1:44" ht="14.5">
       <c r="A463" t="s">
         <v>12</v>
       </c>
@@ -24006,7 +24006,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="464" spans="1:44" ht="15">
+    <row r="464" spans="1:44" ht="14.5">
       <c r="A464" t="s">
         <v>12</v>
       </c>
@@ -24050,7 +24050,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="465" spans="1:44" ht="15">
+    <row r="465" spans="1:44" ht="14.5">
       <c r="A465" t="s">
         <v>12</v>
       </c>
@@ -24094,7 +24094,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="466" spans="1:44" ht="15">
+    <row r="466" spans="1:44" ht="14.5">
       <c r="A466" t="s">
         <v>12</v>
       </c>
@@ -24138,7 +24138,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="467" spans="1:44" ht="15">
+    <row r="467" spans="1:44" ht="14.5">
       <c r="A467" t="s">
         <v>12</v>
       </c>
@@ -24182,7 +24182,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="468" spans="1:44" ht="15">
+    <row r="468" spans="1:44" ht="14.5">
       <c r="A468" t="s">
         <v>10</v>
       </c>
@@ -24239,7 +24239,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="469" spans="1:44" ht="15">
+    <row r="469" spans="1:44" ht="14.5">
       <c r="A469" t="s">
         <v>10</v>
       </c>
@@ -24296,7 +24296,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="470" spans="1:44" ht="15">
+    <row r="470" spans="1:44" ht="14.5">
       <c r="A470" t="s">
         <v>10</v>
       </c>
@@ -24353,7 +24353,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="471" spans="1:44" ht="15">
+    <row r="471" spans="1:44" ht="14.5">
       <c r="A471" t="s">
         <v>10</v>
       </c>
@@ -24410,7 +24410,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="472" spans="1:44" ht="15">
+    <row r="472" spans="1:44" ht="14.5">
       <c r="A472" t="s">
         <v>10</v>
       </c>
@@ -24467,7 +24467,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="473" spans="1:44" ht="15">
+    <row r="473" spans="1:44" ht="14.5">
       <c r="A473" t="s">
         <v>10</v>
       </c>
@@ -24517,7 +24517,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="474" spans="1:44" ht="15">
+    <row r="474" spans="1:44" ht="14.5">
       <c r="A474" t="s">
         <v>10</v>
       </c>
@@ -24567,7 +24567,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="475" spans="1:44" ht="15">
+    <row r="475" spans="1:44" ht="14.5">
       <c r="A475" t="s">
         <v>10</v>
       </c>
@@ -24616,7 +24616,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="476" spans="1:44" ht="15">
+    <row r="476" spans="1:44" ht="14.5">
       <c r="A476" t="s">
         <v>10</v>
       </c>
@@ -24658,7 +24658,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="477" spans="1:44" ht="15">
+    <row r="477" spans="1:44" ht="14.5">
       <c r="A477" t="s">
         <v>10</v>
       </c>
@@ -24700,7 +24700,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="478" spans="1:44" ht="15">
+    <row r="478" spans="1:44" ht="14.5">
       <c r="A478" t="s">
         <v>10</v>
       </c>
@@ -24742,7 +24742,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="479" spans="1:44" ht="15">
+    <row r="479" spans="1:44" ht="14.5">
       <c r="A479" t="s">
         <v>10</v>
       </c>
@@ -24784,7 +24784,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="480" spans="1:44" ht="15">
+    <row r="480" spans="1:44" ht="14.5">
       <c r="A480" t="s">
         <v>10</v>
       </c>
@@ -24826,7 +24826,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="481" spans="1:44" ht="15">
+    <row r="481" spans="1:44" ht="14.5">
       <c r="A481" t="s">
         <v>10</v>
       </c>
@@ -24868,7 +24868,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="482" spans="1:44" ht="15">
+    <row r="482" spans="1:44" ht="14.5">
       <c r="A482" t="s">
         <v>10</v>
       </c>
@@ -24910,7 +24910,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="483" spans="1:44" ht="15">
+    <row r="483" spans="1:44" ht="14.5">
       <c r="A483" s="1" t="s">
         <v>21</v>
       </c>
@@ -24965,7 +24965,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="484" spans="1:44" ht="15">
+    <row r="484" spans="1:44" ht="14.5">
       <c r="A484" s="1" t="s">
         <v>21</v>
       </c>
@@ -25020,7 +25020,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="485" spans="1:44" ht="15">
+    <row r="485" spans="1:44" ht="14.5">
       <c r="A485" s="1" t="s">
         <v>21</v>
       </c>
@@ -25075,7 +25075,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="486" spans="1:44" ht="15">
+    <row r="486" spans="1:44" ht="14.5">
       <c r="A486" s="1" t="s">
         <v>21</v>
       </c>
@@ -25130,7 +25130,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="487" spans="1:44" ht="15">
+    <row r="487" spans="1:44" ht="14.5">
       <c r="A487" s="1" t="s">
         <v>21</v>
       </c>
@@ -25185,7 +25185,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="488" spans="1:44" ht="15">
+    <row r="488" spans="1:44" ht="14.5">
       <c r="A488" s="1" t="s">
         <v>21</v>
       </c>
@@ -25234,7 +25234,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="489" spans="1:44" ht="15">
+    <row r="489" spans="1:44" ht="14.5">
       <c r="A489" s="1" t="s">
         <v>21</v>
       </c>
@@ -25283,7 +25283,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="490" spans="1:44" ht="15">
+    <row r="490" spans="1:44" ht="14.5">
       <c r="A490" s="1" t="s">
         <v>21</v>
       </c>
@@ -25334,7 +25334,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="491" spans="1:44" ht="15">
+    <row r="491" spans="1:44" ht="14.5">
       <c r="A491" s="1" t="s">
         <v>21</v>
       </c>
@@ -25376,7 +25376,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="492" spans="1:44" ht="15">
+    <row r="492" spans="1:44" ht="14.5">
       <c r="A492" s="1" t="s">
         <v>21</v>
       </c>
@@ -25418,7 +25418,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="493" spans="1:44" ht="15">
+    <row r="493" spans="1:44" ht="14.5">
       <c r="A493" s="1" t="s">
         <v>21</v>
       </c>
@@ -25460,7 +25460,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="494" spans="1:44" ht="15">
+    <row r="494" spans="1:44" ht="14.5">
       <c r="A494" s="1" t="s">
         <v>21</v>
       </c>
@@ -25502,7 +25502,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="495" spans="1:44" ht="15">
+    <row r="495" spans="1:44" ht="14.5">
       <c r="A495" s="1" t="s">
         <v>21</v>
       </c>
@@ -25544,7 +25544,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="496" spans="1:44" ht="15">
+    <row r="496" spans="1:44" ht="14.5">
       <c r="A496" s="1" t="s">
         <v>21</v>
       </c>
@@ -25586,7 +25586,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="497" spans="1:44" ht="15">
+    <row r="497" spans="1:44" ht="14.5">
       <c r="A497" s="1" t="s">
         <v>21</v>
       </c>
@@ -25628,7 +25628,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="498" spans="1:44" ht="15">
+    <row r="498" spans="1:44" ht="14.5">
       <c r="A498" t="s">
         <v>4</v>
       </c>
@@ -25672,7 +25672,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="499" spans="1:44" ht="15">
+    <row r="499" spans="1:44" ht="14.5">
       <c r="A499" t="s">
         <v>4</v>
       </c>
@@ -25716,7 +25716,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="500" spans="1:44" ht="15">
+    <row r="500" spans="1:44" ht="14.5">
       <c r="A500" t="s">
         <v>4</v>
       </c>
@@ -25760,7 +25760,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="501" spans="1:44" ht="15">
+    <row r="501" spans="1:44" ht="14.5">
       <c r="A501" t="s">
         <v>4</v>
       </c>
@@ -25804,7 +25804,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="502" spans="1:44" ht="15">
+    <row r="502" spans="1:44" ht="14.5">
       <c r="A502" t="s">
         <v>5</v>
       </c>
@@ -25848,7 +25848,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="503" spans="1:44" ht="15">
+    <row r="503" spans="1:44" ht="14.5">
       <c r="A503" t="s">
         <v>5</v>
       </c>
@@ -25892,7 +25892,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="504" spans="1:44" ht="15">
+    <row r="504" spans="1:44" ht="14.5">
       <c r="A504" t="s">
         <v>5</v>
       </c>
@@ -25936,7 +25936,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="505" spans="1:44" ht="15">
+    <row r="505" spans="1:44" ht="14.5">
       <c r="A505" t="s">
         <v>5</v>
       </c>
@@ -25980,7 +25980,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="506" spans="1:44" ht="15">
+    <row r="506" spans="1:44" ht="14.5">
       <c r="A506" t="s">
         <v>6</v>
       </c>
@@ -26024,7 +26024,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="507" spans="1:44" ht="15">
+    <row r="507" spans="1:44" ht="14.5">
       <c r="A507" t="s">
         <v>6</v>
       </c>
@@ -26068,7 +26068,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="508" spans="1:44" ht="15">
+    <row r="508" spans="1:44" ht="14.5">
       <c r="A508" t="s">
         <v>6</v>
       </c>
@@ -26112,7 +26112,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="509" spans="1:44" ht="15">
+    <row r="509" spans="1:44" ht="14.5">
       <c r="A509" t="s">
         <v>6</v>
       </c>
@@ -26156,7 +26156,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="510" spans="1:44" ht="15">
+    <row r="510" spans="1:44" ht="14.5">
       <c r="A510" t="s">
         <v>11</v>
       </c>
@@ -26200,7 +26200,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="511" spans="1:44" ht="15">
+    <row r="511" spans="1:44" ht="14.5">
       <c r="A511" t="s">
         <v>11</v>
       </c>
@@ -26244,7 +26244,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="512" spans="1:44" ht="15">
+    <row r="512" spans="1:44" ht="14.5">
       <c r="A512" t="s">
         <v>11</v>
       </c>
@@ -26288,7 +26288,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="513" spans="1:45" ht="15">
+    <row r="513" spans="1:45" ht="14.5">
       <c r="A513" t="s">
         <v>11</v>
       </c>
@@ -26332,7 +26332,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="514" spans="1:45" ht="15">
+    <row r="514" spans="1:45" ht="14.5">
       <c r="A514" t="s">
         <v>9</v>
       </c>
@@ -26376,7 +26376,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="515" spans="1:45" ht="15">
+    <row r="515" spans="1:45" ht="14.5">
       <c r="A515" t="s">
         <v>9</v>
       </c>
@@ -26420,7 +26420,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="516" spans="1:45" ht="15">
+    <row r="516" spans="1:45" ht="14.5">
       <c r="A516" t="s">
         <v>9</v>
       </c>
@@ -26464,7 +26464,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="517" spans="1:45" ht="15">
+    <row r="517" spans="1:45" ht="14.5">
       <c r="A517" t="s">
         <v>9</v>
       </c>
@@ -26508,7 +26508,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="518" spans="1:45" ht="15">
+    <row r="518" spans="1:45" ht="14.5">
       <c r="A518" t="s">
         <v>12</v>
       </c>
@@ -26552,7 +26552,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="519" spans="1:45" ht="15">
+    <row r="519" spans="1:45" ht="14.5">
       <c r="A519" t="s">
         <v>12</v>
       </c>
@@ -26596,7 +26596,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="520" spans="1:45" ht="15">
+    <row r="520" spans="1:45" ht="14.5">
       <c r="A520" t="s">
         <v>12</v>
       </c>
@@ -26640,7 +26640,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="521" spans="1:45" ht="15">
+    <row r="521" spans="1:45" ht="14.5">
       <c r="A521" t="s">
         <v>12</v>
       </c>
@@ -26684,7 +26684,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="522" spans="1:45" ht="15">
+    <row r="522" spans="1:45" ht="14.5">
       <c r="A522" t="s">
         <v>10</v>
       </c>
@@ -26728,7 +26728,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="523" spans="1:45" ht="15">
+    <row r="523" spans="1:45" ht="14.5">
       <c r="A523" t="s">
         <v>10</v>
       </c>
@@ -26773,7 +26773,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="524" spans="1:45" ht="15">
+    <row r="524" spans="1:45" ht="14.5">
       <c r="A524" t="s">
         <v>10</v>
       </c>
@@ -26818,7 +26818,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="525" spans="1:45" ht="15">
+    <row r="525" spans="1:45" ht="14.5">
       <c r="A525" t="s">
         <v>10</v>
       </c>
@@ -26863,7 +26863,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="526" spans="1:45" ht="15">
+    <row r="526" spans="1:45" ht="14.5">
       <c r="A526" s="1" t="s">
         <v>4</v>
       </c>
@@ -26911,7 +26911,7 @@
         <v>273.82</v>
       </c>
     </row>
-    <row r="527" spans="1:45" ht="15">
+    <row r="527" spans="1:45" ht="14.5">
       <c r="A527" s="1" t="s">
         <v>4</v>
       </c>
@@ -26959,7 +26959,7 @@
         <v>268.62</v>
       </c>
     </row>
-    <row r="528" spans="1:45" ht="15">
+    <row r="528" spans="1:45" ht="14.5">
       <c r="A528" s="1" t="s">
         <v>4</v>
       </c>
@@ -27007,7 +27007,7 @@
         <v>269.58999999999997</v>
       </c>
     </row>
-    <row r="529" spans="1:45" ht="15">
+    <row r="529" spans="1:45" ht="14.5">
       <c r="A529" s="1" t="s">
         <v>4</v>
       </c>
@@ -27055,7 +27055,7 @@
         <v>329.11</v>
       </c>
     </row>
-    <row r="530" spans="1:45" ht="15">
+    <row r="530" spans="1:45" ht="14.5">
       <c r="A530" s="1" t="s">
         <v>4</v>
       </c>
@@ -27103,7 +27103,7 @@
         <v>347.97</v>
       </c>
     </row>
-    <row r="531" spans="1:45" ht="15">
+    <row r="531" spans="1:45" ht="14.5">
       <c r="A531" s="1" t="s">
         <v>4</v>
       </c>
@@ -27151,7 +27151,7 @@
         <v>365.53</v>
       </c>
     </row>
-    <row r="532" spans="1:45" ht="15">
+    <row r="532" spans="1:45" ht="14.5">
       <c r="A532" s="1" t="s">
         <v>4</v>
       </c>
@@ -27199,7 +27199,7 @@
         <v>366.18</v>
       </c>
     </row>
-    <row r="533" spans="1:45" ht="15">
+    <row r="533" spans="1:45" ht="14.5">
       <c r="A533" s="1" t="s">
         <v>4</v>
       </c>
@@ -27247,7 +27247,7 @@
         <v>367.15</v>
       </c>
     </row>
-    <row r="534" spans="1:45" ht="15">
+    <row r="534" spans="1:45" ht="14.5">
       <c r="A534" s="1" t="s">
         <v>4</v>
       </c>
@@ -27295,7 +27295,7 @@
         <v>333.33</v>
       </c>
     </row>
-    <row r="535" spans="1:45" ht="15">
+    <row r="535" spans="1:45" ht="14.5">
       <c r="A535" s="1" t="s">
         <v>4</v>
       </c>
@@ -27343,7 +27343,7 @@
         <v>293.98</v>
       </c>
     </row>
-    <row r="536" spans="1:45" ht="15">
+    <row r="536" spans="1:45" ht="14.5">
       <c r="A536" s="1" t="s">
         <v>4</v>
       </c>
@@ -27391,7 +27391,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="537" spans="1:45" ht="15">
+    <row r="537" spans="1:45" ht="14.5">
       <c r="A537" s="1" t="s">
         <v>4</v>
       </c>
@@ -27439,7 +27439,7 @@
         <v>246.5</v>
       </c>
     </row>
-    <row r="538" spans="1:45" ht="15">
+    <row r="538" spans="1:45" ht="14.5">
       <c r="A538" s="1" t="s">
         <v>4</v>
       </c>
@@ -27487,7 +27487,7 @@
         <v>220.49</v>
       </c>
     </row>
-    <row r="539" spans="1:45" ht="15">
+    <row r="539" spans="1:45" ht="14.5">
       <c r="A539" s="1" t="s">
         <v>4</v>
       </c>
@@ -27535,7 +27535,7 @@
         <v>202.6</v>
       </c>
     </row>
-    <row r="540" spans="1:45" ht="15">
+    <row r="540" spans="1:45" ht="14.5">
       <c r="A540" s="1" t="s">
         <v>4</v>
       </c>
@@ -27583,7 +27583,7 @@
         <v>189.92</v>
       </c>
     </row>
-    <row r="541" spans="1:45" ht="15">
+    <row r="541" spans="1:45" ht="14.5">
       <c r="A541" s="1" t="s">
         <v>4</v>
       </c>
@@ -27631,7 +27631,7 @@
         <v>175.61</v>
       </c>
     </row>
-    <row r="542" spans="1:45" ht="15">
+    <row r="542" spans="1:45" ht="14.5">
       <c r="A542" s="1" t="s">
         <v>4</v>
       </c>
@@ -27679,7 +27679,7 @@
         <v>171.38</v>
       </c>
     </row>
-    <row r="543" spans="1:45" ht="15">
+    <row r="543" spans="1:45" ht="14.5">
       <c r="A543" s="1" t="s">
         <v>4</v>
       </c>
@@ -27727,7 +27727,7 @@
         <v>163.58000000000001</v>
       </c>
     </row>
-    <row r="544" spans="1:45" ht="15">
+    <row r="544" spans="1:45" ht="14.5">
       <c r="A544" s="1" t="s">
         <v>4</v>
       </c>
@@ -27775,7 +27775,7 @@
         <v>155.12</v>
       </c>
     </row>
-    <row r="545" spans="1:45" ht="15">
+    <row r="545" spans="1:45" ht="14.5">
       <c r="A545" s="1" t="s">
         <v>4</v>
       </c>
@@ -27823,7 +27823,7 @@
         <v>158.05000000000001</v>
       </c>
     </row>
-    <row r="546" spans="1:45" ht="15">
+    <row r="546" spans="1:45" ht="14.5">
       <c r="A546" s="1" t="s">
         <v>4</v>
       </c>
@@ -27871,7 +27871,7 @@
         <v>284.55</v>
       </c>
     </row>
-    <row r="547" spans="1:45" ht="15">
+    <row r="547" spans="1:45" ht="14.5">
       <c r="A547" s="1" t="s">
         <v>4</v>
       </c>
@@ -27919,7 +27919,7 @@
         <v>278.7</v>
       </c>
     </row>
-    <row r="548" spans="1:45" ht="15">
+    <row r="548" spans="1:45" ht="14.5">
       <c r="A548" s="1" t="s">
         <v>4</v>
       </c>
@@ -27967,7 +27967,7 @@
         <v>248.13</v>
       </c>
     </row>
-    <row r="549" spans="1:45" ht="15">
+    <row r="549" spans="1:45" ht="14.5">
       <c r="A549" s="1" t="s">
         <v>4</v>
       </c>
@@ -28015,7 +28015,7 @@
         <v>230.24</v>
       </c>
     </row>
-    <row r="550" spans="1:45" ht="15">
+    <row r="550" spans="1:45" ht="14.5">
       <c r="A550" s="1" t="s">
         <v>4</v>
       </c>
@@ -28063,7 +28063,7 @@
         <v>218.54</v>
       </c>
     </row>
-    <row r="551" spans="1:45" ht="15">
+    <row r="551" spans="1:45" ht="14.5">
       <c r="A551" s="1" t="s">
         <v>4</v>
       </c>
@@ -28111,7 +28111,7 @@
         <v>216.59</v>
       </c>
     </row>
-    <row r="552" spans="1:45" ht="15">
+    <row r="552" spans="1:45" ht="14.5">
       <c r="A552" s="1" t="s">
         <v>4</v>
       </c>
@@ -28159,7 +28159,7 @@
         <v>216.59</v>
       </c>
     </row>
-    <row r="553" spans="1:45" ht="15">
+    <row r="553" spans="1:45" ht="14.5">
       <c r="A553" s="1" t="s">
         <v>4</v>
       </c>
@@ -28207,7 +28207,7 @@
         <v>219.84</v>
       </c>
     </row>
-    <row r="554" spans="1:45" ht="15">
+    <row r="554" spans="1:45" ht="14.5">
       <c r="A554" s="1" t="s">
         <v>4</v>
       </c>
@@ -28255,7 +28255,7 @@
         <v>214.63</v>
       </c>
     </row>
-    <row r="555" spans="1:45" ht="15">
+    <row r="555" spans="1:45" ht="14.5">
       <c r="A555" s="1" t="s">
         <v>4</v>
       </c>
@@ -28303,7 +28303,7 @@
         <v>230.57</v>
       </c>
     </row>
-    <row r="556" spans="1:45" ht="15">
+    <row r="556" spans="1:45" ht="14.5">
       <c r="A556" s="1" t="s">
         <v>4</v>
       </c>
@@ -28351,7 +28351,7 @@
         <v>220.81</v>
       </c>
     </row>
-    <row r="557" spans="1:45" ht="15">
+    <row r="557" spans="1:45" ht="14.5">
       <c r="A557" s="1" t="s">
         <v>4</v>
       </c>
@@ -28399,7 +28399,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="558" spans="1:45" ht="15">
+    <row r="558" spans="1:45" ht="14.5">
       <c r="A558" s="1" t="s">
         <v>4</v>
       </c>
@@ -28447,7 +28447,7 @@
         <v>300.49</v>
       </c>
     </row>
-    <row r="559" spans="1:45" ht="15">
+    <row r="559" spans="1:45" ht="14.5">
       <c r="A559" s="1" t="s">
         <v>4</v>
       </c>
@@ -28495,7 +28495,7 @@
         <v>287.8</v>
       </c>
     </row>
-    <row r="560" spans="1:45" ht="15">
+    <row r="560" spans="1:45" ht="14.5">
       <c r="A560" s="1" t="s">
         <v>4</v>
       </c>
@@ -28543,7 +28543,7 @@
         <v>318.7</v>
       </c>
     </row>
-    <row r="561" spans="1:45" ht="15">
+    <row r="561" spans="1:45" ht="14.5">
       <c r="A561" s="1" t="s">
         <v>4</v>
       </c>
@@ -28591,7 +28591,7 @@
         <v>284.88</v>
       </c>
     </row>
-    <row r="562" spans="1:45" ht="15">
+    <row r="562" spans="1:45" ht="14.5">
       <c r="A562" s="1" t="s">
         <v>4</v>
       </c>
@@ -28639,7 +28639,7 @@
         <v>274.8</v>
       </c>
     </row>
-    <row r="563" spans="1:45" ht="15">
+    <row r="563" spans="1:45" ht="14.5">
       <c r="A563" s="1" t="s">
         <v>4</v>
       </c>
@@ -28687,7 +28687,7 @@
         <v>251.06</v>
       </c>
     </row>
-    <row r="564" spans="1:45" ht="15">
+    <row r="564" spans="1:45" ht="14.5">
       <c r="A564" s="1" t="s">
         <v>4</v>
       </c>
@@ -28735,7 +28735,7 @@
         <v>237.4</v>
       </c>
     </row>
-    <row r="565" spans="1:45" ht="15">
+    <row r="565" spans="1:45" ht="14.5">
       <c r="A565" s="1" t="s">
         <v>4</v>
       </c>
@@ -28783,7 +28783,7 @@
         <v>230.89</v>
       </c>
     </row>
-    <row r="566" spans="1:45" ht="15">
+    <row r="566" spans="1:45" ht="14.5">
       <c r="A566" s="1" t="s">
         <v>4</v>
       </c>
@@ -28831,7 +28831,7 @@
         <v>189.92</v>
       </c>
     </row>
-    <row r="567" spans="1:45" ht="15">
+    <row r="567" spans="1:45" ht="14.5">
       <c r="A567" s="1" t="s">
         <v>4</v>
       </c>
@@ -28879,7 +28879,7 @@
         <v>180.16</v>
       </c>
     </row>
-    <row r="568" spans="1:45" ht="15">
+    <row r="568" spans="1:45" ht="14.5">
       <c r="A568" s="1" t="s">
         <v>4</v>
       </c>
@@ -28927,7 +28927,7 @@
         <v>181.79</v>
       </c>
     </row>
-    <row r="569" spans="1:45" ht="15">
+    <row r="569" spans="1:45" ht="14.5">
       <c r="A569" s="1" t="s">
         <v>4</v>
       </c>
@@ -28975,7 +28975,7 @@
         <v>169.11</v>
       </c>
     </row>
-    <row r="570" spans="1:45" ht="15">
+    <row r="570" spans="1:45" ht="14.5">
       <c r="A570" s="1" t="s">
         <v>4</v>
       </c>
@@ -29023,7 +29023,7 @@
         <v>167.8</v>
       </c>
     </row>
-    <row r="571" spans="1:45" ht="15">
+    <row r="571" spans="1:45" ht="14.5">
       <c r="A571" s="1" t="s">
         <v>4</v>
       </c>
@@ -29071,7 +29071,7 @@
         <v>159.02000000000001</v>
       </c>
     </row>
-    <row r="572" spans="1:45" ht="15">
+    <row r="572" spans="1:45" ht="14.5">
       <c r="A572" s="1" t="s">
         <v>4</v>
       </c>
@@ -29119,7 +29119,7 @@
         <v>148.29</v>
       </c>
     </row>
-    <row r="573" spans="1:45" ht="15">
+    <row r="573" spans="1:45" ht="14.5">
       <c r="A573" s="1" t="s">
         <v>4</v>
       </c>
@@ -29167,7 +29167,7 @@
         <v>150.24</v>
       </c>
     </row>
-    <row r="574" spans="1:45" ht="15">
+    <row r="574" spans="1:45" ht="14.5">
       <c r="A574" s="1" t="s">
         <v>4</v>
       </c>
@@ -29215,7 +29215,7 @@
         <v>155.77000000000001</v>
       </c>
     </row>
-    <row r="575" spans="1:45" ht="15">
+    <row r="575" spans="1:45" ht="14.5">
       <c r="A575" s="1" t="s">
         <v>4</v>
       </c>
@@ -29263,7 +29263,7 @@
         <v>189.92</v>
       </c>
     </row>
-    <row r="576" spans="1:45" ht="15">
+    <row r="576" spans="1:45" ht="14.5">
       <c r="A576" s="1" t="s">
         <v>4</v>
       </c>
@@ -29311,7 +29311,7 @@
         <v>206.18</v>
       </c>
     </row>
-    <row r="577" spans="1:45" ht="15">
+    <row r="577" spans="1:45" ht="14.5">
       <c r="A577" s="1" t="s">
         <v>4</v>
       </c>
@@ -29359,7 +29359,7 @@
         <v>217.56</v>
       </c>
     </row>
-    <row r="578" spans="1:45" ht="15">
+    <row r="578" spans="1:45" ht="14.5">
       <c r="A578" s="1" t="s">
         <v>4</v>
       </c>
@@ -29407,7 +29407,7 @@
         <v>209.76</v>
       </c>
     </row>
-    <row r="579" spans="1:45" ht="15">
+    <row r="579" spans="1:45" ht="14.5">
       <c r="A579" s="1" t="s">
         <v>4</v>
       </c>
@@ -29455,7 +29455,7 @@
         <v>196.75</v>
       </c>
     </row>
-    <row r="580" spans="1:45" ht="15">
+    <row r="580" spans="1:45" ht="14.5">
       <c r="A580" s="1" t="s">
         <v>4</v>
       </c>
@@ -29503,7 +29503,7 @@
         <v>249.76</v>
       </c>
     </row>
-    <row r="581" spans="1:45" ht="15">
+    <row r="581" spans="1:45" ht="14.5">
       <c r="A581" s="1" t="s">
         <v>4</v>
       </c>
@@ -29551,7 +29551,7 @@
         <v>295.27999999999997</v>
       </c>
     </row>
-    <row r="582" spans="1:45" ht="15">
+    <row r="582" spans="1:45" ht="14.5">
       <c r="A582" s="1" t="s">
         <v>4</v>
       </c>
@@ -29599,7 +29599,7 @@
         <v>276.75</v>
       </c>
     </row>
-    <row r="583" spans="1:45" ht="15">
+    <row r="583" spans="1:45" ht="14.5">
       <c r="A583" s="1" t="s">
         <v>4</v>
       </c>
@@ -29647,7 +29647,7 @@
         <v>296.26</v>
       </c>
     </row>
-    <row r="584" spans="1:45" ht="15">
+    <row r="584" spans="1:45" ht="14.5">
       <c r="A584" s="1" t="s">
         <v>4</v>
       </c>
@@ -29695,7 +29695,7 @@
         <v>273.5</v>
       </c>
     </row>
-    <row r="585" spans="1:45" ht="15">
+    <row r="585" spans="1:45" ht="14.5">
       <c r="A585" s="1" t="s">
         <v>4</v>
       </c>
@@ -29743,7 +29743,7 @@
         <v>269.58999999999997</v>
       </c>
     </row>
-    <row r="586" spans="1:45" ht="15">
+    <row r="586" spans="1:45" ht="14.5">
       <c r="A586" s="1" t="s">
         <v>4</v>
       </c>
@@ -29791,7 +29791,7 @@
         <v>256.91000000000003</v>
       </c>
     </row>
-    <row r="587" spans="1:45" ht="15">
+    <row r="587" spans="1:45" ht="14.5">
       <c r="A587" s="1" t="s">
         <v>4</v>
       </c>
@@ -29839,7 +29839,7 @@
         <v>270.89</v>
       </c>
     </row>
-    <row r="588" spans="1:45" ht="15">
+    <row r="588" spans="1:45" ht="14.5">
       <c r="A588" s="1" t="s">
         <v>4</v>
       </c>
@@ -29887,7 +29887,7 @@
         <v>239.02</v>
       </c>
     </row>
-    <row r="589" spans="1:45" ht="15">
+    <row r="589" spans="1:45" ht="14.5">
       <c r="A589" s="1" t="s">
         <v>4</v>
       </c>
@@ -29935,7 +29935,7 @@
         <v>249.11</v>
       </c>
     </row>
-    <row r="590" spans="1:45" ht="15">
+    <row r="590" spans="1:45" ht="14.5">
       <c r="A590" s="1" t="s">
         <v>4</v>
       </c>
@@ -29983,7 +29983,7 @@
         <v>222.11</v>
       </c>
     </row>
-    <row r="591" spans="1:45" ht="15">
+    <row r="591" spans="1:45" ht="14.5">
       <c r="A591" s="1" t="s">
         <v>4</v>
       </c>
@@ -30031,7 +30031,7 @@
         <v>211.38</v>
       </c>
     </row>
-    <row r="592" spans="1:45" ht="15">
+    <row r="592" spans="1:45" ht="14.5">
       <c r="A592" s="1" t="s">
         <v>4</v>
       </c>
@@ -30079,7 +30079,7 @@
         <v>183.09</v>
       </c>
     </row>
-    <row r="593" spans="1:45" ht="15">
+    <row r="593" spans="1:45" ht="14.5">
       <c r="A593" s="1" t="s">
         <v>4</v>
       </c>
@@ -30127,7 +30127,7 @@
         <v>175.61</v>
       </c>
     </row>
-    <row r="594" spans="1:45" ht="15">
+    <row r="594" spans="1:45" ht="14.5">
       <c r="A594" s="1" t="s">
         <v>4</v>
       </c>
@@ -30175,7 +30175,7 @@
         <v>159.66999999999999</v>
       </c>
     </row>
-    <row r="595" spans="1:45" ht="15">
+    <row r="595" spans="1:45" ht="14.5">
       <c r="A595" s="1" t="s">
         <v>4</v>
       </c>
@@ -30223,7 +30223,7 @@
         <v>172.36</v>
       </c>
     </row>
-    <row r="596" spans="1:45" ht="15">
+    <row r="596" spans="1:45" ht="14.5">
       <c r="A596" s="1" t="s">
         <v>4</v>
       </c>
@@ -30271,7 +30271,7 @@
         <v>165.2</v>
       </c>
     </row>
-    <row r="597" spans="1:45" ht="15">
+    <row r="597" spans="1:45" ht="14.5">
       <c r="A597" s="1" t="s">
         <v>4</v>
       </c>
@@ -30319,7 +30319,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="598" spans="1:45" ht="15">
+    <row r="598" spans="1:45" ht="14.5">
       <c r="A598" s="1" t="s">
         <v>4</v>
       </c>
@@ -30367,7 +30367,7 @@
         <v>150.57</v>
       </c>
     </row>
-    <row r="599" spans="1:45" ht="15">
+    <row r="599" spans="1:45" ht="14.5">
       <c r="A599" s="1" t="s">
         <v>4</v>
       </c>
@@ -30415,7 +30415,7 @@
         <v>151.87</v>
       </c>
     </row>
-    <row r="600" spans="1:45" ht="15">
+    <row r="600" spans="1:45" ht="14.5">
       <c r="A600" s="1" t="s">
         <v>4</v>
       </c>
@@ -30463,7 +30463,7 @@
         <v>157.72</v>
       </c>
     </row>
-    <row r="601" spans="1:45" ht="15">
+    <row r="601" spans="1:45" ht="14.5">
       <c r="A601" s="1" t="s">
         <v>4</v>
       </c>
@@ -30511,7 +30511,7 @@
         <v>164.55</v>
       </c>
     </row>
-    <row r="602" spans="1:45" ht="15">
+    <row r="602" spans="1:45" ht="14.5">
       <c r="A602" s="1" t="s">
         <v>4</v>
       </c>
@@ -30559,7 +30559,7 @@
         <v>161.63</v>
       </c>
     </row>
-    <row r="603" spans="1:45" ht="15">
+    <row r="603" spans="1:45" ht="14.5">
       <c r="A603" s="1" t="s">
         <v>4</v>
       </c>
@@ -30607,7 +30607,7 @@
         <v>186.67</v>
       </c>
     </row>
-    <row r="604" spans="1:45" ht="15">
+    <row r="604" spans="1:45" ht="14.5">
       <c r="A604" s="1" t="s">
         <v>4</v>
       </c>
@@ -30655,7 +30655,7 @@
         <v>185.37</v>
       </c>
     </row>
-    <row r="605" spans="1:45" ht="15">
+    <row r="605" spans="1:45" ht="14.5">
       <c r="A605" s="1" t="s">
         <v>4</v>
       </c>
@@ -30703,7 +30703,7 @@
         <v>178.54</v>
       </c>
     </row>
-    <row r="606" spans="1:45" ht="15">
+    <row r="606" spans="1:45" ht="14.5">
       <c r="A606" s="1" t="s">
         <v>4</v>
       </c>
@@ -30751,7 +30751,7 @@
         <v>198.7</v>
       </c>
     </row>
-    <row r="607" spans="1:45" ht="15">
+    <row r="607" spans="1:45" ht="14.5">
       <c r="A607" s="1" t="s">
         <v>4</v>
       </c>
@@ -30799,7 +30799,7 @@
         <v>200.98</v>
       </c>
     </row>
-    <row r="608" spans="1:45" ht="15">
+    <row r="608" spans="1:45" ht="14.5">
       <c r="A608" s="1" t="s">
         <v>4</v>
       </c>
@@ -30847,7 +30847,7 @@
         <v>194.15</v>
       </c>
     </row>
-    <row r="609" spans="1:45" ht="15">
+    <row r="609" spans="1:45" ht="14.5">
       <c r="A609" s="1" t="s">
         <v>4</v>
       </c>
@@ -30895,7 +30895,7 @@
         <v>174.96</v>
       </c>
     </row>
-    <row r="610" spans="1:45" ht="15">
+    <row r="610" spans="1:45" ht="14.5">
       <c r="A610" s="1" t="s">
         <v>4</v>
       </c>
@@ -30943,7 +30943,7 @@
         <v>169.11</v>
       </c>
     </row>
-    <row r="611" spans="1:45" ht="15">
+    <row r="611" spans="1:45" ht="14.5">
       <c r="A611" s="1" t="s">
         <v>4</v>
       </c>
@@ -30991,7 +30991,7 @@
         <v>156.1</v>
       </c>
     </row>
-    <row r="612" spans="1:45" ht="15">
+    <row r="612" spans="1:45" ht="14.5">
       <c r="A612" s="1" t="s">
         <v>4</v>
       </c>
@@ -31039,7 +31039,7 @@
         <v>166.5</v>
       </c>
     </row>
-    <row r="613" spans="1:45" ht="15">
+    <row r="613" spans="1:45" ht="14.5">
       <c r="A613" s="1" t="s">
         <v>4</v>
       </c>
@@ -31087,7 +31087,7 @@
         <v>167.8</v>
       </c>
     </row>
-    <row r="614" spans="1:45" ht="15">
+    <row r="614" spans="1:45" ht="14.5">
       <c r="A614" s="1" t="s">
         <v>4</v>
       </c>
@@ -31135,7 +31135,7 @@
         <v>159.35</v>
       </c>
     </row>
-    <row r="615" spans="1:45" ht="15">
+    <row r="615" spans="1:45" ht="14.5">
       <c r="A615" s="1" t="s">
         <v>4</v>
       </c>
@@ -31183,7 +31183,7 @@
         <v>153.82</v>
       </c>
     </row>
-    <row r="616" spans="1:45" ht="15">
+    <row r="616" spans="1:45" ht="14.5">
       <c r="A616" s="1" t="s">
         <v>4</v>
       </c>
@@ -31231,7 +31231,7 @@
         <v>163.9</v>
       </c>
     </row>
-    <row r="617" spans="1:45" ht="15">
+    <row r="617" spans="1:45" ht="14.5">
       <c r="A617" s="1" t="s">
         <v>4</v>
       </c>
@@ -31279,7 +31279,7 @@
         <v>153.82</v>
       </c>
     </row>
-    <row r="618" spans="1:45" ht="15">
+    <row r="618" spans="1:45" ht="14.5">
       <c r="A618" s="1" t="s">
         <v>4</v>
       </c>
@@ -31327,7 +31327,7 @@
         <v>153.82</v>
       </c>
     </row>
-    <row r="619" spans="1:45" ht="15">
+    <row r="619" spans="1:45" ht="14.5">
       <c r="A619" s="1" t="s">
         <v>4</v>
       </c>
@@ -31375,7 +31375,7 @@
         <v>171.38</v>
       </c>
     </row>
-    <row r="620" spans="1:45" ht="15">
+    <row r="620" spans="1:45" ht="14.5">
       <c r="A620" s="1" t="s">
         <v>4</v>
       </c>
@@ -31423,7 +31423,7 @@
         <v>154.15</v>
       </c>
     </row>
-    <row r="621" spans="1:45" ht="15">
+    <row r="621" spans="1:45" ht="14.5">
       <c r="A621" s="1" t="s">
         <v>4</v>
       </c>
@@ -31471,7 +31471,7 @@
         <v>151.54</v>
       </c>
     </row>
-    <row r="622" spans="1:45" ht="15">
+    <row r="622" spans="1:45" ht="14.5">
       <c r="A622" s="1" t="s">
         <v>4</v>
       </c>
@@ -31519,7 +31519,7 @@
         <v>147.32</v>
       </c>
     </row>
-    <row r="623" spans="1:45" ht="15">
+    <row r="623" spans="1:45" ht="14.5">
       <c r="A623" s="1" t="s">
         <v>4</v>
       </c>
@@ -31567,7 +31567,7 @@
         <v>148.62</v>
       </c>
     </row>
-    <row r="624" spans="1:45" ht="15">
+    <row r="624" spans="1:45" ht="14.5">
       <c r="A624" s="1" t="s">
         <v>4</v>
       </c>
@@ -31615,7 +31615,7 @@
         <v>160.65</v>
       </c>
     </row>
-    <row r="625" spans="1:45" ht="15">
+    <row r="625" spans="1:45" ht="14.5">
       <c r="A625" s="1" t="s">
         <v>4</v>
       </c>
@@ -31663,7 +31663,7 @@
         <v>206.83</v>
       </c>
     </row>
-    <row r="626" spans="1:45" ht="15">
+    <row r="626" spans="1:45" ht="14.5">
       <c r="A626" s="1" t="s">
         <v>4</v>
       </c>
@@ -31711,7 +31711,7 @@
         <v>239.02</v>
       </c>
     </row>
-    <row r="627" spans="1:45" ht="15">
+    <row r="627" spans="1:45" ht="14.5">
       <c r="A627" s="1" t="s">
         <v>4</v>
       </c>
@@ -31759,7 +31759,7 @@
         <v>252.03</v>
       </c>
     </row>
-    <row r="628" spans="1:45" ht="15">
+    <row r="628" spans="1:45" ht="14.5">
       <c r="A628" s="1" t="s">
         <v>4</v>
       </c>
@@ -31807,7 +31807,7 @@
         <v>284.23</v>
       </c>
     </row>
-    <row r="629" spans="1:45" ht="15">
+    <row r="629" spans="1:45" ht="14.5">
       <c r="A629" s="1" t="s">
         <v>4</v>
       </c>
@@ -31855,7 +31855,7 @@
         <v>288.13</v>
       </c>
     </row>
-    <row r="630" spans="1:45" ht="15">
+    <row r="630" spans="1:45" ht="14.5">
       <c r="A630" s="26" t="s">
         <v>5</v>
       </c>
@@ -31903,7 +31903,7 @@
         <v>323.76816399999996</v>
       </c>
     </row>
-    <row r="631" spans="1:45" ht="15">
+    <row r="631" spans="1:45" ht="14.5">
       <c r="A631" s="26" t="s">
         <v>5</v>
       </c>
@@ -31951,7 +31951,7 @@
         <v>335.32658400000003</v>
       </c>
     </row>
-    <row r="632" spans="1:45" ht="15">
+    <row r="632" spans="1:45" ht="14.5">
       <c r="A632" s="26" t="s">
         <v>5</v>
       </c>
@@ -31999,7 +31999,7 @@
         <v>350.22689500000001</v>
       </c>
     </row>
-    <row r="633" spans="1:45" ht="15">
+    <row r="633" spans="1:45" ht="14.5">
       <c r="A633" s="26" t="s">
         <v>5</v>
       </c>
@@ -32047,7 +32047,7 @@
         <v>363.26780800000006</v>
       </c>
     </row>
-    <row r="634" spans="1:45" ht="15">
+    <row r="634" spans="1:45" ht="14.5">
       <c r="A634" s="26" t="s">
         <v>5</v>
       </c>
@@ -32095,7 +32095,7 @@
         <v>365.152333</v>
       </c>
     </row>
-    <row r="635" spans="1:45" ht="15">
+    <row r="635" spans="1:45" ht="14.5">
       <c r="A635" s="26" t="s">
         <v>5</v>
       </c>
@@ -32143,7 +32143,7 @@
         <v>359.22236099999998</v>
       </c>
     </row>
-    <row r="636" spans="1:45" ht="15">
+    <row r="636" spans="1:45" ht="14.5">
       <c r="A636" s="26" t="s">
         <v>5</v>
       </c>
@@ -32191,7 +32191,7 @@
         <v>353.66929399999998</v>
       </c>
     </row>
-    <row r="637" spans="1:45" ht="15">
+    <row r="637" spans="1:45" ht="14.5">
       <c r="A637" s="26" t="s">
         <v>5</v>
       </c>
@@ -32239,7 +32239,7 @@
         <v>365.62974600000001</v>
       </c>
     </row>
-    <row r="638" spans="1:45" ht="15">
+    <row r="638" spans="1:45" ht="14.5">
       <c r="A638" s="26" t="s">
         <v>5</v>
       </c>
@@ -32287,7 +32287,7 @@
         <v>324.69786299999998</v>
       </c>
     </row>
-    <row r="639" spans="1:45" ht="15">
+    <row r="639" spans="1:45" ht="14.5">
       <c r="A639" s="26" t="s">
         <v>5</v>
       </c>
@@ -32335,7 +32335,7 @@
         <v>365.35334899999998</v>
       </c>
     </row>
-    <row r="640" spans="1:45" ht="15">
+    <row r="640" spans="1:45" ht="14.5">
       <c r="A640" s="26" t="s">
         <v>5</v>
       </c>
@@ -32383,7 +32383,7 @@
         <v>365.805635</v>
       </c>
     </row>
-    <row r="641" spans="1:45" ht="15">
+    <row r="641" spans="1:45" ht="14.5">
       <c r="A641" s="26" t="s">
         <v>5</v>
       </c>
@@ -32431,7 +32431,7 @@
         <v>315.17473000000001</v>
       </c>
     </row>
-    <row r="642" spans="1:45" ht="15">
+    <row r="642" spans="1:45" ht="14.5">
       <c r="A642" s="26" t="s">
         <v>5</v>
       </c>
@@ -32479,7 +32479,7 @@
         <v>300.67645099999999</v>
       </c>
     </row>
-    <row r="643" spans="1:45" ht="15">
+    <row r="643" spans="1:45" ht="14.5">
       <c r="A643" s="26" t="s">
         <v>5</v>
       </c>
@@ -32527,7 +32527,7 @@
         <v>270.17227300000002</v>
       </c>
     </row>
-    <row r="644" spans="1:45" ht="15">
+    <row r="644" spans="1:45" ht="14.5">
       <c r="A644" s="26" t="s">
         <v>5</v>
       </c>
@@ -32575,7 +32575,7 @@
         <v>254.54327900000001</v>
       </c>
     </row>
-    <row r="645" spans="1:45" ht="15">
+    <row r="645" spans="1:45" ht="14.5">
       <c r="A645" s="26" t="s">
         <v>5</v>
       </c>
@@ -32623,7 +32623,7 @@
         <v>234.064774</v>
       </c>
     </row>
-    <row r="646" spans="1:45" ht="15">
+    <row r="646" spans="1:45" ht="14.5">
       <c r="A646" s="26" t="s">
         <v>5</v>
       </c>
@@ -32671,7 +32671,7 @@
         <v>211.77712500000001</v>
       </c>
     </row>
-    <row r="647" spans="1:45" ht="15">
+    <row r="647" spans="1:45" ht="14.5">
       <c r="A647" s="26" t="s">
         <v>5</v>
       </c>
@@ -32719,7 +32719,7 @@
         <v>285.92690200000004</v>
       </c>
     </row>
-    <row r="648" spans="1:45" ht="15">
+    <row r="648" spans="1:45" ht="14.5">
       <c r="A648" s="26" t="s">
         <v>5</v>
       </c>
@@ -32767,7 +32767,7 @@
         <v>280.02205700000002</v>
       </c>
     </row>
-    <row r="649" spans="1:45" ht="15">
+    <row r="649" spans="1:45" ht="14.5">
       <c r="A649" s="26" t="s">
         <v>5</v>
       </c>
@@ -32815,7 +32815,7 @@
         <v>233.88888500000002</v>
       </c>
     </row>
-    <row r="650" spans="1:45" ht="15">
+    <row r="650" spans="1:45" ht="14.5">
       <c r="A650" s="26" t="s">
         <v>5</v>
       </c>
@@ -32863,7 +32863,7 @@
         <v>224.99392699999999</v>
       </c>
     </row>
-    <row r="651" spans="1:45" ht="15">
+    <row r="651" spans="1:45" ht="14.5">
       <c r="A651" s="26" t="s">
         <v>5</v>
       </c>
@@ -32911,7 +32911,7 @@
         <v>216.09896900000001</v>
       </c>
     </row>
-    <row r="652" spans="1:45" ht="15">
+    <row r="652" spans="1:45" ht="14.5">
       <c r="A652" s="26" t="s">
         <v>5</v>
       </c>
@@ -32959,7 +32959,7 @@
         <v>274.644879</v>
       </c>
     </row>
-    <row r="653" spans="1:45" ht="15">
+    <row r="653" spans="1:45" ht="14.5">
       <c r="A653" s="26" t="s">
         <v>5</v>
       </c>
@@ -33007,7 +33007,7 @@
         <v>292.18352500000003</v>
       </c>
     </row>
-    <row r="654" spans="1:45" ht="15">
+    <row r="654" spans="1:45" ht="14.5">
       <c r="A654" s="26" t="s">
         <v>5</v>
       </c>
@@ -33055,7 +33055,7 @@
         <v>320.20013000000006</v>
       </c>
     </row>
-    <row r="655" spans="1:45" ht="15">
+    <row r="655" spans="1:45" ht="14.5">
       <c r="A655" s="26" t="s">
         <v>5</v>
       </c>
@@ -33103,7 +33103,7 @@
         <v>321.33084499999995</v>
       </c>
     </row>
-    <row r="656" spans="1:45" ht="15">
+    <row r="656" spans="1:45" ht="14.5">
       <c r="A656" s="26" t="s">
         <v>5</v>
       </c>
@@ -33151,7 +33151,7 @@
         <v>293.31424000000004</v>
       </c>
     </row>
-    <row r="657" spans="1:45" ht="15">
+    <row r="657" spans="1:45" ht="14.5">
       <c r="A657" s="26" t="s">
         <v>5</v>
       </c>
@@ -33199,7 +33199,7 @@
         <v>267.05652500000002</v>
       </c>
     </row>
-    <row r="658" spans="1:45" ht="15">
+    <row r="658" spans="1:45" ht="14.5">
       <c r="A658" s="26" t="s">
         <v>5</v>
       </c>
@@ -33247,7 +33247,7 @@
         <v>256.251915</v>
       </c>
     </row>
-    <row r="659" spans="1:45" ht="15">
+    <row r="659" spans="1:45" ht="14.5">
       <c r="A659" s="26" t="s">
         <v>5</v>
       </c>
@@ -33295,7 +33295,7 @@
         <v>233.93913900000001</v>
       </c>
     </row>
-    <row r="660" spans="1:45" ht="15">
+    <row r="660" spans="1:45" ht="14.5">
       <c r="A660" s="26" t="s">
         <v>5</v>
       </c>
@@ -33343,7 +33343,7 @@
         <v>158.80940900000002</v>
       </c>
     </row>
-    <row r="661" spans="1:45" ht="15">
+    <row r="661" spans="1:45" ht="14.5">
       <c r="A661" s="26" t="s">
         <v>5</v>
       </c>
@@ -33391,7 +33391,7 @@
         <v>118.731844</v>
       </c>
     </row>
-    <row r="662" spans="1:45" ht="15">
+    <row r="662" spans="1:45" ht="14.5">
       <c r="A662" s="26" t="s">
         <v>5</v>
       </c>
@@ -33439,7 +33439,7 @@
         <v>118.807225</v>
       </c>
     </row>
-    <row r="663" spans="1:45" ht="15">
+    <row r="663" spans="1:45" ht="14.5">
       <c r="A663" s="26" t="s">
         <v>5</v>
       </c>
@@ -33487,7 +33487,7 @@
         <v>292.81169999999997</v>
       </c>
     </row>
-    <row r="664" spans="1:45" ht="15">
+    <row r="664" spans="1:45" ht="14.5">
       <c r="A664" s="26" t="s">
         <v>5</v>
       </c>
@@ -33535,7 +33535,7 @@
         <v>247.40721099999999</v>
       </c>
     </row>
-    <row r="665" spans="1:45" ht="15">
+    <row r="665" spans="1:45" ht="14.5">
       <c r="A665" s="26" t="s">
         <v>5</v>
       </c>
@@ -33583,7 +33583,7 @@
         <v>227.70764300000002</v>
       </c>
     </row>
-    <row r="666" spans="1:45" ht="15">
+    <row r="666" spans="1:45" ht="14.5">
       <c r="A666" s="26" t="s">
         <v>5</v>
       </c>
@@ -33631,7 +33631,7 @@
         <v>213.98830100000001</v>
       </c>
     </row>
-    <row r="667" spans="1:45" ht="15">
+    <row r="667" spans="1:45" ht="14.5">
       <c r="A667" s="26" t="s">
         <v>5</v>
       </c>
@@ -33679,7 +33679,7 @@
         <v>206.60096300000001</v>
       </c>
     </row>
-    <row r="668" spans="1:45" ht="15">
+    <row r="668" spans="1:45" ht="14.5">
       <c r="A668" s="26" t="s">
         <v>5</v>
       </c>
@@ -33727,7 +33727,7 @@
         <v>206.70147099999997</v>
       </c>
     </row>
-    <row r="669" spans="1:45" ht="15">
+    <row r="669" spans="1:45" ht="14.5">
       <c r="A669" s="26" t="s">
         <v>5</v>
       </c>
@@ -33749,7 +33749,7 @@
         <v>201.90221400000001</v>
       </c>
     </row>
-    <row r="670" spans="1:45" ht="15">
+    <row r="670" spans="1:45" ht="14.5">
       <c r="A670" s="26" t="s">
         <v>5</v>
       </c>
@@ -33771,7 +33771,7 @@
         <v>275.75046699999996</v>
       </c>
     </row>
-    <row r="671" spans="1:45" ht="15">
+    <row r="671" spans="1:45" ht="14.5">
       <c r="A671" s="26" t="s">
         <v>5</v>
       </c>
@@ -33792,7 +33792,7 @@
         <v>272.40857600000004</v>
       </c>
     </row>
-    <row r="672" spans="1:45" ht="15">
+    <row r="672" spans="1:45" ht="14.5">
       <c r="A672" s="26" t="s">
         <v>5</v>
       </c>
@@ -33814,7 +33814,7 @@
         <v>273.94132300000001</v>
       </c>
     </row>
-    <row r="673" spans="1:45" ht="15">
+    <row r="673" spans="1:45" ht="14.5">
       <c r="A673" s="26" t="s">
         <v>5</v>
       </c>
@@ -33836,7 +33836,7 @@
         <v>310.82775900000001</v>
       </c>
     </row>
-    <row r="674" spans="1:45" ht="15">
+    <row r="674" spans="1:45" ht="14.5">
       <c r="A674" s="26" t="s">
         <v>5</v>
       </c>
@@ -33857,7 +33857,7 @@
         <v>275.47406999999998</v>
       </c>
     </row>
-    <row r="675" spans="1:45" ht="15">
+    <row r="675" spans="1:45" ht="14.5">
       <c r="A675" s="26" t="s">
         <v>5</v>
       </c>
@@ -33879,7 +33879,7 @@
         <v>243.16074799999998</v>
       </c>
     </row>
-    <row r="676" spans="1:45" ht="15">
+    <row r="676" spans="1:45" ht="14.5">
       <c r="A676" s="26" t="s">
         <v>5</v>
       </c>
@@ -33901,7 +33901,7 @@
         <v>218.96344699999997</v>
       </c>
     </row>
-    <row r="677" spans="1:45" ht="15">
+    <row r="677" spans="1:45" ht="14.5">
       <c r="A677" s="26" t="s">
         <v>5</v>
       </c>
@@ -33922,7 +33922,7 @@
         <v>208.76188500000001</v>
       </c>
     </row>
-    <row r="678" spans="1:45" ht="15">
+    <row r="678" spans="1:45" ht="14.5">
       <c r="A678" s="26" t="s">
         <v>5</v>
       </c>
@@ -33949,7 +33949,7 @@
         <v>169.161733</v>
       </c>
     </row>
-    <row r="679" spans="1:45" ht="15">
+    <row r="679" spans="1:45" ht="14.5">
       <c r="A679" s="26" t="s">
         <v>5</v>
       </c>
@@ -33976,7 +33976,7 @@
         <v>161.39749</v>
       </c>
     </row>
-    <row r="680" spans="1:45" ht="15">
+    <row r="680" spans="1:45" ht="14.5">
       <c r="A680" s="26" t="s">
         <v>5</v>
       </c>
@@ -34003,7 +34003,7 @@
         <v>166.47314399999999</v>
       </c>
     </row>
-    <row r="681" spans="1:45" ht="15">
+    <row r="681" spans="1:45" ht="14.5">
       <c r="A681" s="26" t="s">
         <v>5</v>
       </c>
@@ -34030,7 +34030,7 @@
         <v>153.28146900000002</v>
       </c>
     </row>
-    <row r="682" spans="1:45" ht="15">
+    <row r="682" spans="1:45" ht="14.5">
       <c r="A682" s="26" t="s">
         <v>5</v>
       </c>
@@ -34057,7 +34057,7 @@
         <v>148.08017999999998</v>
       </c>
     </row>
-    <row r="683" spans="1:45" ht="15">
+    <row r="683" spans="1:45" ht="14.5">
       <c r="A683" s="26" t="s">
         <v>5</v>
       </c>
@@ -34084,7 +34084,7 @@
         <v>142.92914500000001</v>
       </c>
     </row>
-    <row r="684" spans="1:45" ht="15">
+    <row r="684" spans="1:45" ht="14.5">
       <c r="A684" s="26" t="s">
         <v>5</v>
       </c>
@@ -34111,7 +34111,7 @@
         <v>131.06920099999999</v>
       </c>
     </row>
-    <row r="685" spans="1:45" ht="15">
+    <row r="685" spans="1:45" ht="14.5">
       <c r="A685" s="26" t="s">
         <v>5</v>
       </c>
@@ -34138,7 +34138,7 @@
         <v>192.30369999999999</v>
       </c>
     </row>
-    <row r="686" spans="1:45" ht="15">
+    <row r="686" spans="1:45" ht="14.5">
       <c r="A686" s="26" t="s">
         <v>5</v>
       </c>
@@ -34165,7 +34165,7 @@
         <v>173.38306900000001</v>
       </c>
     </row>
-    <row r="687" spans="1:45" ht="15">
+    <row r="687" spans="1:45" ht="14.5">
       <c r="A687" s="26" t="s">
         <v>5</v>
       </c>
@@ -34192,7 +34192,7 @@
         <v>224.843165</v>
       </c>
     </row>
-    <row r="688" spans="1:45" ht="15">
+    <row r="688" spans="1:45" ht="14.5">
       <c r="A688" s="26" t="s">
         <v>5</v>
       </c>
@@ -34219,7 +34219,7 @@
         <v>246.12573399999999</v>
       </c>
     </row>
-    <row r="689" spans="1:45" ht="15">
+    <row r="689" spans="1:45" ht="14.5">
       <c r="A689" s="26" t="s">
         <v>5</v>
       </c>
@@ -34246,7 +34246,7 @@
         <v>237.95945900000001</v>
       </c>
     </row>
-    <row r="690" spans="1:45" ht="15">
+    <row r="690" spans="1:45" ht="14.5">
       <c r="A690" s="26" t="s">
         <v>5</v>
       </c>
@@ -34273,7 +34273,7 @@
         <v>253.28692900000001</v>
       </c>
     </row>
-    <row r="691" spans="1:45" ht="15">
+    <row r="691" spans="1:45" ht="14.5">
       <c r="A691" s="26" t="s">
         <v>5</v>
       </c>
@@ -34300,7 +34300,7 @@
         <v>233.96426600000001</v>
       </c>
     </row>
-    <row r="692" spans="1:45" ht="15">
+    <row r="692" spans="1:45" ht="14.5">
       <c r="A692" s="26" t="s">
         <v>5</v>
       </c>
@@ -34327,7 +34327,7 @@
         <v>221.55152800000002</v>
       </c>
     </row>
-    <row r="693" spans="1:45" ht="15">
+    <row r="693" spans="1:45" ht="14.5">
       <c r="A693" s="26" t="s">
         <v>5</v>
       </c>
@@ -34354,7 +34354,7 @@
         <v>229.59216800000002</v>
       </c>
     </row>
-    <row r="694" spans="1:45" ht="15">
+    <row r="694" spans="1:45" ht="14.5">
       <c r="A694" s="26" t="s">
         <v>5</v>
       </c>
@@ -34381,7 +34381,7 @@
         <v>208.41010699999998</v>
       </c>
     </row>
-    <row r="695" spans="1:45" ht="15">
+    <row r="695" spans="1:45" ht="14.5">
       <c r="A695" s="26" t="s">
         <v>5</v>
       </c>
@@ -34408,7 +34408,7 @@
         <v>223.53656100000001</v>
       </c>
     </row>
-    <row r="696" spans="1:45" ht="15">
+    <row r="696" spans="1:45" ht="14.5">
       <c r="A696" s="26" t="s">
         <v>5</v>
       </c>
@@ -34435,7 +34435,7 @@
         <v>203.259072</v>
       </c>
     </row>
-    <row r="697" spans="1:45" ht="15">
+    <row r="697" spans="1:45" ht="14.5">
       <c r="A697" s="26" t="s">
         <v>5</v>
       </c>
@@ -34462,7 +34462,7 @@
         <v>160.492918</v>
       </c>
     </row>
-    <row r="698" spans="1:45" ht="15">
+    <row r="698" spans="1:45" ht="14.5">
       <c r="A698" s="26" t="s">
         <v>5</v>
       </c>
@@ -34489,7 +34489,7 @@
         <v>151.22105499999998</v>
       </c>
     </row>
-    <row r="699" spans="1:45" ht="15">
+    <row r="699" spans="1:45" ht="14.5">
       <c r="A699" s="26" t="s">
         <v>5</v>
       </c>
@@ -34516,7 +34516,7 @@
         <v>136.92379199999999</v>
       </c>
     </row>
-    <row r="700" spans="1:45" ht="15">
+    <row r="700" spans="1:45" ht="14.5">
       <c r="A700" s="26" t="s">
         <v>5</v>
       </c>
@@ -34543,7 +34543,7 @@
         <v>142.92914500000001</v>
       </c>
     </row>
-    <row r="701" spans="1:45" ht="15">
+    <row r="701" spans="1:45" ht="14.5">
       <c r="A701" s="26" t="s">
         <v>5</v>
       </c>
@@ -34570,7 +34570,7 @@
         <v>162.50307800000002</v>
       </c>
     </row>
-    <row r="702" spans="1:45" ht="15">
+    <row r="702" spans="1:45" ht="14.5">
       <c r="A702" s="26" t="s">
         <v>5</v>
       </c>
@@ -34597,7 +34597,7 @@
         <v>153.98502500000001</v>
       </c>
     </row>
-    <row r="703" spans="1:45" ht="15">
+    <row r="703" spans="1:45" ht="14.5">
       <c r="A703" s="26" t="s">
         <v>5</v>
       </c>
@@ -34624,7 +34624,7 @@
         <v>141.37127100000001</v>
       </c>
     </row>
-    <row r="704" spans="1:45" ht="15">
+    <row r="704" spans="1:45" ht="14.5">
       <c r="A704" s="26" t="s">
         <v>5</v>
       </c>
@@ -34651,7 +34651,7 @@
         <v>132.09940799999998</v>
       </c>
     </row>
-    <row r="705" spans="1:45" ht="15">
+    <row r="705" spans="1:45" ht="14.5">
       <c r="A705" s="26" t="s">
         <v>5</v>
       </c>
@@ -34678,7 +34678,7 @@
         <v>131.77275699999998</v>
       </c>
     </row>
-    <row r="706" spans="1:45" ht="15">
+    <row r="706" spans="1:45" ht="14.5">
       <c r="A706" s="26" t="s">
         <v>5</v>
       </c>
@@ -34705,7 +34705,7 @@
         <v>140.36619099999999</v>
       </c>
     </row>
-    <row r="707" spans="1:45" ht="15">
+    <row r="707" spans="1:45" ht="14.5">
       <c r="A707" s="26" t="s">
         <v>5</v>
       </c>
@@ -34732,7 +34732,7 @@
         <v>145.81874999999999</v>
       </c>
     </row>
-    <row r="708" spans="1:45" ht="15">
+    <row r="708" spans="1:45" ht="14.5">
       <c r="A708" s="26" t="s">
         <v>5</v>
       </c>
@@ -34759,7 +34759,7 @@
         <v>143.255796</v>
       </c>
     </row>
-    <row r="709" spans="1:45" ht="15">
+    <row r="709" spans="1:45" ht="14.5">
       <c r="A709" s="26" t="s">
         <v>5</v>
       </c>
@@ -34786,7 +34786,7 @@
         <v>161.724141</v>
       </c>
     </row>
-    <row r="710" spans="1:45" ht="15">
+    <row r="710" spans="1:45" ht="14.5">
       <c r="A710" s="26" t="s">
         <v>5</v>
       </c>
@@ -34813,7 +34813,7 @@
         <v>157.1259</v>
       </c>
     </row>
-    <row r="711" spans="1:45" ht="15">
+    <row r="711" spans="1:45" ht="14.5">
       <c r="A711" s="26" t="s">
         <v>5</v>
       </c>
@@ -34840,7 +34840,7 @@
         <v>175.242467</v>
       </c>
     </row>
-    <row r="712" spans="1:45" ht="15">
+    <row r="712" spans="1:45" ht="14.5">
       <c r="A712" s="26" t="s">
         <v>5</v>
       </c>
@@ -34867,7 +34867,7 @@
         <v>180.89604199999999</v>
       </c>
     </row>
-    <row r="713" spans="1:45" ht="15">
+    <row r="713" spans="1:45" ht="14.5">
       <c r="A713" s="26" t="s">
         <v>5</v>
       </c>
@@ -34894,7 +34894,7 @@
         <v>171.649306</v>
       </c>
     </row>
-    <row r="714" spans="1:45" ht="15">
+    <row r="714" spans="1:45" ht="14.5">
       <c r="A714" s="26" t="s">
         <v>5</v>
       </c>
@@ -34921,7 +34921,7 @@
         <v>153.784009</v>
       </c>
     </row>
-    <row r="715" spans="1:45" ht="15">
+    <row r="715" spans="1:45" ht="14.5">
       <c r="A715" s="26" t="s">
         <v>5</v>
       </c>
@@ -34948,7 +34948,7 @@
         <v>156.07056599999999</v>
       </c>
     </row>
-    <row r="716" spans="1:45" ht="15">
+    <row r="716" spans="1:45" ht="14.5">
       <c r="A716" s="26" t="s">
         <v>5</v>
       </c>
@@ -34975,7 +34975,7 @@
         <v>140.46669900000001</v>
       </c>
     </row>
-    <row r="717" spans="1:45" ht="15">
+    <row r="717" spans="1:45" ht="14.5">
       <c r="A717" s="26" t="s">
         <v>5</v>
       </c>
@@ -35002,7 +35002,7 @@
         <v>153.90964400000001</v>
       </c>
     </row>
-    <row r="718" spans="1:45" ht="15">
+    <row r="718" spans="1:45" ht="14.5">
       <c r="A718" s="26" t="s">
         <v>5</v>
       </c>
@@ -35029,7 +35029,7 @@
         <v>157.67869400000001</v>
       </c>
     </row>
-    <row r="719" spans="1:45" ht="15">
+    <row r="719" spans="1:45" ht="14.5">
       <c r="A719" s="26" t="s">
         <v>5</v>
       </c>
@@ -35056,7 +35056,7 @@
         <v>143.959352</v>
       </c>
     </row>
-    <row r="720" spans="1:45" ht="15">
+    <row r="720" spans="1:45" ht="14.5">
       <c r="A720" s="27" t="s">
         <v>9</v>
       </c>
@@ -35083,7 +35083,7 @@
         <v>323.76816399999996</v>
       </c>
     </row>
-    <row r="721" spans="1:45" ht="15">
+    <row r="721" spans="1:45" ht="14.5">
       <c r="A721" s="27" t="s">
         <v>9</v>
       </c>
@@ -35110,7 +35110,7 @@
         <v>335.32658400000003</v>
       </c>
     </row>
-    <row r="722" spans="1:45" ht="15">
+    <row r="722" spans="1:45" ht="14.5">
       <c r="A722" s="27" t="s">
         <v>9</v>
       </c>
@@ -35137,7 +35137,7 @@
         <v>357.31270900000004</v>
       </c>
     </row>
-    <row r="723" spans="1:45" ht="15">
+    <row r="723" spans="1:45" ht="14.5">
       <c r="A723" s="27" t="s">
         <v>9</v>
       </c>
@@ -35164,7 +35164,7 @@
         <v>363.26780800000006</v>
       </c>
     </row>
-    <row r="724" spans="1:45" ht="15">
+    <row r="724" spans="1:45" ht="14.5">
       <c r="A724" s="27" t="s">
         <v>9</v>
       </c>
@@ -45973,9 +45973,6 @@
       <c r="C1136" s="3">
         <v>10</v>
       </c>
-      <c r="AD1136" s="3">
-        <v>102</v>
-      </c>
       <c r="AF1136" s="3">
         <v>132</v>
       </c>
@@ -45996,9 +45993,6 @@
       <c r="C1137" s="3">
         <v>10</v>
       </c>
-      <c r="AD1137" s="3">
-        <v>162</v>
-      </c>
       <c r="AF1137" s="3">
         <v>171</v>
       </c>
@@ -46019,9 +46013,6 @@
       <c r="C1138" s="3">
         <v>10</v>
       </c>
-      <c r="AD1138" s="3">
-        <v>160</v>
-      </c>
       <c r="AF1138" s="3">
         <v>200</v>
       </c>
@@ -46042,9 +46033,6 @@
       <c r="C1139" s="3">
         <v>10</v>
       </c>
-      <c r="AD1139" s="3">
-        <v>158</v>
-      </c>
       <c r="AF1139" s="3">
         <v>189</v>
       </c>
@@ -46065,9 +46053,6 @@
       <c r="C1140" s="3">
         <v>10</v>
       </c>
-      <c r="AD1140" s="3">
-        <v>94</v>
-      </c>
       <c r="AF1140" s="3">
         <v>113</v>
       </c>
@@ -46088,9 +46073,6 @@
       <c r="C1141" s="3">
         <v>10</v>
       </c>
-      <c r="AD1141" s="3">
-        <v>182</v>
-      </c>
       <c r="AF1141" s="3">
         <v>188</v>
       </c>
@@ -46111,9 +46093,6 @@
       <c r="C1142" s="3">
         <v>10</v>
       </c>
-      <c r="AD1142" s="3">
-        <v>151</v>
-      </c>
       <c r="AF1142" s="3">
         <v>169</v>
       </c>
@@ -46134,9 +46113,6 @@
       <c r="C1143" s="3">
         <v>10</v>
       </c>
-      <c r="AD1143" s="3">
-        <v>148</v>
-      </c>
       <c r="AF1143" s="3">
         <v>163</v>
       </c>
@@ -46157,9 +46133,6 @@
       <c r="C1144" s="3">
         <v>10</v>
       </c>
-      <c r="AD1144" s="3">
-        <v>91</v>
-      </c>
       <c r="AF1144" s="3">
         <v>106</v>
       </c>
@@ -46180,9 +46153,6 @@
       <c r="C1145" s="3">
         <v>10</v>
       </c>
-      <c r="AD1145" s="3">
-        <v>149</v>
-      </c>
       <c r="AF1145" s="3">
         <v>142</v>
       </c>
@@ -46203,9 +46173,6 @@
       <c r="C1146" s="3">
         <v>10</v>
       </c>
-      <c r="AD1146" s="3">
-        <v>130</v>
-      </c>
       <c r="AF1146" s="3">
         <v>146</v>
       </c>
@@ -46226,9 +46193,6 @@
       <c r="C1147" s="3">
         <v>10</v>
       </c>
-      <c r="AD1147" s="3">
-        <v>131</v>
-      </c>
       <c r="AF1147" s="3">
         <v>135</v>
       </c>
@@ -46258,11 +46222,8 @@
       <c r="AA1148" s="3">
         <v>19.399999999999999</v>
       </c>
-      <c r="AD1148" s="3">
-        <v>216</v>
-      </c>
       <c r="AE1148" s="3">
-        <v>11.5</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="AF1148" s="3">
         <v>279</v>
@@ -46293,11 +46254,8 @@
       <c r="AA1149" s="3">
         <v>22</v>
       </c>
-      <c r="AD1149" s="3">
-        <v>321</v>
-      </c>
       <c r="AE1149" s="3">
-        <v>19.399999999999999</v>
+        <v>1.94</v>
       </c>
       <c r="AF1149" s="3">
         <v>340.5</v>
@@ -46328,11 +46286,8 @@
       <c r="AA1150" s="3">
         <v>21.4</v>
       </c>
-      <c r="AD1150" s="3">
-        <v>306</v>
-      </c>
       <c r="AE1150" s="3">
-        <v>14.6</v>
+        <v>1.46</v>
       </c>
       <c r="AF1150" s="3">
         <v>381</v>
@@ -46363,11 +46318,8 @@
       <c r="AA1151" s="3">
         <v>21</v>
       </c>
-      <c r="AD1151" s="3">
-        <v>315</v>
-      </c>
       <c r="AE1151" s="3">
-        <v>14.3</v>
+        <v>1.4300000000000002</v>
       </c>
       <c r="AF1151" s="3">
         <v>376.5</v>
@@ -46398,11 +46350,8 @@
       <c r="AA1152" s="3">
         <v>18.600000000000001</v>
       </c>
-      <c r="AD1152" s="3">
-        <v>208.5</v>
-      </c>
       <c r="AE1152" s="3">
-        <v>15.7</v>
+        <v>1.5699999999999998</v>
       </c>
       <c r="AF1152" s="3">
         <v>252</v>
@@ -46433,11 +46382,8 @@
       <c r="AA1153" s="3">
         <v>22</v>
       </c>
-      <c r="AD1153" s="3">
-        <v>360</v>
-      </c>
       <c r="AE1153" s="3">
-        <v>21</v>
+        <v>2.1</v>
       </c>
       <c r="AF1153" s="3">
         <v>373.5</v>
@@ -46468,11 +46414,8 @@
       <c r="AA1154" s="3">
         <v>20.5</v>
       </c>
-      <c r="AD1154" s="3">
-        <v>292.5</v>
-      </c>
       <c r="AE1154" s="3">
-        <v>19</v>
+        <v>1.9</v>
       </c>
       <c r="AF1154" s="3">
         <v>330</v>
@@ -46503,11 +46446,8 @@
       <c r="AA1155" s="3">
         <v>21.3</v>
       </c>
-      <c r="AD1155" s="3">
-        <v>298.5</v>
-      </c>
       <c r="AE1155" s="3">
-        <v>17.8</v>
+        <v>1.78</v>
       </c>
       <c r="AF1155" s="3">
         <v>331.5</v>
@@ -46538,11 +46478,8 @@
       <c r="AA1156" s="3">
         <v>18.100000000000001</v>
       </c>
-      <c r="AD1156" s="3">
-        <v>181.5</v>
-      </c>
       <c r="AE1156" s="3">
-        <v>15.6</v>
+        <v>1.56</v>
       </c>
       <c r="AF1156" s="3">
         <v>211.5</v>
@@ -46573,11 +46510,8 @@
       <c r="AA1157" s="3">
         <v>19.7</v>
       </c>
-      <c r="AD1157" s="3">
-        <v>301.5</v>
-      </c>
       <c r="AE1157" s="3">
-        <v>18.2</v>
+        <v>1.8199999999999998</v>
       </c>
       <c r="AF1157" s="3">
         <v>288</v>
@@ -46608,11 +46542,8 @@
       <c r="AA1158" s="3">
         <v>19.7</v>
       </c>
-      <c r="AD1158" s="3">
-        <v>252</v>
-      </c>
       <c r="AE1158" s="3">
-        <v>16.2</v>
+        <v>1.6199999999999999</v>
       </c>
       <c r="AF1158" s="3">
         <v>282</v>
@@ -46643,11 +46574,8 @@
       <c r="AA1159" s="3">
         <v>19.399999999999999</v>
       </c>
-      <c r="AD1159" s="3">
-        <v>258</v>
-      </c>
       <c r="AE1159" s="3">
-        <v>16.399999999999999</v>
+        <v>1.64</v>
       </c>
       <c r="AF1159" s="3">
         <v>265.5</v>
@@ -47257,7 +47185,7 @@
         <v>15.000000000000002</v>
       </c>
     </row>
-    <row r="1179" spans="1:72" ht="15">
+    <row r="1179" spans="1:72" ht="14.5">
       <c r="A1179" s="3" t="s">
         <v>65</v>
       </c>
@@ -47282,7 +47210,7 @@
         <v>7.4476923076923072</v>
       </c>
     </row>
-    <row r="1180" spans="1:72" ht="15">
+    <row r="1180" spans="1:72" ht="14.5">
       <c r="A1180" s="3" t="s">
         <v>65</v>
       </c>
@@ -47854,7 +47782,7 @@
         <v>1.11E-2</v>
       </c>
     </row>
-    <row r="1197" spans="1:72" ht="15">
+    <row r="1197" spans="1:72" ht="14.5">
       <c r="A1197" s="3" t="s">
         <v>87</v>
       </c>

</xml_diff>

<commit_message>
Improved BFG soil water and interception, and deleted spurious low branch weights that were actually just copy of age
</commit_message>
<xml_diff>
--- a/Prototypes/Pinus/Observed.xlsx
+++ b/Prototypes/Pinus/Observed.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\APSIMxSourceTree\Prototypes\Pinus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4552B3E-B55C-4F5E-A9BC-2E71EC1F40D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C4DC9AF-E521-47E2-8556-AA038669EA5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" tabRatio="653" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -987,10 +987,10 @@
   <dimension ref="A1:BT1438"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="AC1146" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="E1048554" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AC1148" sqref="AC1148:AD1159"/>
+      <selection pane="bottomRight" activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.26953125" defaultRowHeight="12.5"/>
@@ -17797,12 +17797,7 @@
       <c r="E343" s="20">
         <v>625</v>
       </c>
-      <c r="I343" s="6">
-        <v>30482.42</v>
-      </c>
-      <c r="J343" s="3">
-        <v>10</v>
-      </c>
+      <c r="I343" s="6"/>
       <c r="L343" s="6"/>
       <c r="Q343" s="36"/>
       <c r="R343" s="6"/>
@@ -17856,12 +17851,7 @@
       <c r="E344" s="20">
         <v>625</v>
       </c>
-      <c r="I344" s="6">
-        <v>32382.68144</v>
-      </c>
-      <c r="J344" s="3">
-        <v>15.2</v>
-      </c>
+      <c r="I344" s="6"/>
       <c r="L344" s="6"/>
       <c r="Q344" s="36"/>
       <c r="R344" s="6"/>
@@ -17915,12 +17905,7 @@
       <c r="E345" s="20">
         <v>275</v>
       </c>
-      <c r="I345" s="6">
-        <v>32601.82676</v>
-      </c>
-      <c r="J345" s="3">
-        <v>15.8</v>
-      </c>
+      <c r="I345" s="6"/>
       <c r="L345" s="6"/>
       <c r="Q345" s="36"/>
       <c r="R345" s="6"/>
@@ -17974,12 +17959,7 @@
       <c r="E346" s="20">
         <v>275</v>
       </c>
-      <c r="I346" s="6">
-        <v>34135.843999999997</v>
-      </c>
-      <c r="J346" s="3">
-        <v>20</v>
-      </c>
+      <c r="I346" s="6"/>
       <c r="L346" s="6"/>
       <c r="Q346" s="36"/>
       <c r="R346" s="6"/>
@@ -18033,12 +18013,7 @@
       <c r="E347" s="20">
         <v>275</v>
       </c>
-      <c r="I347" s="6">
-        <v>37057.781600000002</v>
-      </c>
-      <c r="J347" s="3">
-        <v>28</v>
-      </c>
+      <c r="I347" s="6"/>
       <c r="L347" s="6"/>
       <c r="Q347" s="36"/>
       <c r="R347" s="6"/>

</xml_diff>

<commit_message>
Added more SE Qld sites
</commit_message>
<xml_diff>
--- a/Prototypes/Pinus/Observed.xlsx
+++ b/Prototypes/Pinus/Observed.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\APSIMxSourceTree\Prototypes\Pinus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F437DF84-DE40-44FF-9A70-5F3ED9D8A804}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{276604AB-B48F-40A3-B886-8C03C6C96BE2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" tabRatio="653" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2444" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2458" uniqueCount="115">
   <si>
     <t>SimulationName</t>
   </si>
@@ -392,6 +392,15 @@
   <si>
     <t>321GYMR1</t>
   </si>
+  <si>
+    <t>248MBRF1ContainerLargeMound</t>
+  </si>
+  <si>
+    <t>251MBRF1MB6</t>
+  </si>
+  <si>
+    <t>350GYMHighFWC</t>
+  </si>
 </sst>
 </file>
 
@@ -403,7 +412,7 @@
     <numFmt numFmtId="166" formatCode="0.000"/>
     <numFmt numFmtId="167" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -492,6 +501,11 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Monospace"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -540,7 +554,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -636,6 +650,10 @@
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="0.0" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -1015,13 +1033,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr codeName="Sheet7"/>
-  <dimension ref="A1:BT1455"/>
+  <dimension ref="A1:BT1463"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="F1406" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="AA1418" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F1447" sqref="F1447"/>
+      <selection pane="bottomRight" activeCell="B1458" sqref="B1458"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="12.75"/>
@@ -54951,18 +54969,47 @@
       </c>
     </row>
     <row r="1450" spans="1:36">
-      <c r="B1450" s="54"/>
-      <c r="C1450" s="23"/>
+      <c r="A1450" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1450" s="54">
+        <v>36600</v>
+      </c>
+      <c r="C1450" s="23">
+        <v>0</v>
+      </c>
+      <c r="D1450" s="1">
+        <v>100</v>
+      </c>
+      <c r="E1450" s="1">
+        <v>833</v>
+      </c>
     </row>
     <row r="1451" spans="1:36">
+      <c r="A1451" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1451" s="5">
+        <f>B$1450+365.25*C1451</f>
+        <v>37421.8125</v>
+      </c>
+      <c r="C1451" s="23">
+        <v>2.25</v>
+      </c>
+      <c r="D1451" s="1">
+        <v>100</v>
+      </c>
+      <c r="E1451" s="1">
+        <v>833</v>
+      </c>
       <c r="W1451" s="49"/>
       <c r="X1451" s="49"/>
       <c r="Y1451" s="49"/>
       <c r="Z1451" s="49"/>
-      <c r="AA1451" s="49"/>
-      <c r="AB1451" s="49"/>
-      <c r="AC1451" s="49"/>
-      <c r="AD1451" s="49"/>
+      <c r="AA1451" s="53"/>
+      <c r="AB1451" s="53"/>
+      <c r="AC1451" s="53"/>
+      <c r="AD1451" s="53"/>
       <c r="AE1451" s="49"/>
       <c r="AF1451" s="49"/>
       <c r="AG1451" s="49"/>
@@ -54970,14 +55017,30 @@
       <c r="AI1451" s="50"/>
     </row>
     <row r="1452" spans="1:36">
+      <c r="A1452" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1452" s="5">
+        <f t="shared" ref="B1452:B1455" si="20">B$1450+365.25*C1452</f>
+        <v>37798.019999999997</v>
+      </c>
+      <c r="C1452" s="23">
+        <v>3.28</v>
+      </c>
+      <c r="D1452" s="1">
+        <v>100</v>
+      </c>
+      <c r="E1452" s="1">
+        <v>833</v>
+      </c>
       <c r="W1452" s="49"/>
       <c r="X1452" s="49"/>
       <c r="Y1452" s="49"/>
       <c r="Z1452" s="49"/>
-      <c r="AA1452" s="49"/>
-      <c r="AB1452" s="49"/>
-      <c r="AC1452" s="49"/>
-      <c r="AD1452" s="49"/>
+      <c r="AA1452" s="53"/>
+      <c r="AB1452" s="53"/>
+      <c r="AC1452" s="53"/>
+      <c r="AD1452" s="53"/>
       <c r="AE1452" s="49"/>
       <c r="AF1452" s="49"/>
       <c r="AG1452" s="49"/>
@@ -54985,6 +55048,22 @@
       <c r="AI1452" s="50"/>
     </row>
     <row r="1453" spans="1:36">
+      <c r="A1453" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1453" s="5">
+        <f t="shared" si="20"/>
+        <v>38981.43</v>
+      </c>
+      <c r="C1453" s="23">
+        <v>6.52</v>
+      </c>
+      <c r="D1453" s="1">
+        <v>100</v>
+      </c>
+      <c r="E1453" s="1">
+        <v>833</v>
+      </c>
       <c r="T1453" s="50"/>
       <c r="U1453" s="51"/>
       <c r="V1453" s="51"/>
@@ -54992,25 +55071,259 @@
       <c r="X1453" s="51"/>
       <c r="Y1453" s="51"/>
       <c r="Z1453" s="51"/>
-      <c r="AA1453" s="51"/>
-      <c r="AB1453" s="51"/>
-      <c r="AC1453" s="51"/>
-      <c r="AD1453" s="51"/>
+      <c r="AA1453" s="53"/>
+      <c r="AB1453" s="53"/>
+      <c r="AD1453" s="53"/>
       <c r="AE1453" s="51"/>
       <c r="AF1453" s="51"/>
       <c r="AG1453" s="51"/>
       <c r="AH1453" s="51"/>
       <c r="AI1453" s="50"/>
     </row>
+    <row r="1454" spans="1:36">
+      <c r="A1454" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1454" s="5">
+        <f t="shared" si="20"/>
+        <v>40712.714999999997</v>
+      </c>
+      <c r="C1454" s="23">
+        <v>11.26</v>
+      </c>
+      <c r="D1454" s="1">
+        <v>100</v>
+      </c>
+      <c r="E1454" s="1">
+        <v>833</v>
+      </c>
+      <c r="AA1454" s="55"/>
+      <c r="AB1454" s="55"/>
+      <c r="AD1454" s="55"/>
+    </row>
     <row r="1455" spans="1:36">
-      <c r="AA1455" s="1"/>
-      <c r="AB1455" s="1"/>
-      <c r="AC1455" s="1"/>
-      <c r="AD1455" s="1"/>
+      <c r="A1455" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1455" s="5">
+        <f t="shared" si="20"/>
+        <v>42126.232499999998</v>
+      </c>
+      <c r="C1455" s="23">
+        <v>15.13</v>
+      </c>
+      <c r="D1455" s="1">
+        <v>100</v>
+      </c>
+      <c r="E1455" s="1">
+        <v>833</v>
+      </c>
+      <c r="AA1455" s="55"/>
+      <c r="AB1455" s="55"/>
       <c r="AE1455" s="1"/>
-      <c r="AF1455" s="1"/>
+      <c r="AF1455" s="55">
+        <v>414.5</v>
+      </c>
       <c r="AG1455" s="1"/>
       <c r="AH1455" s="1"/>
+    </row>
+    <row r="1456" spans="1:36">
+      <c r="A1456" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B1456" s="54">
+        <v>37408</v>
+      </c>
+      <c r="C1456" s="23">
+        <v>0</v>
+      </c>
+      <c r="D1456" s="1">
+        <v>100</v>
+      </c>
+      <c r="E1456" s="1">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="1457" spans="1:32">
+      <c r="A1457" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B1457" s="54">
+        <f>B$1456+365.25*C1457</f>
+        <v>42156.25</v>
+      </c>
+      <c r="C1457" s="23">
+        <v>13</v>
+      </c>
+      <c r="D1457" s="3">
+        <f>E1457/E1456*100</f>
+        <v>97.858942065491178</v>
+      </c>
+      <c r="E1457" s="1">
+        <v>777</v>
+      </c>
+      <c r="AB1457" s="3">
+        <v>23.6</v>
+      </c>
+      <c r="AD1457" s="3">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="1458" spans="1:32">
+      <c r="A1458" s="56" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1458" s="5">
+        <v>36285</v>
+      </c>
+      <c r="C1458" s="23">
+        <v>0</v>
+      </c>
+      <c r="D1458" s="1">
+        <v>100</v>
+      </c>
+      <c r="E1458" s="19">
+        <v>833.3</v>
+      </c>
+    </row>
+    <row r="1459" spans="1:32">
+      <c r="A1459" s="56" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1459" s="54">
+        <f>B$1458+365.25*C1459</f>
+        <v>36504.15</v>
+      </c>
+      <c r="C1459" s="23">
+        <v>0.6</v>
+      </c>
+      <c r="D1459" s="1">
+        <v>98.3</v>
+      </c>
+      <c r="E1459" s="20">
+        <f>E$1458*D1459/100</f>
+        <v>819.13390000000004</v>
+      </c>
+      <c r="F1459" s="7"/>
+      <c r="AA1459" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1460" spans="1:32">
+      <c r="A1460" s="56" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1460" s="54">
+        <f t="shared" ref="B1460" si="21">B$1458+365.25*C1460</f>
+        <v>37307.699999999997</v>
+      </c>
+      <c r="C1460" s="23">
+        <v>2.8</v>
+      </c>
+      <c r="D1460" s="1">
+        <v>97.1</v>
+      </c>
+      <c r="E1460" s="20">
+        <f t="shared" ref="E1460:E1463" si="22">E$1458*D1460/100</f>
+        <v>809.13429999999994</v>
+      </c>
+      <c r="F1460" s="7"/>
+      <c r="AA1460" s="3">
+        <v>3</v>
+      </c>
+      <c r="AB1460" s="3">
+        <v>5.5</v>
+      </c>
+      <c r="AC1460" s="3">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="AF1460" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1461" spans="1:32">
+      <c r="A1461" s="56" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1461" s="54">
+        <f>B$1458+365.25*C1461</f>
+        <v>37782.525000000001</v>
+      </c>
+      <c r="C1461" s="23">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="D1461" s="1">
+        <v>96.5</v>
+      </c>
+      <c r="E1461" s="20">
+        <f t="shared" si="22"/>
+        <v>804.1345</v>
+      </c>
+      <c r="F1461" s="7"/>
+      <c r="AA1461" s="3">
+        <v>8.5</v>
+      </c>
+      <c r="AB1461" s="3">
+        <v>11.8</v>
+      </c>
+      <c r="AC1461" s="3">
+        <v>9.5</v>
+      </c>
+      <c r="AF1461" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="1462" spans="1:32">
+      <c r="A1462" s="56" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1462" s="54">
+        <f>B$1458+365.25*C1462</f>
+        <v>38878.275000000001</v>
+      </c>
+      <c r="C1462" s="23">
+        <v>7.1</v>
+      </c>
+      <c r="D1462" s="1">
+        <v>96</v>
+      </c>
+      <c r="E1462" s="20">
+        <f t="shared" si="22"/>
+        <v>799.96799999999985</v>
+      </c>
+      <c r="F1462" s="7"/>
+    </row>
+    <row r="1463" spans="1:32">
+      <c r="A1463" s="56" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1463" s="54">
+        <f>B$1458+365.25*C1463</f>
+        <v>39243.525000000001</v>
+      </c>
+      <c r="C1463" s="23">
+        <v>8.1</v>
+      </c>
+      <c r="D1463" s="1">
+        <v>96</v>
+      </c>
+      <c r="E1463" s="20">
+        <f t="shared" si="22"/>
+        <v>799.96799999999985</v>
+      </c>
+      <c r="F1463" s="7"/>
+      <c r="AA1463" s="1">
+        <v>15.2</v>
+      </c>
+      <c r="AB1463" s="3">
+        <v>19.5</v>
+      </c>
+      <c r="AC1463" s="3">
+        <v>25.2</v>
+      </c>
+      <c r="AF1463" s="1">
+        <v>130</v>
+      </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A238:BK627">

</xml_diff>

<commit_message>
Worked on SEQld genotype sowing
</commit_message>
<xml_diff>
--- a/Prototypes/Pinus/Observed.xlsx
+++ b/Prototypes/Pinus/Observed.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\APSIMxSourceTree\Prototypes\Pinus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4C5034D-B96F-4C32-B707-81A69B5B5D22}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4F8242E-E833-4580-AA6D-175A34C2A6FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" tabRatio="653" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -393,12 +393,6 @@
     <t>HQP251MBRF1MB6</t>
   </si>
   <si>
-    <t>HQP3HQP21GYMR1</t>
-  </si>
-  <si>
-    <t>HQP3HQP21GYMBLHQP2TWC</t>
-  </si>
-  <si>
     <t>HQP350GYMHighFWC</t>
   </si>
   <si>
@@ -406,6 +400,12 @@
   </si>
   <si>
     <t>FSA704</t>
+  </si>
+  <si>
+    <t>HQP321GYMR1</t>
+  </si>
+  <si>
+    <t>HQP321GYMBL2TWC</t>
   </si>
 </sst>
 </file>
@@ -1070,15 +1070,15 @@
   <dimension ref="A1:BT1505"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D1461" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D1430" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D1482" sqref="D1482:D1505"/>
+      <selection pane="bottomRight" activeCell="A1437" sqref="A1437"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" style="3" customWidth="1"/>
+    <col min="1" max="1" width="22" style="3" customWidth="1"/>
     <col min="2" max="2" width="12.28515625" style="3" customWidth="1"/>
     <col min="3" max="3" width="9.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.28515625" style="62"/>
@@ -55260,7 +55260,7 @@
     </row>
     <row r="1439" spans="1:21" s="20" customFormat="1">
       <c r="A1439" s="1" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="B1439" s="5">
         <v>24303</v>
@@ -55279,7 +55279,7 @@
     </row>
     <row r="1440" spans="1:21" s="20" customFormat="1">
       <c r="A1440" s="1" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="B1440" s="5">
         <f>B$1439+365.25*C1440</f>
@@ -55300,7 +55300,7 @@
     </row>
     <row r="1441" spans="1:36" s="20" customFormat="1">
       <c r="A1441" s="1" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="B1441" s="5">
         <f>B$1439+365.25*C1441</f>
@@ -55351,7 +55351,7 @@
     </row>
     <row r="1442" spans="1:36">
       <c r="A1442" s="1" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B1442" s="5">
         <v>35200</v>
@@ -55374,7 +55374,7 @@
     </row>
     <row r="1443" spans="1:36">
       <c r="A1443" s="1" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B1443" s="5">
         <f>B$1442+365.25*C1443</f>
@@ -55398,7 +55398,7 @@
     </row>
     <row r="1444" spans="1:36">
       <c r="A1444" s="1" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B1444" s="5">
         <f t="shared" ref="B1444:B1449" si="18">B$1442+365.25*C1444</f>
@@ -55427,7 +55427,7 @@
     </row>
     <row r="1445" spans="1:36">
       <c r="A1445" s="1" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B1445" s="5">
         <f t="shared" ref="B1445" si="19">B$1442+365.25*C1445</f>
@@ -55473,7 +55473,7 @@
     </row>
     <row r="1446" spans="1:36">
       <c r="A1446" s="1" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B1446" s="5">
         <f t="shared" si="18"/>
@@ -55527,7 +55527,7 @@
     </row>
     <row r="1447" spans="1:36">
       <c r="A1447" s="1" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B1447" s="5">
         <f t="shared" si="18"/>
@@ -55558,7 +55558,7 @@
     </row>
     <row r="1448" spans="1:36">
       <c r="A1448" s="1" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B1448" s="5">
         <f t="shared" si="18"/>
@@ -55589,7 +55589,7 @@
     </row>
     <row r="1449" spans="1:36">
       <c r="A1449" s="1" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B1449" s="5">
         <f t="shared" si="18"/>
@@ -55823,7 +55823,7 @@
     </row>
     <row r="1458" spans="1:32">
       <c r="A1458" s="56" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B1458" s="5">
         <v>36285</v>
@@ -55840,7 +55840,7 @@
     </row>
     <row r="1459" spans="1:32">
       <c r="A1459" s="56" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B1459" s="54">
         <f>B$1458+365.25*C1459</f>
@@ -55863,7 +55863,7 @@
     </row>
     <row r="1460" spans="1:32">
       <c r="A1460" s="56" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B1460" s="54">
         <f t="shared" ref="B1460" si="21">B$1458+365.25*C1460</f>
@@ -55895,7 +55895,7 @@
     </row>
     <row r="1461" spans="1:32">
       <c r="A1461" s="56" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B1461" s="54">
         <f>B$1458+365.25*C1461</f>
@@ -55927,7 +55927,7 @@
     </row>
     <row r="1462" spans="1:32">
       <c r="A1462" s="56" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B1462" s="54">
         <f>B$1458+365.25*C1462</f>
@@ -55947,7 +55947,7 @@
     </row>
     <row r="1463" spans="1:32">
       <c r="A1463" s="56" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B1463" s="54">
         <f>B$1458+365.25*C1463</f>
@@ -55979,7 +55979,7 @@
     </row>
     <row r="1464" spans="1:32">
       <c r="A1464" s="56" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B1464" s="54">
         <v>13346</v>
@@ -55996,7 +55996,7 @@
     </row>
     <row r="1465" spans="1:32">
       <c r="A1465" s="56" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B1465" s="54">
         <f>B$1464+365.25*C1465</f>
@@ -56021,7 +56021,7 @@
     </row>
     <row r="1466" spans="1:32">
       <c r="A1466" s="56" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B1466" s="54">
         <f t="shared" ref="B1466:B1481" si="23">B$1464+365.25*C1466</f>
@@ -56031,7 +56031,7 @@
         <v>14</v>
       </c>
       <c r="D1466" s="59">
-        <f t="shared" ref="D1466:D1482" si="24">E1466*100/E$1464</f>
+        <f t="shared" ref="D1466:D1480" si="24">E1466*100/E$1464</f>
         <v>86.285714285714292</v>
       </c>
       <c r="E1466" s="58">
@@ -56046,7 +56046,7 @@
     </row>
     <row r="1467" spans="1:32">
       <c r="A1467" s="56" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B1467" s="54">
         <f t="shared" si="23"/>
@@ -56071,7 +56071,7 @@
     </row>
     <row r="1468" spans="1:32">
       <c r="A1468" s="56" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B1468" s="54">
         <f t="shared" si="23"/>
@@ -56096,7 +56096,7 @@
     </row>
     <row r="1469" spans="1:32">
       <c r="A1469" s="56" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B1469" s="54">
         <f t="shared" si="23"/>
@@ -56121,7 +56121,7 @@
     </row>
     <row r="1470" spans="1:32">
       <c r="A1470" s="56" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B1470" s="54">
         <f t="shared" si="23"/>
@@ -56146,7 +56146,7 @@
     </row>
     <row r="1471" spans="1:32">
       <c r="A1471" s="56" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B1471" s="54">
         <f t="shared" si="23"/>
@@ -56169,7 +56169,7 @@
     </row>
     <row r="1472" spans="1:32">
       <c r="A1472" s="56" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B1472" s="54">
         <f t="shared" si="23"/>
@@ -56194,7 +56194,7 @@
     </row>
     <row r="1473" spans="1:30">
       <c r="A1473" s="56" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B1473" s="54">
         <f t="shared" si="23"/>
@@ -56217,7 +56217,7 @@
     </row>
     <row r="1474" spans="1:30">
       <c r="A1474" s="56" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B1474" s="54">
         <f t="shared" si="23"/>
@@ -56240,7 +56240,7 @@
     </row>
     <row r="1475" spans="1:30">
       <c r="A1475" s="56" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B1475" s="54">
         <f t="shared" si="23"/>
@@ -56265,7 +56265,7 @@
     </row>
     <row r="1476" spans="1:30">
       <c r="A1476" s="56" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B1476" s="54">
         <f t="shared" si="23"/>
@@ -56288,7 +56288,7 @@
     </row>
     <row r="1477" spans="1:30">
       <c r="A1477" s="56" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B1477" s="54">
         <f t="shared" si="23"/>
@@ -56313,7 +56313,7 @@
     </row>
     <row r="1478" spans="1:30">
       <c r="A1478" s="56" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B1478" s="54">
         <f t="shared" si="23"/>
@@ -56336,7 +56336,7 @@
     </row>
     <row r="1479" spans="1:30">
       <c r="A1479" s="56" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B1479" s="54">
         <f t="shared" si="23"/>
@@ -56359,7 +56359,7 @@
     </row>
     <row r="1480" spans="1:30">
       <c r="A1480" s="56" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B1480" s="54">
         <f t="shared" si="23"/>
@@ -56384,7 +56384,7 @@
     </row>
     <row r="1481" spans="1:30">
       <c r="A1481" s="56" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B1481" s="54">
         <f t="shared" si="23"/>
@@ -56402,7 +56402,7 @@
     </row>
     <row r="1482" spans="1:30">
       <c r="A1482" s="56" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B1482" s="54">
         <f>B$1481+365.25*C1482</f>
@@ -56427,7 +56427,7 @@
     </row>
     <row r="1483" spans="1:30">
       <c r="A1483" s="56" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B1483" s="54">
         <f t="shared" ref="B1483:B1505" si="25">B$1481+365.25*C1483</f>
@@ -56452,7 +56452,7 @@
     </row>
     <row r="1484" spans="1:30">
       <c r="A1484" s="56" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B1484" s="54">
         <f t="shared" si="25"/>
@@ -56477,7 +56477,7 @@
     </row>
     <row r="1485" spans="1:30">
       <c r="A1485" s="56" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B1485" s="54">
         <f t="shared" si="25"/>
@@ -56502,7 +56502,7 @@
     </row>
     <row r="1486" spans="1:30">
       <c r="A1486" s="56" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B1486" s="54">
         <f t="shared" si="25"/>
@@ -56527,7 +56527,7 @@
     </row>
     <row r="1487" spans="1:30">
       <c r="A1487" s="56" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B1487" s="54">
         <f t="shared" si="25"/>
@@ -56550,7 +56550,7 @@
     </row>
     <row r="1488" spans="1:30">
       <c r="A1488" s="56" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B1488" s="54">
         <f t="shared" si="25"/>
@@ -56575,7 +56575,7 @@
     </row>
     <row r="1489" spans="1:30">
       <c r="A1489" s="56" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B1489" s="54">
         <f t="shared" si="25"/>
@@ -56598,7 +56598,7 @@
     </row>
     <row r="1490" spans="1:30">
       <c r="A1490" s="56" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B1490" s="54">
         <f t="shared" si="25"/>
@@ -56621,7 +56621,7 @@
     </row>
     <row r="1491" spans="1:30">
       <c r="A1491" s="56" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B1491" s="54">
         <f t="shared" si="25"/>
@@ -56646,7 +56646,7 @@
     </row>
     <row r="1492" spans="1:30">
       <c r="A1492" s="56" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B1492" s="54">
         <f t="shared" si="25"/>
@@ -56669,7 +56669,7 @@
     </row>
     <row r="1493" spans="1:30">
       <c r="A1493" s="56" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B1493" s="54">
         <f t="shared" si="25"/>
@@ -56692,7 +56692,7 @@
     </row>
     <row r="1494" spans="1:30">
       <c r="A1494" s="56" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B1494" s="54">
         <f t="shared" si="25"/>
@@ -56717,7 +56717,7 @@
     </row>
     <row r="1495" spans="1:30">
       <c r="A1495" s="56" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B1495" s="54">
         <f t="shared" si="25"/>
@@ -56742,7 +56742,7 @@
     </row>
     <row r="1496" spans="1:30">
       <c r="A1496" s="56" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B1496" s="54">
         <f t="shared" si="25"/>
@@ -56767,7 +56767,7 @@
     </row>
     <row r="1497" spans="1:30">
       <c r="A1497" s="56" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B1497" s="54">
         <f t="shared" si="25"/>
@@ -56790,7 +56790,7 @@
     </row>
     <row r="1498" spans="1:30">
       <c r="A1498" s="56" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B1498" s="54">
         <f t="shared" si="25"/>
@@ -56815,7 +56815,7 @@
     </row>
     <row r="1499" spans="1:30">
       <c r="A1499" s="56" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B1499" s="54">
         <f t="shared" si="25"/>
@@ -56840,7 +56840,7 @@
     </row>
     <row r="1500" spans="1:30">
       <c r="A1500" s="56" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B1500" s="54">
         <f t="shared" si="25"/>
@@ -56863,7 +56863,7 @@
     </row>
     <row r="1501" spans="1:30">
       <c r="A1501" s="56" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B1501" s="54">
         <f t="shared" si="25"/>
@@ -56886,7 +56886,7 @@
     </row>
     <row r="1502" spans="1:30">
       <c r="A1502" s="56" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B1502" s="54">
         <f t="shared" si="25"/>
@@ -56909,7 +56909,7 @@
     </row>
     <row r="1503" spans="1:30">
       <c r="A1503" s="56" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B1503" s="54">
         <f t="shared" si="25"/>
@@ -56934,7 +56934,7 @@
     </row>
     <row r="1504" spans="1:30">
       <c r="A1504" s="56" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B1504" s="54">
         <f t="shared" si="25"/>
@@ -56957,7 +56957,7 @@
     </row>
     <row r="1505" spans="1:30">
       <c r="A1505" s="56" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B1505" s="54">
         <f t="shared" si="25"/>

</xml_diff>